<commit_message>
Added columns: thrust, mdot
</commit_message>
<xml_diff>
--- a/Aero210/dynamics_template.xlsx
+++ b/Aero210/dynamics_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23300" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-80" yWindow="460" windowWidth="15540" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -259,21 +259,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Mach number
-M = v / c</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Mach number
+M = v / c
 </t>
         </r>
       </text>
@@ -328,8 +319,8 @@
             <rFont val="Calibri"/>
           </rPr>
           <t>Drag in the x direction
-Dx = - (0.5)(pho)(v^2)(Cd)(S)cos(rad)
-Drag_x = - (0.5)(density of air)(drag coefficient)(frontal area)cos(rad)</t>
+Dx = - (0.5)(pho)(v^2)(Cd)(S)cos(theta)
+Drag_x = - (0.5)(density of air)(drag coefficient)(frontal area)cos(theta)</t>
         </r>
       </text>
     </comment>
@@ -342,8 +333,8 @@
             <rFont val="Calibri"/>
           </rPr>
           <t>Drag in the y direction
-Dy = - (0.5)(pho)(v^2)(Cd)(S)sin(rad)
-Drag_y = - (0.5)(density of air)(drag coefficient)(frontal area)sin(rad)</t>
+Dy = - (0.5)(pho)(v^2)(Cd)(S)sin(theta)
+Drag_y = - (0.5)(density of air)(drag coefficient)(frontal area)sin(theta)</t>
         </r>
       </text>
     </comment>
@@ -356,7 +347,7 @@
             <rFont val="Calibri"/>
           </rPr>
           <t>Acceleration in the x direction
-ax = Drag_x / mass</t>
+ax = (drag_x + thrust_x) / mass</t>
         </r>
       </text>
     </comment>
@@ -369,7 +360,63 @@
             <rFont val="Calibri"/>
           </rPr>
           <t>Acceleration in the y direction
-ay = drag_y / mass</t>
+ay = (drag_y + thrust_y) / mass</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Mass loss
+m_(i+1) = mi - (mdot)(dt)
+current mass = previous mass - (mass loss)(dt)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Thrust
+Th = (Isp)(g0)(m')
+Th = (specific impulse)(standard gravity)(rate of mass loss)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Thrust in the x direction
+Th = (Isp)(g0)(m')cos(theta)
+Th = (specific impulse)(standard gravity)(rate of mass loss)cos(theta)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Thrust in the y direction
+Th = (Isp)(g0)(m')sin(theta)
+Th = (specific impulse)(standard gravity)(rate of mass loss)sin(theta)</t>
         </r>
       </text>
     </comment>
@@ -378,7 +425,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Constants</t>
   </si>
@@ -476,16 +523,10 @@
     <t>c (m/s)</t>
   </si>
   <si>
-    <t>Object mass</t>
-  </si>
-  <si>
     <t>Dia</t>
   </si>
   <si>
     <t>Frontal area</t>
-  </si>
-  <si>
-    <t>D (N)</t>
   </si>
   <si>
     <t>Mach</t>
@@ -502,6 +543,51 @@
   <si>
     <t>ay (m/s^2)</t>
   </si>
+  <si>
+    <t>Thrust</t>
+  </si>
+  <si>
+    <t>Drag (N)</t>
+  </si>
+  <si>
+    <t>Empty mass</t>
+  </si>
+  <si>
+    <t>Init fuel mass</t>
+  </si>
+  <si>
+    <t>Standard g</t>
+  </si>
+  <si>
+    <t>m/s^2</t>
+  </si>
+  <si>
+    <t>m^2</t>
+  </si>
+  <si>
+    <t>kg/s</t>
+  </si>
+  <si>
+    <t>Mass loss</t>
+  </si>
+  <si>
+    <t>ISP</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Thrust (N)</t>
+  </si>
+  <si>
+    <t>Th_y (N)</t>
+  </si>
+  <si>
+    <t>Th_x (N)</t>
+  </si>
+  <si>
+    <t>mdot (kg/s)</t>
+  </si>
 </sst>
 </file>
 
@@ -511,7 +597,14 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -604,8 +697,20 @@
       <color theme="0"/>
       <name val="Deja Vu"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,6 +754,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -709,80 +819,93 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="8" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="7" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="8" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="14" fillId="7" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="16" fillId="9" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Bad" xfId="5" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
@@ -1139,15 +1262,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK2687"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="17" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="21" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="30" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" style="2" customWidth="1"/>
     <col min="6" max="14" width="10.6640625" style="3" customWidth="1"/>
@@ -1157,16 +1280,16 @@
     <col min="19" max="19" width="10.6640625" style="5" customWidth="1"/>
     <col min="20" max="21" width="10.6640625" customWidth="1"/>
     <col min="22" max="22" width="10.6640625" style="5" customWidth="1"/>
-    <col min="23" max="27" width="10.6640625" style="3" customWidth="1"/>
-    <col min="28" max="16384" width="10.83203125" style="5"/>
+    <col min="23" max="31" width="10.6640625" style="3" customWidth="1"/>
+    <col min="32" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="8" t="s">
         <v>10</v>
       </c>
@@ -1212,42 +1335,54 @@
       <c r="R1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="23" t="s">
+      <c r="S1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="23" t="s">
+      <c r="T1" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="V1" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="W1" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="X1" s="24" t="s">
+      <c r="Z1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="24" t="s">
+      <c r="AA1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA1" s="24" t="s">
-        <v>40</v>
+      <c r="AB1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC1" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE1" s="21" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="23">
         <v>0.1</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="29" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1">
@@ -1292,11 +1427,11 @@
         <v>29.999999999999996</v>
       </c>
       <c r="O2" s="1">
-        <f t="shared" ref="O2:O65" si="0">(0.5)*($B$11)*(H2^2)</f>
+        <f>(0.5)*($B$8)*(H2^2)</f>
         <v>500000</v>
       </c>
       <c r="P2" s="1">
-        <f t="shared" ref="P2:P65" si="1">($B$11)*L2*J2</f>
+        <f>($B$8)*L2*J2</f>
         <v>0</v>
       </c>
       <c r="Q2" s="1">
@@ -1304,7 +1439,7 @@
         <v>500000</v>
       </c>
       <c r="R2" s="1">
-        <f t="shared" ref="R2:R65" si="2" xml:space="preserve"> ($B$11)*H2</f>
+        <f xml:space="preserve"> ($B$8)*H2</f>
         <v>10000</v>
       </c>
       <c r="S2" s="3">
@@ -1324,7 +1459,7 @@
         <v>#NAME?</v>
       </c>
       <c r="W2" s="3" t="e">
-        <f>(0.5)*(U2)*(H2)*(V2)*($B$13)</f>
+        <f>(0.5)*(U2)*(H2)*(V2)*($B$17)</f>
         <v>#NAME?</v>
       </c>
       <c r="X2" s="3" t="e">
@@ -1336,22 +1471,38 @@
         <v>#NAME?</v>
       </c>
       <c r="Z2" s="3" t="e">
-        <f xml:space="preserve"> X2/($B$11)</f>
+        <f xml:space="preserve"> (X2+AD2)/($B$8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AA2" s="3" t="e">
-        <f xml:space="preserve"> Y2/($B$11)</f>
+        <f xml:space="preserve"> (Y2+AE2)/($B$8)</f>
         <v>#NAME?</v>
+      </c>
+      <c r="AB2" s="34">
+        <f xml:space="preserve"> 0</f>
+        <v>0</v>
+      </c>
+      <c r="AC2" s="1">
+        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
+        <v>98066.5</v>
+      </c>
+      <c r="AD2" s="1">
+        <f xml:space="preserve"> AC2*COS(M2)</f>
+        <v>84928.080260226663</v>
+      </c>
+      <c r="AE2" s="1">
+        <f xml:space="preserve"> AC2*SIN(M2)</f>
+        <v>49033.249999999993</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="24">
         <v>30</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1">
@@ -1371,14 +1522,14 @@
         <v>49.018929578416049</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H66" ca="1" si="3">SQRT(F3^2 + G3^2)</f>
+        <f t="shared" ref="H3:H12" ca="1" si="0">SQRT(F3^2 + G3^2)</f>
         <v>99.51309188751857</v>
       </c>
       <c r="I3" s="3">
         <f>I2 + F2*($B$2)</f>
         <v>8.6602540378443873</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="22">
         <f xml:space="preserve"> J2 + G2*($B$2) + (0.5)*(L2)*($B$2)^2</f>
         <v>4.9509464789208026</v>
       </c>
@@ -1391,39 +1542,39 @@
         <v>-9.810554785931588</v>
       </c>
       <c r="M3" s="3">
-        <f t="shared" ref="M3:M66" ca="1" si="4">ATAN(G3/F3)</f>
+        <f t="shared" ref="M3:M12" ca="1" si="1">ATAN(G3/F3)</f>
         <v>0.51506078110312425</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N66" ca="1" si="5">M3*(180/PI())</f>
+        <f t="shared" ref="N3:N12" ca="1" si="2">M3*(180/PI())</f>
         <v>29.510808949920566</v>
       </c>
       <c r="O3" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">(0.5)*($B$8)*(H3^2)</f>
         <v>495142.77285068575</v>
       </c>
       <c r="P3" s="1">
-        <f t="shared" si="1"/>
+        <f>($B$8)*L3*J3</f>
         <v>-4857.1531673667623</v>
       </c>
       <c r="Q3" s="1">
-        <f t="shared" ref="Q3:Q66" ca="1" si="6" xml:space="preserve"> ABS(O3) + ABS(P3)</f>
+        <f t="shared" ref="Q3:Q12" ca="1" si="3" xml:space="preserve"> ABS(O3) + ABS(P3)</f>
         <v>499999.9260180525</v>
       </c>
       <c r="R3" s="1">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1" xml:space="preserve"> ($B$8)*H3</f>
         <v>9951.3091887518567</v>
       </c>
       <c r="S3" s="3">
-        <f t="shared" ref="S3:S66" si="7">IF(J3&lt;30000,( (-0.00406576*J3)+340.3), "")</f>
+        <f t="shared" ref="S3:S12" si="4">IF(J3&lt;30000,( (-0.00406576*J3)+340.3), "")</f>
         <v>340.27987063984386</v>
       </c>
       <c r="T3" s="13">
-        <f t="shared" ref="T3:T66" ca="1" si="8" xml:space="preserve"> IF(J3&lt;30000, H3/S3, "")</f>
+        <f t="shared" ref="T3:T12" ca="1" si="5" xml:space="preserve"> IF(J3&lt;30000, H3/S3, "")</f>
         <v>0.29244483871584742</v>
       </c>
       <c r="U3" s="13">
-        <f t="shared" ref="U3:U66" si="9" xml:space="preserve"> IF(J3&lt;30000, (( 359.01*(1 - (2.25577*10^(-5))*(J3))^(5.25588) ) / (298.15 - 0.0074545*J3)), "")</f>
+        <f t="shared" ref="U3:U12" si="6" xml:space="preserve"> IF(J3&lt;30000, (( 359.01*(1 - (2.25577*10^(-5))*(J3))^(5.25588) ) / (298.15 - 0.0074545*J3)), "")</f>
         <v>1.2035677871607093</v>
       </c>
       <c r="V3" s="5" t="e">
@@ -1431,24 +1582,40 @@
         <v>#NAME?</v>
       </c>
       <c r="W3" s="3" t="e">
-        <f t="shared" ref="W3:W66" ca="1" si="10">(0.5)*(U3)*(H3)*(V3)*($B$13)</f>
+        <f ca="1">(0.5)*(U3)*(H3)*(V3)*($B$17)</f>
         <v>#NAME?</v>
       </c>
       <c r="X3" s="3" t="e">
-        <f t="shared" ref="X3:X66" ca="1" si="11" xml:space="preserve"> - W3*COS(M3)</f>
+        <f t="shared" ref="X3:X12" ca="1" si="7" xml:space="preserve"> - W3*COS(M3)</f>
         <v>#NAME?</v>
       </c>
       <c r="Y3" s="3" t="e">
-        <f t="shared" ref="Y3:Y66" ca="1" si="12" xml:space="preserve"> - W3*SIN(M3)</f>
+        <f t="shared" ref="Y3:Y12" ca="1" si="8" xml:space="preserve"> - W3*SIN(M3)</f>
         <v>#NAME?</v>
       </c>
       <c r="Z3" s="3" t="e">
-        <f t="shared" ref="Z3:Z12" ca="1" si="13" xml:space="preserve"> X3/($B$11)</f>
+        <f ca="1" xml:space="preserve"> X3/($B$8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AA3" s="3" t="e">
-        <f t="shared" ref="AA3:AA12" ca="1" si="14" xml:space="preserve"> Y3/($B$11)</f>
+        <f ca="1" xml:space="preserve"> Y3/($B$8)</f>
         <v>#NAME?</v>
+      </c>
+      <c r="AB3" s="1">
+        <f>IF(AB2 &gt;( $B$8 + $B$18*$B$2), AB2 -( $B$18*$B$2), $B$8)</f>
+        <v>100</v>
+      </c>
+      <c r="AC3" s="1">
+        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
+        <v>98066.5</v>
+      </c>
+      <c r="AD3" s="1">
+        <f ca="1" xml:space="preserve"> AC3*COS(M3)</f>
+        <v>85343.625295275124</v>
+      </c>
+      <c r="AE3" s="1">
+        <f ca="1" xml:space="preserve"> AC3*SIN(M3)</f>
+        <v>48306.356141916534</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
@@ -1459,35 +1626,35 @@
         <f>B3*(PI()/180)</f>
         <v>0.52359877559829882</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="29" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D67" si="15">D3 + 1</f>
+        <f t="shared" ref="D4:D12" si="9">D3 + 1</f>
         <v>2</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" ref="E4:E67" si="16" xml:space="preserve"> E3 + $B$2</f>
+        <f t="shared" ref="E4:E12" si="10" xml:space="preserve"> E3 + $B$2</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:F67" ca="1" si="17">INDIRECT(ADDRESS(ROW()-1,COLUMN()))</f>
+        <f t="shared" ref="F4:F12" ca="1" si="11">INDIRECT(ADDRESS(ROW()-1,COLUMN()))</f>
         <v>86.602540378443877</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G4:G67" si="18">G3 + L3*$B$2</f>
+        <f t="shared" ref="G4:G12" si="12">G3 + L3*$B$2</f>
         <v>48.037874099822893</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="0"/>
         <v>99.033516286308028</v>
       </c>
       <c r="I4" s="3">
-        <f t="shared" ref="I4:I67" ca="1" si="19">I3 + F3*($B$2)</f>
+        <f t="shared" ref="I4:I12" ca="1" si="13">I3 + F3*($B$2)</f>
         <v>17.320508075688775</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J67" si="20" xml:space="preserve"> J3 + G3*($B$2) + (0.5)*(L3)*($B$2)^2</f>
+        <f t="shared" ref="J4:J12" si="14" xml:space="preserve"> J3 + G3*($B$2) + (0.5)*(L3)*($B$2)^2</f>
         <v>9.803786662832751</v>
       </c>
       <c r="K4" s="3">
@@ -1495,43 +1662,43 @@
         <v>19.902801873602684</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" ref="L4:L66" si="21" xml:space="preserve"> -(9.780327 * (1 + 0.0053024 * ((SIN($B$7))^2) - (5.8*10^(-6)) * (SIN(2*($B$7))^2) - (3.086*10^(-6)) * J4))</f>
+        <f t="shared" ref="L4:L12" si="15" xml:space="preserve"> -(9.780327 * (1 + 0.0053024 * ((SIN($B$7))^2) - (5.8*10^(-6)) * (SIN(2*($B$7))^2) - (3.086*10^(-6)) * J4))</f>
         <v>-9.8104083170766643</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.50643959223510326</v>
       </c>
       <c r="N4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>29.016851213397796</v>
+      </c>
+      <c r="O4" s="1">
+        <f ca="1">(0.5)*($B$8)*(H4^2)</f>
+        <v>490381.86740152189</v>
+      </c>
+      <c r="P4" s="1">
+        <f>($B$8)*L4*J4</f>
+        <v>-9617.9150215899699</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>499999.78242311184</v>
+      </c>
+      <c r="R4" s="1">
+        <f ca="1" xml:space="preserve"> ($B$8)*H4</f>
+        <v>9903.3516286308022</v>
+      </c>
+      <c r="S4" s="3">
+        <f t="shared" si="4"/>
+        <v>340.26014015633774</v>
+      </c>
+      <c r="T4" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>29.016851213397796</v>
-      </c>
-      <c r="O4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>490381.86740152189</v>
-      </c>
-      <c r="P4" s="1">
-        <f t="shared" si="1"/>
-        <v>-9617.9150215899699</v>
-      </c>
-      <c r="Q4" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>499999.78242311184</v>
-      </c>
-      <c r="R4" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>9903.3516286308022</v>
-      </c>
-      <c r="S4" s="3">
-        <f t="shared" si="7"/>
-        <v>340.26014015633774</v>
-      </c>
-      <c r="T4" s="13">
-        <f t="shared" ca="1" si="8"/>
         <v>0.2910523584713906</v>
       </c>
       <c r="U4" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1.2030213763478994</v>
       </c>
       <c r="V4" s="5" t="e">
@@ -1539,24 +1706,40 @@
         <v>#NAME?</v>
       </c>
       <c r="W4" s="3" t="e">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">(0.5)*(U4)*(H4)*(V4)*($B$17)</f>
         <v>#NAME?</v>
       </c>
       <c r="X4" s="3" t="e">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="7"/>
         <v>#NAME?</v>
       </c>
       <c r="Y4" s="3" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v>#NAME?</v>
       </c>
       <c r="Z4" s="3" t="e">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1" xml:space="preserve"> X4/($B$8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AA4" s="3" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1" xml:space="preserve"> Y4/($B$8)</f>
         <v>#NAME?</v>
+      </c>
+      <c r="AB4" s="1">
+        <f>IF(AB3 &gt;( $B$8 + $B$18*$B$2), AB3 -( $B$18*$B$2), $B$8)</f>
+        <v>100</v>
+      </c>
+      <c r="AC4" s="1">
+        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
+        <v>98066.5</v>
+      </c>
+      <c r="AD4" s="1">
+        <f ca="1" xml:space="preserve"> AC4*COS(M4)</f>
+        <v>85756.906797793345</v>
+      </c>
+      <c r="AE4" s="1">
+        <f ca="1" xml:space="preserve"> AC4*SIN(M4)</f>
+        <v>47568.806572422916</v>
       </c>
       <c r="AJ4"/>
       <c r="AK4"/>
@@ -1565,82 +1748,82 @@
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="24">
         <v>100</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="29" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="10"/>
+        <v>0.4</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ca="1" si="11"/>
+        <v>86.602540378443877</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="12"/>
+        <v>47.056833268115227</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>98.561379643464804</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>25.98076211353316</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="14"/>
+        <v>14.558522031229657</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" ref="K5:K12" ca="1" si="16">K4+ SQRT( (I5-I4)^2 + (J5-J4)^2 )</f>
+        <v>29.782453103453079</v>
+      </c>
+      <c r="L5" s="3">
         <f t="shared" si="15"/>
-        <v>3</v>
-      </c>
-      <c r="E5" s="2">
-        <f t="shared" si="16"/>
-        <v>0.4</v>
-      </c>
-      <c r="F5" s="3">
-        <f t="shared" ca="1" si="17"/>
-        <v>86.602540378443877</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" si="18"/>
-        <v>47.056833268115227</v>
-      </c>
-      <c r="H5" s="3">
+        <v>-9.8102648092300235</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.49773528472143636</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>28.518131129280668</v>
+      </c>
+      <c r="O5" s="1">
+        <f ca="1">(0.5)*($B$8)*(H5^2)</f>
+        <v>485717.27786115988</v>
+      </c>
+      <c r="P5" s="1">
+        <f>($B$8)*L5*J5</f>
+        <v>-14282.295635737231</v>
+      </c>
+      <c r="Q5" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>98.561379643464804</v>
-      </c>
-      <c r="I5" s="3">
-        <f t="shared" ca="1" si="19"/>
-        <v>25.98076211353316</v>
-      </c>
-      <c r="J5" s="3">
-        <f t="shared" si="20"/>
-        <v>14.558522031229657</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" ref="K5:K68" ca="1" si="22">K4+ SQRT( (I5-I4)^2 + (J5-J4)^2 )</f>
-        <v>29.782453103453079</v>
-      </c>
-      <c r="L5" s="3">
-        <f t="shared" si="21"/>
-        <v>-9.8102648092300235</v>
-      </c>
-      <c r="M5" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.49773528472143636</v>
-      </c>
-      <c r="N5" s="3">
+        <v>499999.57349689712</v>
+      </c>
+      <c r="R5" s="1">
+        <f ca="1" xml:space="preserve"> ($B$8)*H5</f>
+        <v>9856.1379643464807</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" si="4"/>
+        <v>340.2408085434663</v>
+      </c>
+      <c r="T5" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>28.518131129280668</v>
-      </c>
-      <c r="O5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>485717.27786115988</v>
-      </c>
-      <c r="P5" s="1">
-        <f t="shared" si="1"/>
-        <v>-14282.295635737231</v>
-      </c>
-      <c r="Q5" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>499999.57349689712</v>
-      </c>
-      <c r="R5" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>9856.1379643464807</v>
-      </c>
-      <c r="S5" s="3">
-        <f t="shared" si="7"/>
-        <v>340.2408085434663</v>
-      </c>
-      <c r="T5" s="13">
-        <f t="shared" ca="1" si="8"/>
         <v>0.28968124095811815</v>
       </c>
       <c r="U5" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1.2024861960387194</v>
       </c>
       <c r="V5" s="5" t="e">
@@ -1648,24 +1831,40 @@
         <v>#NAME?</v>
       </c>
       <c r="W5" s="3" t="e">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">(0.5)*(U5)*(H5)*(V5)*($B$17)</f>
         <v>#NAME?</v>
       </c>
       <c r="X5" s="3" t="e">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="7"/>
         <v>#NAME?</v>
       </c>
       <c r="Y5" s="3" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v>#NAME?</v>
       </c>
       <c r="Z5" s="3" t="e">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1" xml:space="preserve"> X5/($B$8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AA5" s="3" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1" xml:space="preserve"> Y5/($B$8)</f>
         <v>#NAME?</v>
+      </c>
+      <c r="AB5" s="1">
+        <f>IF(AB4 &gt;( $B$8 + $B$18*$B$2), AB4 -( $B$18*$B$2), $B$8)</f>
+        <v>100</v>
+      </c>
+      <c r="AC5" s="1">
+        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
+        <v>98066.5</v>
+      </c>
+      <c r="AD5" s="1">
+        <f ca="1" xml:space="preserve"> AC5*COS(M5)</f>
+        <v>86167.706425625205</v>
+      </c>
+      <c r="AE5" s="1">
+        <f ca="1" xml:space="preserve"> AC5*SIN(M5)</f>
+        <v>46820.559496841452</v>
       </c>
       <c r="AJ5"/>
       <c r="AK5"/>
@@ -1674,82 +1873,82 @@
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="24">
         <v>50</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="1">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" ca="1" si="11"/>
+        <v>86.602540378443877</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="12"/>
+        <v>46.075806787192228</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>98.096788790921551</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>34.641016151377549</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="14"/>
+        <v>19.215154033995031</v>
+      </c>
+      <c r="K6" s="25">
+        <f t="shared" ca="1" si="16"/>
+        <v>39.615266617863831</v>
+      </c>
+      <c r="L6" s="3">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" si="16"/>
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="3">
-        <f t="shared" ca="1" si="17"/>
-        <v>86.602540378443877</v>
-      </c>
-      <c r="G6" s="3">
-        <f t="shared" si="18"/>
-        <v>46.075806787192228</v>
-      </c>
-      <c r="H6" s="3">
+        <v>-9.8101242623479088</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.48894798608108997</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>28.014656003867774</v>
+      </c>
+      <c r="O6" s="1">
+        <f ca="1">(0.5)*($B$8)*(H6^2)</f>
+        <v>481148.99855453358</v>
+      </c>
+      <c r="P6" s="1">
+        <f>($B$8)*L6*J6</f>
+        <v>-18850.304879364692</v>
+      </c>
+      <c r="Q6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>98.096788790921551</v>
-      </c>
-      <c r="I6" s="3">
-        <f t="shared" ca="1" si="19"/>
-        <v>34.641016151377549</v>
-      </c>
-      <c r="J6" s="14">
-        <f t="shared" si="20"/>
-        <v>19.215154033995031</v>
-      </c>
-      <c r="K6" s="29">
-        <f t="shared" ca="1" si="22"/>
-        <v>39.615266617863831</v>
-      </c>
-      <c r="L6" s="3">
-        <f t="shared" si="21"/>
-        <v>-9.8101242623479088</v>
-      </c>
-      <c r="M6" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.48894798608108997</v>
-      </c>
-      <c r="N6" s="3">
+        <v>499999.30343389825</v>
+      </c>
+      <c r="R6" s="1">
+        <f ca="1" xml:space="preserve"> ($B$8)*H6</f>
+        <v>9809.6788790921546</v>
+      </c>
+      <c r="S6" s="3">
+        <f t="shared" si="4"/>
+        <v>340.22187579533477</v>
+      </c>
+      <c r="T6" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>28.014656003867774</v>
-      </c>
-      <c r="O6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>481148.99855453358</v>
-      </c>
-      <c r="P6" s="1">
-        <f t="shared" si="1"/>
-        <v>-18850.304879364692</v>
-      </c>
-      <c r="Q6" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>499999.30343389825</v>
-      </c>
-      <c r="R6" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>9809.6788790921546</v>
-      </c>
-      <c r="S6" s="3">
-        <f t="shared" si="7"/>
-        <v>340.22187579533477</v>
-      </c>
-      <c r="T6" s="13">
-        <f t="shared" ca="1" si="8"/>
         <v>0.28833180865163721</v>
       </c>
       <c r="U6" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1.2019622347376375</v>
       </c>
       <c r="V6" s="5" t="e">
@@ -1757,24 +1956,40 @@
         <v>#NAME?</v>
       </c>
       <c r="W6" s="3" t="e">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">(0.5)*(U6)*(H6)*(V6)*($B$17)</f>
         <v>#NAME?</v>
       </c>
       <c r="X6" s="3" t="e">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="7"/>
         <v>#NAME?</v>
       </c>
       <c r="Y6" s="3" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v>#NAME?</v>
       </c>
       <c r="Z6" s="3" t="e">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1" xml:space="preserve"> X6/($B$8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AA6" s="3" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1" xml:space="preserve"> Y6/($B$8)</f>
         <v>#NAME?</v>
+      </c>
+      <c r="AB6" s="1">
+        <f>IF(AB5 &gt;( $B$8 + $B$18*$B$2), AB5 -( $B$18*$B$2), $B$8)</f>
+        <v>100</v>
+      </c>
+      <c r="AC6" s="1">
+        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
+        <v>98066.5</v>
+      </c>
+      <c r="AD6" s="1">
+        <f ca="1" xml:space="preserve"> AC6*COS(M6)</f>
+        <v>86575.800601626222</v>
+      </c>
+      <c r="AE6" s="1">
+        <f ca="1" xml:space="preserve"> AC6*SIN(M6)</f>
+        <v>46061.580220802854</v>
       </c>
       <c r="AJ6"/>
       <c r="AK6"/>
@@ -1787,79 +2002,79 @@
         <f xml:space="preserve"> B6 *(PI()/180)</f>
         <v>0.87266462599716477</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="29" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="10"/>
+        <v>0.6</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" ca="1" si="11"/>
+        <v>86.602540378443877</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="12"/>
+        <v>45.094794360957437</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>97.639850872771405</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>43.301270189221938</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="14"/>
+        <v>23.773684091402515</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" ca="1" si="16"/>
+        <v>49.402002349673879</v>
+      </c>
+      <c r="L7" s="3">
         <f t="shared" si="15"/>
-        <v>5</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="16"/>
-        <v>0.6</v>
-      </c>
-      <c r="F7" s="3">
-        <f t="shared" ca="1" si="17"/>
-        <v>86.602540378443877</v>
-      </c>
-      <c r="G7" s="3">
-        <f t="shared" si="18"/>
-        <v>45.094794360957437</v>
-      </c>
-      <c r="H7" s="3">
+        <v>-9.8099866763874495</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.48007787748679526</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>27.506436217591968</v>
+      </c>
+      <c r="O7" s="1">
+        <f ca="1">(0.5)*($B$8)*(H7^2)</f>
+        <v>476677.02392285189</v>
+      </c>
+      <c r="P7" s="1">
+        <f>($B$8)*L7*J7</f>
+        <v>-23321.952418530294</v>
+      </c>
+      <c r="Q7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>97.639850872771405</v>
-      </c>
-      <c r="I7" s="3">
-        <f t="shared" ca="1" si="19"/>
-        <v>43.301270189221938</v>
-      </c>
-      <c r="J7" s="3">
-        <f t="shared" si="20"/>
-        <v>23.773684091402515</v>
-      </c>
-      <c r="K7" s="3">
-        <f t="shared" ca="1" si="22"/>
-        <v>49.402002349673879</v>
-      </c>
-      <c r="L7" s="3">
-        <f t="shared" si="21"/>
-        <v>-9.8099866763874495</v>
-      </c>
-      <c r="M7" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.48007787748679526</v>
-      </c>
-      <c r="N7" s="3">
+        <v>499998.97634138219</v>
+      </c>
+      <c r="R7" s="1">
+        <f ca="1" xml:space="preserve"> ($B$8)*H7</f>
+        <v>9763.9850872771403</v>
+      </c>
+      <c r="S7" s="3">
+        <f t="shared" si="4"/>
+        <v>340.20334190616853</v>
+      </c>
+      <c r="T7" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>27.506436217591968</v>
-      </c>
-      <c r="O7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>476677.02392285189</v>
-      </c>
-      <c r="P7" s="1">
-        <f t="shared" si="1"/>
-        <v>-23321.952418530294</v>
-      </c>
-      <c r="Q7" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>499998.97634138219</v>
-      </c>
-      <c r="R7" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>9763.9850872771403</v>
-      </c>
-      <c r="S7" s="3">
-        <f t="shared" si="7"/>
-        <v>340.20334190616853</v>
-      </c>
-      <c r="T7" s="13">
-        <f t="shared" ca="1" si="8"/>
         <v>0.28700438486492424</v>
       </c>
       <c r="U7" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1.2014494811908036</v>
       </c>
       <c r="V7" s="5" t="e">
@@ -1867,108 +2082,124 @@
         <v>#NAME?</v>
       </c>
       <c r="W7" s="3" t="e">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">(0.5)*(U7)*(H7)*(V7)*($B$17)</f>
         <v>#NAME?</v>
       </c>
       <c r="X7" s="3" t="e">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="7"/>
         <v>#NAME?</v>
       </c>
       <c r="Y7" s="3" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v>#NAME?</v>
       </c>
       <c r="Z7" s="3" t="e">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1" xml:space="preserve"> X7/($B$8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AA7" s="3" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1" xml:space="preserve"> Y7/($B$8)</f>
         <v>#NAME?</v>
+      </c>
+      <c r="AB7" s="1">
+        <f>IF(AB6 &gt;( $B$8 + $B$18*$B$2), AB6 -( $B$18*$B$2), $B$8)</f>
+        <v>100</v>
+      </c>
+      <c r="AC7" s="1">
+        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
+        <v>98066.5</v>
+      </c>
+      <c r="AD7" s="1">
+        <f ca="1" xml:space="preserve"> AC7*COS(M7)</f>
+        <v>86980.960643714323</v>
+      </c>
+      <c r="AE7" s="1">
+        <f ca="1" xml:space="preserve"> AC7*SIN(M7)</f>
+        <v>45291.841514191263</v>
       </c>
       <c r="AJ7"/>
       <c r="AK7"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="16">
-        <v>6378137</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>5</v>
+        <v>41</v>
+      </c>
+      <c r="B8" s="24">
+        <v>100</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>22</v>
       </c>
       <c r="D8" s="1">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="10"/>
+        <v>0.7</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" ca="1" si="11"/>
+        <v>86.602540378443877</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="12"/>
+        <v>44.113795693318693</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>97.190673268950377</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>51.961524227066327</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="14"/>
+        <v>28.234113594116323</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" ca="1" si="16"/>
+        <v>59.143430958901575</v>
+      </c>
+      <c r="L8" s="3">
         <f t="shared" si="15"/>
-        <v>6</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="16"/>
-        <v>0.7</v>
-      </c>
-      <c r="F8" s="3">
-        <f t="shared" ca="1" si="17"/>
-        <v>86.602540378443877</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" si="18"/>
-        <v>44.113795693318693</v>
-      </c>
-      <c r="H8" s="3">
+        <v>-9.8098520513066774</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.47112519560883803</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>26.993485330661763</v>
+      </c>
+      <c r="O8" s="1">
+        <f ca="1">(0.5)*($B$8)*(H8^2)</f>
+        <v>472301.34852359322</v>
+      </c>
+      <c r="P8" s="1">
+        <f>($B$8)*L8*J8</f>
+        <v>-27697.247715806774</v>
+      </c>
+      <c r="Q8" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>97.190673268950377</v>
-      </c>
-      <c r="I8" s="3">
-        <f t="shared" ca="1" si="19"/>
-        <v>51.961524227066327</v>
-      </c>
-      <c r="J8" s="3">
-        <f t="shared" si="20"/>
-        <v>28.234113594116323</v>
-      </c>
-      <c r="K8" s="3">
-        <f t="shared" ca="1" si="22"/>
-        <v>59.143430958901575</v>
-      </c>
-      <c r="L8" s="3">
-        <f t="shared" si="21"/>
-        <v>-9.8098520513066774</v>
-      </c>
-      <c r="M8" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.47112519560883803</v>
-      </c>
-      <c r="N8" s="3">
+        <v>499998.59623939998</v>
+      </c>
+      <c r="R8" s="1">
+        <f ca="1" xml:space="preserve"> ($B$8)*H8</f>
+        <v>9719.0673268950377</v>
+      </c>
+      <c r="S8" s="3">
+        <f t="shared" si="4"/>
+        <v>340.18520687031361</v>
+      </c>
+      <c r="T8" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>26.993485330661763</v>
-      </c>
-      <c r="O8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>472301.34852359322</v>
-      </c>
-      <c r="P8" s="1">
-        <f t="shared" si="1"/>
-        <v>-27697.247715806774</v>
-      </c>
-      <c r="Q8" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>499998.59623939998</v>
-      </c>
-      <c r="R8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>9719.0673268950377</v>
-      </c>
-      <c r="S8" s="3">
-        <f t="shared" si="7"/>
-        <v>340.18520687031361</v>
-      </c>
-      <c r="T8" s="13">
-        <f t="shared" ca="1" si="8"/>
         <v>0.28569929352043133</v>
       </c>
       <c r="U8" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1.2009479243857608</v>
       </c>
       <c r="V8" s="5" t="e">
@@ -1976,108 +2207,124 @@
         <v>#NAME?</v>
       </c>
       <c r="W8" s="3" t="e">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">(0.5)*(U8)*(H8)*(V8)*($B$17)</f>
         <v>#NAME?</v>
       </c>
       <c r="X8" s="3" t="e">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="7"/>
         <v>#NAME?</v>
       </c>
       <c r="Y8" s="3" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v>#NAME?</v>
       </c>
       <c r="Z8" s="3" t="e">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1" xml:space="preserve"> X8/($B$8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AA8" s="3" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1" xml:space="preserve"> Y8/($B$8)</f>
         <v>#NAME?</v>
+      </c>
+      <c r="AB8" s="1">
+        <f>IF(AB7 &gt;( $B$8 + $B$18*$B$2), AB7 -( $B$18*$B$2), $B$8)</f>
+        <v>100</v>
+      </c>
+      <c r="AC8" s="1">
+        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
+        <v>98066.5</v>
+      </c>
+      <c r="AD8" s="1">
+        <f ca="1" xml:space="preserve"> AC8*COS(M8)</f>
+        <v>87382.952914843889</v>
+      </c>
+      <c r="AE8" s="1">
+        <f ca="1" xml:space="preserve"> AC8*SIN(M8)</f>
+        <v>44511.323976401523</v>
       </c>
       <c r="AJ8"/>
       <c r="AK8"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="16">
-        <v>6356752.2999999998</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>5</v>
+      <c r="A9" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="24">
+        <v>100</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>22</v>
       </c>
       <c r="D9" s="1">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="10"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" ca="1" si="11"/>
+        <v>86.602540378443877</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="12"/>
+        <v>43.132810488188028</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>96.749363515270446</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>60.621778264910716</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="14"/>
+        <v>32.596443903191663</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" ca="1" si="16"/>
+        <v>68.840333852376247</v>
+      </c>
+      <c r="L9" s="3">
         <f t="shared" si="15"/>
-        <v>7</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" si="16"/>
-        <v>0.79999999999999993</v>
-      </c>
-      <c r="F9" s="3">
-        <f t="shared" ca="1" si="17"/>
-        <v>86.602540378443877</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" si="18"/>
-        <v>43.132810488188028</v>
-      </c>
-      <c r="H9" s="3">
+        <v>-9.8097203870645089</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.46209023443392433</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>26.47582018727465</v>
+      </c>
+      <c r="O9" s="1">
+        <f ca="1">(0.5)*($B$8)*(H9^2)</f>
+        <v>468021.96703049721</v>
+      </c>
+      <c r="P9" s="1">
+        <f>($B$8)*L9*J9</f>
+        <v>-31976.200030294389</v>
+      </c>
+      <c r="Q9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>96.749363515270446</v>
-      </c>
-      <c r="I9" s="3">
-        <f t="shared" ca="1" si="19"/>
-        <v>60.621778264910716</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="20"/>
-        <v>32.596443903191663</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" ca="1" si="22"/>
-        <v>68.840333852376247</v>
-      </c>
-      <c r="L9" s="3">
-        <f t="shared" si="21"/>
-        <v>-9.8097203870645089</v>
-      </c>
-      <c r="M9" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.46209023443392433</v>
-      </c>
-      <c r="N9" s="3">
+        <v>499998.16706079157</v>
+      </c>
+      <c r="R9" s="1">
+        <f ca="1" xml:space="preserve"> ($B$8)*H9</f>
+        <v>9674.9363515270452</v>
+      </c>
+      <c r="S9" s="3">
+        <f t="shared" si="4"/>
+        <v>340.16747068223617</v>
+      </c>
+      <c r="T9" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>26.47582018727465</v>
-      </c>
-      <c r="O9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>468021.96703049721</v>
-      </c>
-      <c r="P9" s="1">
-        <f t="shared" si="1"/>
-        <v>-31976.200030294389</v>
-      </c>
-      <c r="Q9" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>499998.16706079157</v>
-      </c>
-      <c r="R9" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>9674.9363515270452</v>
-      </c>
-      <c r="S9" s="3">
-        <f t="shared" si="7"/>
-        <v>340.16747068223617</v>
-      </c>
-      <c r="T9" s="13">
-        <f t="shared" ca="1" si="8"/>
         <v>0.28441685891137969</v>
       </c>
       <c r="U9" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1.2004575535511621</v>
       </c>
       <c r="V9" s="5" t="e">
@@ -2085,108 +2332,124 @@
         <v>#NAME?</v>
       </c>
       <c r="W9" s="3" t="e">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">(0.5)*(U9)*(H9)*(V9)*($B$17)</f>
         <v>#NAME?</v>
       </c>
       <c r="X9" s="3" t="e">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="7"/>
         <v>#NAME?</v>
       </c>
       <c r="Y9" s="3" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v>#NAME?</v>
       </c>
       <c r="Z9" s="3" t="e">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1" xml:space="preserve"> X9/($B$8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AA9" s="3" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1" xml:space="preserve"> Y9/($B$8)</f>
         <v>#NAME?</v>
+      </c>
+      <c r="AB9" s="1">
+        <f>IF(AB8 &gt;( $B$8 + $B$18*$B$2), AB8 -( $B$18*$B$2), $B$8)</f>
+        <v>100</v>
+      </c>
+      <c r="AC9" s="1">
+        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
+        <v>98066.5</v>
+      </c>
+      <c r="AD9" s="1">
+        <f ca="1" xml:space="preserve"> AC9*COS(M9)</f>
+        <v>87781.53899361004</v>
+      </c>
+      <c r="AE9" s="1">
+        <f ca="1" xml:space="preserve"> AC9*SIN(M9)</f>
+        <v>43720.016401681729</v>
       </c>
       <c r="AJ9"/>
       <c r="AK9"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="16">
-        <v>6365755.0999999996</v>
-      </c>
-      <c r="C10" s="19" t="s">
+        <v>6378137</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="1">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="10"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" ca="1" si="11"/>
+        <v>86.602540378443877</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="12"/>
+        <v>42.151838449481573</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>96.316029219809479</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>69.282032302755098</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="14"/>
+        <v>36.860676350075138</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" ca="1" si="16"/>
+        <v>78.493503195190755</v>
+      </c>
+      <c r="L10" s="3">
         <f t="shared" si="15"/>
-        <v>8</v>
-      </c>
-      <c r="E10" s="2">
-        <f t="shared" si="16"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="F10" s="3">
-        <f t="shared" ca="1" si="17"/>
-        <v>86.602540378443877</v>
-      </c>
-      <c r="G10" s="3">
-        <f t="shared" si="18"/>
-        <v>42.151838449481573</v>
-      </c>
-      <c r="H10" s="3">
+        <v>-9.8095916836207593</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.45297334705206066</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>25.953461017997785</v>
+      </c>
+      <c r="O10" s="1">
+        <f ca="1">(0.5)*($B$8)*(H10^2)</f>
+        <v>463838.87423355965</v>
+      </c>
+      <c r="P10" s="1">
+        <f>($B$8)*L10*J10</f>
+        <v>-36158.818417633353</v>
+      </c>
+      <c r="Q10" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>96.316029219809479</v>
-      </c>
-      <c r="I10" s="3">
-        <f t="shared" ca="1" si="19"/>
-        <v>69.282032302755098</v>
-      </c>
-      <c r="J10" s="3">
-        <f t="shared" si="20"/>
-        <v>36.860676350075138</v>
-      </c>
-      <c r="K10" s="3">
-        <f t="shared" ca="1" si="22"/>
-        <v>78.493503195190755</v>
-      </c>
-      <c r="L10" s="3">
-        <f t="shared" si="21"/>
-        <v>-9.8095916836207593</v>
-      </c>
-      <c r="M10" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.45297334705206066</v>
-      </c>
-      <c r="N10" s="3">
+        <v>499997.69265119301</v>
+      </c>
+      <c r="R10" s="1">
+        <f ca="1" xml:space="preserve"> ($B$8)*H10</f>
+        <v>9631.6029219809479</v>
+      </c>
+      <c r="S10" s="3">
+        <f t="shared" si="4"/>
+        <v>340.15013333652291</v>
+      </c>
+      <c r="T10" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>25.953461017997785</v>
-      </c>
-      <c r="O10" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>463838.87423355965</v>
-      </c>
-      <c r="P10" s="1">
-        <f t="shared" si="1"/>
-        <v>-36158.818417633353</v>
-      </c>
-      <c r="Q10" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>499997.69265119301</v>
-      </c>
-      <c r="R10" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>9631.6029219809479</v>
-      </c>
-      <c r="S10" s="3">
-        <f t="shared" si="7"/>
-        <v>340.15013333652291</v>
-      </c>
-      <c r="T10" s="13">
-        <f t="shared" ca="1" si="8"/>
         <v>0.28315740545225809</v>
       </c>
       <c r="U10" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1.1999783581565004</v>
       </c>
       <c r="V10" s="5" t="e">
@@ -2194,108 +2457,124 @@
         <v>#NAME?</v>
       </c>
       <c r="W10" s="3" t="e">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">(0.5)*(U10)*(H10)*(V10)*($B$17)</f>
         <v>#NAME?</v>
       </c>
       <c r="X10" s="3" t="e">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="7"/>
         <v>#NAME?</v>
       </c>
       <c r="Y10" s="3" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v>#NAME?</v>
       </c>
       <c r="Z10" s="3" t="e">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1" xml:space="preserve"> X10/($B$8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AA10" s="3" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1" xml:space="preserve"> Y10/($B$8)</f>
         <v>#NAME?</v>
+      </c>
+      <c r="AB10" s="1">
+        <f>IF(AB9 &gt;( $B$8 + $B$18*$B$2), AB9 -( $B$18*$B$2), $B$8)</f>
+        <v>100</v>
+      </c>
+      <c r="AC10" s="1">
+        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
+        <v>98066.5</v>
+      </c>
+      <c r="AD10" s="1">
+        <f ca="1" xml:space="preserve"> AC10*COS(M10)</f>
+        <v>88176.475866136883</v>
+      </c>
+      <c r="AE10" s="1">
+        <f ca="1" xml:space="preserve"> AC10*SIN(M10)</f>
+        <v>42917.916143244649</v>
       </c>
       <c r="AJ10"/>
       <c r="AK10"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="28">
-        <v>100</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="B11" s="16">
+        <v>6356752.2999999998</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>5</v>
       </c>
       <c r="D11" s="1">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="10"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" ca="1" si="11"/>
+        <v>86.602540378443877</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="12"/>
+        <v>41.170879281119497</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>95.890777975676656</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>77.94228634059948</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="14"/>
+        <v>41.026812236605195</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" ca="1" si="16"/>
+        <v>88.103741913611515</v>
+      </c>
+      <c r="L11" s="3">
         <f t="shared" si="15"/>
-        <v>9</v>
-      </c>
-      <c r="E11" s="2">
-        <f t="shared" si="16"/>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="F11" s="3">
-        <f t="shared" ca="1" si="17"/>
-        <v>86.602540378443877</v>
-      </c>
-      <c r="G11" s="3">
-        <f t="shared" si="18"/>
-        <v>41.170879281119497</v>
-      </c>
-      <c r="H11" s="3">
+        <v>-9.8094659409361373</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.44377494740405499</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>25.426431539892437</v>
+      </c>
+      <c r="O11" s="1">
+        <f ca="1">(0.5)*($B$8)*(H11^2)</f>
+        <v>459752.06503902574</v>
+      </c>
+      <c r="P11" s="1">
+        <f>($B$8)*L11*J11</f>
+        <v>-40245.111730016062</v>
+      </c>
+      <c r="Q11" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>95.890777975676656</v>
-      </c>
-      <c r="I11" s="3">
-        <f t="shared" ca="1" si="19"/>
-        <v>77.94228634059948</v>
-      </c>
-      <c r="J11" s="3">
-        <f t="shared" si="20"/>
-        <v>41.026812236605195</v>
-      </c>
-      <c r="K11" s="3">
-        <f t="shared" ca="1" si="22"/>
-        <v>88.103741913611515</v>
-      </c>
-      <c r="L11" s="3">
-        <f t="shared" si="21"/>
-        <v>-9.8094659409361373</v>
-      </c>
-      <c r="M11" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.44377494740405499</v>
-      </c>
-      <c r="N11" s="3">
+        <v>499997.17676904181</v>
+      </c>
+      <c r="R11" s="1">
+        <f ca="1" xml:space="preserve"> ($B$8)*H11</f>
+        <v>9589.0777975676647</v>
+      </c>
+      <c r="S11" s="3">
+        <f t="shared" si="4"/>
+        <v>340.13319482788091</v>
+      </c>
+      <c r="T11" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>25.426431539892437</v>
-      </c>
-      <c r="O11" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>459752.06503902574</v>
-      </c>
-      <c r="P11" s="1">
-        <f t="shared" si="1"/>
-        <v>-40245.111730016062</v>
-      </c>
-      <c r="Q11" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>499997.17676904181</v>
-      </c>
-      <c r="R11" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>9589.0777975676647</v>
-      </c>
-      <c r="S11" s="3">
-        <f t="shared" si="7"/>
-        <v>340.13319482788091</v>
-      </c>
-      <c r="T11" s="13">
-        <f t="shared" ca="1" si="8"/>
         <v>0.28192125741858476</v>
       </c>
       <c r="U11" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1.1995103279118349</v>
       </c>
       <c r="V11" s="5" t="e">
@@ -2303,108 +2582,124 @@
         <v>#NAME?</v>
       </c>
       <c r="W11" s="3" t="e">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">(0.5)*(U11)*(H11)*(V11)*($B$17)</f>
         <v>#NAME?</v>
       </c>
       <c r="X11" s="3" t="e">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="7"/>
         <v>#NAME?</v>
       </c>
       <c r="Y11" s="3" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v>#NAME?</v>
       </c>
       <c r="Z11" s="3" t="e">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1" xml:space="preserve"> X11/($B$8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AA11" s="3" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1" xml:space="preserve"> Y11/($B$8)</f>
         <v>#NAME?</v>
+      </c>
+      <c r="AB11" s="1">
+        <f>IF(AB10 &gt;( $B$8 + $B$18*$B$2), AB10 -( $B$18*$B$2), $B$8)</f>
+        <v>100</v>
+      </c>
+      <c r="AC11" s="1">
+        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
+        <v>98066.5</v>
+      </c>
+      <c r="AD11" s="1">
+        <f ca="1" xml:space="preserve"> AC11*COS(M11)</f>
+        <v>88567.516139841144</v>
+      </c>
+      <c r="AE11" s="1">
+        <f ca="1" xml:space="preserve"> AC11*SIN(M11)</f>
+        <v>42105.029474743023</v>
       </c>
       <c r="AJ11"/>
       <c r="AK11"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="C12" s="21" t="s">
+      <c r="A12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="16">
+        <v>6365755.0999999996</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="1">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="10"/>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" ca="1" si="11"/>
+        <v>86.602540378443877</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="12"/>
+        <v>40.18993268702588</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>95.473717270187365</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>86.602540378443862</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="14"/>
+        <v>45.094852835012468</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" ca="1" si="16"/>
+        <v>97.671863689084987</v>
+      </c>
+      <c r="L12" s="3">
         <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="E12" s="2">
-        <f t="shared" si="16"/>
-        <v>1.0999999999999999</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" ca="1" si="17"/>
-        <v>86.602540378443877</v>
-      </c>
-      <c r="G12" s="3">
-        <f t="shared" si="18"/>
-        <v>40.18993268702588</v>
-      </c>
-      <c r="H12" s="3">
+        <v>-9.8093431589722435</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.43449551198192587</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>24.894759053940245</v>
+      </c>
+      <c r="O12" s="1">
+        <f ca="1">(0.5)*($B$8)*(H12^2)</f>
+        <v>455761.53446938371</v>
+      </c>
+      <c r="P12" s="1">
+        <f>($B$8)*L12*J12</f>
+        <v>-44235.088616198962</v>
+      </c>
+      <c r="Q12" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>95.473717270187365</v>
-      </c>
-      <c r="I12" s="3">
-        <f t="shared" ca="1" si="19"/>
-        <v>86.602540378443862</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="20"/>
-        <v>45.094852835012468</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" ca="1" si="22"/>
-        <v>97.671863689084987</v>
-      </c>
-      <c r="L12" s="3">
-        <f t="shared" si="21"/>
-        <v>-9.8093431589722435</v>
-      </c>
-      <c r="M12" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.43449551198192587</v>
-      </c>
-      <c r="N12" s="3">
+        <v>499996.62308558269</v>
+      </c>
+      <c r="R12" s="1">
+        <f ca="1" xml:space="preserve"> ($B$8)*H12</f>
+        <v>9547.3717270187371</v>
+      </c>
+      <c r="S12" s="3">
+        <f t="shared" si="4"/>
+        <v>340.11665515113754</v>
+      </c>
+      <c r="T12" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>24.894759053940245</v>
-      </c>
-      <c r="O12" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>455761.53446938371</v>
-      </c>
-      <c r="P12" s="1">
-        <f t="shared" si="1"/>
-        <v>-44235.088616198962</v>
-      </c>
-      <c r="Q12" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>499996.62308558269</v>
-      </c>
-      <c r="R12" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>9547.3717270187371</v>
-      </c>
-      <c r="S12" s="3">
-        <f t="shared" si="7"/>
-        <v>340.11665515113754</v>
-      </c>
-      <c r="T12" s="13">
-        <f t="shared" ca="1" si="8"/>
         <v>0.2807087386760338</v>
       </c>
       <c r="U12" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1.1990534527675287</v>
       </c>
       <c r="V12" s="5" t="e">
@@ -2412,35 +2707,53 @@
         <v>#NAME?</v>
       </c>
       <c r="W12" s="3" t="e">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">(0.5)*(U12)*(H12)*(V12)*($B$17)</f>
         <v>#NAME?</v>
       </c>
       <c r="X12" s="3" t="e">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="7"/>
         <v>#NAME?</v>
       </c>
       <c r="Y12" s="3" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v>#NAME?</v>
       </c>
       <c r="Z12" s="3" t="e">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1" xml:space="preserve"> X12/($B$8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AA12" s="3" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1" xml:space="preserve"> Y12/($B$8)</f>
         <v>#NAME?</v>
+      </c>
+      <c r="AB12" s="1">
+        <f>IF(AB11 &gt;( $B$8 + $B$18*$B$2), AB11 -( $B$18*$B$2), $B$8)</f>
+        <v>100</v>
+      </c>
+      <c r="AC12" s="1">
+        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
+        <v>98066.5</v>
+      </c>
+      <c r="AD12" s="1">
+        <f ca="1" xml:space="preserve"> AC12*COS(M12)</f>
+        <v>88954.408279592899</v>
+      </c>
+      <c r="AE12" s="1">
+        <f ca="1" xml:space="preserve"> AC12*SIN(M12)</f>
+        <v>41281.371947616935</v>
       </c>
       <c r="AJ12"/>
       <c r="AK12"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="22">
-        <f xml:space="preserve"> PI()*((B12/2)^2)</f>
-        <v>0.19634954084936207</v>
+        <v>43</v>
+      </c>
+      <c r="B13" s="28">
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>44</v>
       </c>
       <c r="Q13" s="1"/>
       <c r="S13" s="3"/>
@@ -2466,6 +2779,15 @@
       <c r="AK15"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>5</v>
+      </c>
       <c r="Q16" s="1"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
@@ -2473,7 +2795,17 @@
       <c r="AJ16"/>
       <c r="AK16"/>
     </row>
-    <row r="17" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="19">
+        <f xml:space="preserve"> PI()*((B16/2)^2)</f>
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>45</v>
+      </c>
       <c r="Q17" s="1"/>
       <c r="S17" s="3"/>
       <c r="T17" s="13"/>
@@ -2481,7 +2813,16 @@
       <c r="AJ17"/>
       <c r="AK17"/>
     </row>
-    <row r="18" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="24">
+        <v>100</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>46</v>
+      </c>
       <c r="Q18" s="1"/>
       <c r="S18" s="3"/>
       <c r="T18" s="13"/>
@@ -2489,7 +2830,16 @@
       <c r="AJ18"/>
       <c r="AK18"/>
     </row>
-    <row r="19" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="24">
+        <v>100</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>1</v>
+      </c>
       <c r="Q19" s="1"/>
       <c r="S19" s="3"/>
       <c r="T19" s="13"/>
@@ -2497,7 +2847,17 @@
       <c r="AJ19"/>
       <c r="AK19"/>
     </row>
-    <row r="20" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A20" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="27">
+        <f xml:space="preserve"> B19*B13*B18</f>
+        <v>98066.5</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>49</v>
+      </c>
       <c r="Q20" s="1"/>
       <c r="S20" s="3"/>
       <c r="T20" s="13"/>
@@ -2505,7 +2865,7 @@
       <c r="AJ20"/>
       <c r="AK20"/>
     </row>
-    <row r="21" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q21" s="1"/>
       <c r="S21" s="3"/>
       <c r="T21" s="13"/>
@@ -2513,7 +2873,7 @@
       <c r="AJ21"/>
       <c r="AK21"/>
     </row>
-    <row r="22" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q22" s="1"/>
       <c r="S22" s="3"/>
       <c r="T22" s="13"/>
@@ -2521,7 +2881,7 @@
       <c r="AJ22"/>
       <c r="AK22"/>
     </row>
-    <row r="23" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q23" s="1"/>
       <c r="S23" s="3"/>
       <c r="T23" s="13"/>
@@ -2529,7 +2889,7 @@
       <c r="AJ23"/>
       <c r="AK23"/>
     </row>
-    <row r="24" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q24" s="1"/>
       <c r="S24" s="3"/>
       <c r="T24" s="13"/>
@@ -2537,7 +2897,7 @@
       <c r="AJ24"/>
       <c r="AK24"/>
     </row>
-    <row r="25" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q25" s="1"/>
       <c r="S25" s="3"/>
       <c r="T25" s="13"/>
@@ -2545,7 +2905,7 @@
       <c r="AJ25"/>
       <c r="AK25"/>
     </row>
-    <row r="26" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q26" s="1"/>
       <c r="S26" s="3"/>
       <c r="T26" s="13"/>
@@ -2553,7 +2913,7 @@
       <c r="AJ26"/>
       <c r="AK26"/>
     </row>
-    <row r="27" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q27" s="1"/>
       <c r="S27" s="3"/>
       <c r="T27" s="13"/>
@@ -2561,7 +2921,7 @@
       <c r="AJ27"/>
       <c r="AK27"/>
     </row>
-    <row r="28" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q28" s="1"/>
       <c r="S28" s="3"/>
       <c r="T28" s="13"/>
@@ -2569,7 +2929,7 @@
       <c r="AJ28"/>
       <c r="AK28"/>
     </row>
-    <row r="29" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q29" s="1"/>
       <c r="S29" s="3"/>
       <c r="T29" s="13"/>
@@ -2577,7 +2937,7 @@
       <c r="AJ29"/>
       <c r="AK29"/>
     </row>
-    <row r="30" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q30" s="1"/>
       <c r="S30" s="3"/>
       <c r="T30" s="13"/>
@@ -2585,7 +2945,7 @@
       <c r="AJ30"/>
       <c r="AK30"/>
     </row>
-    <row r="31" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q31" s="1"/>
       <c r="S31" s="3"/>
       <c r="T31" s="13"/>
@@ -2593,7 +2953,7 @@
       <c r="AJ31"/>
       <c r="AK31"/>
     </row>
-    <row r="32" spans="17:37" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Q32" s="1"/>
       <c r="S32" s="3"/>
       <c r="T32" s="13"/>
@@ -19677,7 +20037,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="J3:J2687">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>

</xml_diff>

<commit_message>
added columns: atm P, Temp, updated speed of sound model, updated gravity model
</commit_message>
<xml_diff>
--- a/Aero210/dynamics_template.xlsx
+++ b/Aero210/dynamics_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="460" windowWidth="15540" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="12840" yWindow="0" windowWidth="12760" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -145,9 +145,8 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">Local gravity
-Calculates gravity based on latitudate using the ellipsoidal gravity model (refer to module 2 powerpoint).
-</t>
+          <t>Local gravity
+IF(height&lt;100km, ellipsoidal gravity model, newtonian model)</t>
         </r>
       </text>
     </comment>
@@ -250,8 +249,9 @@
             <rFont val="Calibri"/>
           </rPr>
           <t>Speed of sound
-MSL to 10,000m: c = -0.00406576h + 340.3 m/s
-10,000m to 20,000m: 295 m/s</t>
+MSL to 10km: c = -0.00406576h + 340.3 m/s
+10km to 100km: Ninth order polynomial
+IF(height&lt;100000, IF(height&gt;10000, polynomial, MSL to 10km model), "")</t>
         </r>
       </text>
     </comment>
@@ -388,7 +388,8 @@
           </rPr>
           <t>Thrust
 Th = (Isp)(g0)(m')
-Th = (specific impulse)(standard gravity)(rate of mass loss)</t>
+Th = (specific impulse)(standard gravity)(rate of mass loss)
+IF(height &gt; ignition height, apply thrust, 0)</t>
         </r>
       </text>
     </comment>
@@ -420,12 +421,40 @@
         </r>
       </text>
     </comment>
+    <comment ref="AF1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Atmospheric Pressure
+P = [101325(1 - (2.25577*10^-5)*h)^5.25588]
+IF(height &gt; 38,000m, 0, atmospheric pressure)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AG1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Temperature
+T = 1.6667c - 273.15
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
   <si>
     <t>Constants</t>
   </si>
@@ -587,6 +616,15 @@
   </si>
   <si>
     <t>mdot (kg/s)</t>
+  </si>
+  <si>
+    <t>Ignition height</t>
+  </si>
+  <si>
+    <t>atm P (kPa)</t>
+  </si>
+  <si>
+    <t>Temp (K)</t>
   </si>
 </sst>
 </file>
@@ -882,7 +920,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -903,6 +940,7 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="16" fillId="9" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
@@ -1262,15 +1300,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK2687"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="17" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="30" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="29" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" style="2" customWidth="1"/>
     <col min="6" max="14" width="10.6640625" style="3" customWidth="1"/>
@@ -1280,16 +1318,16 @@
     <col min="19" max="19" width="10.6640625" style="5" customWidth="1"/>
     <col min="20" max="21" width="10.6640625" customWidth="1"/>
     <col min="22" max="22" width="10.6640625" style="5" customWidth="1"/>
-    <col min="23" max="31" width="10.6640625" style="3" customWidth="1"/>
-    <col min="32" max="16384" width="10.83203125" style="5"/>
+    <col min="23" max="33" width="10.6640625" style="3" customWidth="1"/>
+    <col min="34" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
       <c r="D1" s="8" t="s">
         <v>10</v>
       </c>
@@ -1373,6 +1411,12 @@
       </c>
       <c r="AE1" s="21" t="s">
         <v>51</v>
+      </c>
+      <c r="AF1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG1" s="21" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
@@ -1382,7 +1426,7 @@
       <c r="B2" s="23">
         <v>0.1</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="28" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1">
@@ -1415,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="3">
-        <f xml:space="preserve"> -(9.780327 * (1 + 0.0053024 * ((SIN($B$7))^2) - (5.8*10^(-6)) * (SIN(2*($B$7))^2) - (3.086*10^(-6)) * J2))</f>
+        <f>IF(J2&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*J2)+((6.26*10^(-13))*(J2)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
         <v>-9.8107042158394542</v>
       </c>
       <c r="M2" s="3">
@@ -1427,11 +1471,11 @@
         <v>29.999999999999996</v>
       </c>
       <c r="O2" s="1">
-        <f>(0.5)*($B$8)*(H2^2)</f>
+        <f t="shared" ref="O2:O12" si="0">(0.5)*($B$8)*(H2^2)</f>
         <v>500000</v>
       </c>
       <c r="P2" s="1">
-        <f>($B$8)*L2*J2</f>
+        <f t="shared" ref="P2:P12" si="1">($B$8)*L2*J2</f>
         <v>0</v>
       </c>
       <c r="Q2" s="1">
@@ -1439,11 +1483,11 @@
         <v>500000</v>
       </c>
       <c r="R2" s="1">
-        <f xml:space="preserve"> ($B$8)*H2</f>
+        <f t="shared" ref="R2:R12" si="2" xml:space="preserve"> ($B$8)*H2</f>
         <v>10000</v>
       </c>
       <c r="S2" s="3">
-        <f>IF(J2&lt;30000,( (-0.00406576*J2)+340.3), "")</f>
+        <f>IF(J2&lt;100000, IF(J2&gt;10000, (343.2)+(-4.313943*J2)+(-0.291943*J2^2)+(0.053721*J2^3)+((-3.039687*10^(-3))*J2^4)+((9.262166*10^(-5))*J2^5)+((-1.647967*10^(-6))*J2^6)+((1.694814*10^(-8))*J2^7)+((-9.299892*10^(-11))*J2^8)+((2.104694*10^(-13))*J2^9), ((-0.00406576*J2)+340.3)), "")</f>
         <v>340.3</v>
       </c>
       <c r="T2" s="13">
@@ -1459,7 +1503,7 @@
         <v>#NAME?</v>
       </c>
       <c r="W2" s="3" t="e">
-        <f>(0.5)*(U2)*(H2)*(V2)*($B$17)</f>
+        <f t="shared" ref="W2:W12" si="3">(0.5)*(U2)*(H2)*(V2)*($B$17)</f>
         <v>#NAME?</v>
       </c>
       <c r="X2" s="3" t="e">
@@ -1478,21 +1522,29 @@
         <f xml:space="preserve"> (Y2+AE2)/($B$8)</f>
         <v>#NAME?</v>
       </c>
-      <c r="AB2" s="34">
+      <c r="AB2" s="33">
         <f xml:space="preserve"> 0</f>
         <v>0</v>
       </c>
       <c r="AC2" s="1">
-        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
-        <v>98066.5</v>
+        <f>IF(J2&gt;($B$21), $B$19*$B$13*$B$18, 0)</f>
+        <v>0</v>
       </c>
       <c r="AD2" s="1">
-        <f xml:space="preserve"> AC2*COS(M2)</f>
-        <v>84928.080260226663</v>
+        <f t="shared" ref="AD2:AD12" si="4" xml:space="preserve"> AC2*COS(M2)</f>
+        <v>0</v>
       </c>
       <c r="AE2" s="1">
-        <f xml:space="preserve"> AC2*SIN(M2)</f>
-        <v>49033.249999999993</v>
+        <f t="shared" ref="AE2:AE12" si="5" xml:space="preserve"> AC2*SIN(M2)</f>
+        <v>0</v>
+      </c>
+      <c r="AF2" s="1">
+        <f>IF(J2&gt;38000,0,(101325*(1-(2.25577*10^(-5))*J2)^5.25588))</f>
+        <v>101325</v>
+      </c>
+      <c r="AG2" s="1">
+        <f>1.6667*S2-273.15</f>
+        <v>294.02801000000011</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
@@ -1502,7 +1554,7 @@
       <c r="B3" s="24">
         <v>30</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1">
@@ -1522,7 +1574,7 @@
         <v>49.018929578416049</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H12" ca="1" si="0">SQRT(F3^2 + G3^2)</f>
+        <f t="shared" ref="H3:H12" ca="1" si="6">SQRT(F3^2 + G3^2)</f>
         <v>99.51309188751857</v>
       </c>
       <c r="I3" s="3">
@@ -1538,43 +1590,43 @@
         <v>9.9755636952073186</v>
       </c>
       <c r="L3" s="3">
-        <f xml:space="preserve"> -(9.780327 * (1 + 0.0053024 * ((SIN($B$7))^2) - (5.8*10^(-6)) * (SIN(2*($B$7))^2) - (3.086*10^(-6)) * J3))</f>
-        <v>-9.810554785931588</v>
+        <f t="shared" ref="L3:L12" si="7">IF(J3&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*J3)+((6.26*10^(-13))*(J3)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
+        <v>-9.8106889372339641</v>
       </c>
       <c r="M3" s="3">
-        <f t="shared" ref="M3:M12" ca="1" si="1">ATAN(G3/F3)</f>
+        <f t="shared" ref="M3:M12" ca="1" si="8">ATAN(G3/F3)</f>
         <v>0.51506078110312425</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N12" ca="1" si="2">M3*(180/PI())</f>
+        <f t="shared" ref="N3:N12" ca="1" si="9">M3*(180/PI())</f>
         <v>29.510808949920566</v>
       </c>
       <c r="O3" s="1">
-        <f ca="1">(0.5)*($B$8)*(H3^2)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>495142.77285068575</v>
       </c>
       <c r="P3" s="1">
-        <f>($B$8)*L3*J3</f>
-        <v>-4857.1531673667623</v>
+        <f t="shared" si="1"/>
+        <v>-4857.2195849585769</v>
       </c>
       <c r="Q3" s="1">
-        <f t="shared" ref="Q3:Q12" ca="1" si="3" xml:space="preserve"> ABS(O3) + ABS(P3)</f>
-        <v>499999.9260180525</v>
+        <f t="shared" ref="Q3:Q12" ca="1" si="10" xml:space="preserve"> ABS(O3) + ABS(P3)</f>
+        <v>499999.99243564432</v>
       </c>
       <c r="R3" s="1">
-        <f ca="1" xml:space="preserve"> ($B$8)*H3</f>
+        <f t="shared" ca="1" si="2"/>
         <v>9951.3091887518567</v>
       </c>
       <c r="S3" s="3">
-        <f t="shared" ref="S3:S12" si="4">IF(J3&lt;30000,( (-0.00406576*J3)+340.3), "")</f>
+        <f t="shared" ref="S3:S12" si="11">IF(J3&lt;100000, IF(J3&gt;10000, (343.2)+(-4.313943*J3)+(-0.291943*J3^2)+(0.053721*J3^3)+((-3.039687*10^(-3))*J3^4)+((9.262166*10^(-5))*J3^5)+((-1.647967*10^(-6))*J3^6)+((1.694814*10^(-8))*J3^7)+((-9.299892*10^(-11))*J3^8)+((2.104694*10^(-13))*J3^9), ((-0.00406576*J3)+340.3)), "")</f>
         <v>340.27987063984386</v>
       </c>
       <c r="T3" s="13">
-        <f t="shared" ref="T3:T12" ca="1" si="5" xml:space="preserve"> IF(J3&lt;30000, H3/S3, "")</f>
+        <f t="shared" ref="T3:T12" ca="1" si="12" xml:space="preserve"> IF(J3&lt;30000, H3/S3, "")</f>
         <v>0.29244483871584742</v>
       </c>
       <c r="U3" s="13">
-        <f t="shared" ref="U3:U12" si="6" xml:space="preserve"> IF(J3&lt;30000, (( 359.01*(1 - (2.25577*10^(-5))*(J3))^(5.25588) ) / (298.15 - 0.0074545*J3)), "")</f>
+        <f t="shared" ref="U3:U12" si="13" xml:space="preserve"> IF(J3&lt;30000, (( 359.01*(1 - (2.25577*10^(-5))*(J3))^(5.25588) ) / (298.15 - 0.0074545*J3)), "")</f>
         <v>1.2035677871607093</v>
       </c>
       <c r="V3" s="5" t="e">
@@ -1582,40 +1634,48 @@
         <v>#NAME?</v>
       </c>
       <c r="W3" s="3" t="e">
-        <f ca="1">(0.5)*(U3)*(H3)*(V3)*($B$17)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="X3" s="3" t="e">
-        <f t="shared" ref="X3:X12" ca="1" si="7" xml:space="preserve"> - W3*COS(M3)</f>
+        <f t="shared" ref="X3:X12" ca="1" si="14" xml:space="preserve"> - W3*COS(M3)</f>
         <v>#NAME?</v>
       </c>
       <c r="Y3" s="3" t="e">
-        <f t="shared" ref="Y3:Y12" ca="1" si="8" xml:space="preserve"> - W3*SIN(M3)</f>
+        <f t="shared" ref="Y3:Y12" ca="1" si="15" xml:space="preserve"> - W3*SIN(M3)</f>
         <v>#NAME?</v>
       </c>
       <c r="Z3" s="3" t="e">
-        <f ca="1" xml:space="preserve"> X3/($B$8)</f>
+        <f t="shared" ref="Z3:Z12" ca="1" si="16" xml:space="preserve"> X3/($B$8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AA3" s="3" t="e">
-        <f ca="1" xml:space="preserve"> Y3/($B$8)</f>
+        <f t="shared" ref="AA3:AA12" ca="1" si="17" xml:space="preserve"> Y3/($B$8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AB3" s="1">
-        <f>IF(AB2 &gt;( $B$8 + $B$18*$B$2), AB2 -( $B$18*$B$2), $B$8)</f>
+        <f t="shared" ref="AB3:AB12" si="18">IF(AB2 &gt;( $B$8 + $B$18*$B$2), AB2 -( $B$18*$B$2), $B$8)</f>
         <v>100</v>
       </c>
       <c r="AC3" s="1">
-        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
-        <v>98066.5</v>
+        <f>IF(J3&gt;($B$21), $B$19*$B$13*$B$18, 0)</f>
+        <v>0</v>
       </c>
       <c r="AD3" s="1">
-        <f ca="1" xml:space="preserve"> AC3*COS(M3)</f>
-        <v>85343.625295275124</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="AE3" s="1">
-        <f ca="1" xml:space="preserve"> AC3*SIN(M3)</f>
-        <v>48306.356141916534</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF3" s="1">
+        <f t="shared" ref="AF3:AG11" si="19">IF(J3&gt;38000,0,(101325*(1-(2.25577*10^(-5))*J3)^5.25588))</f>
+        <v>101265.53767440718</v>
+      </c>
+      <c r="AG3" s="1">
+        <f t="shared" si="19"/>
+        <v>101205.21943456748</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
@@ -1626,120 +1686,128 @@
         <f>B3*(PI()/180)</f>
         <v>0.52359877559829882</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D12" si="9">D3 + 1</f>
+        <f t="shared" ref="D4:D12" si="20">D3 + 1</f>
         <v>2</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" ref="E4:E12" si="10" xml:space="preserve"> E3 + $B$2</f>
+        <f t="shared" ref="E4:E12" si="21" xml:space="preserve"> E3 + $B$2</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:F12" ca="1" si="11">INDIRECT(ADDRESS(ROW()-1,COLUMN()))</f>
+        <f t="shared" ref="F4:F12" ca="1" si="22">INDIRECT(ADDRESS(ROW()-1,COLUMN()))</f>
         <v>86.602540378443877</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G4:G12" si="12">G3 + L3*$B$2</f>
-        <v>48.037874099822893</v>
+        <f t="shared" ref="G4:G12" si="23">G3 + L3*$B$2</f>
+        <v>48.037860684692653</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>99.033516286308028</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>99.033509779073981</v>
       </c>
       <c r="I4" s="3">
-        <f t="shared" ref="I4:I12" ca="1" si="13">I3 + F3*($B$2)</f>
+        <f t="shared" ref="I4:I12" ca="1" si="24">I3 + F3*($B$2)</f>
         <v>17.320508075688775</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J12" si="14" xml:space="preserve"> J3 + G3*($B$2) + (0.5)*(L3)*($B$2)^2</f>
-        <v>9.803786662832751</v>
+        <f t="shared" ref="J4:J12" si="25" xml:space="preserve"> J3 + G3*($B$2) + (0.5)*(L3)*($B$2)^2</f>
+        <v>9.8037859920762394</v>
       </c>
       <c r="K4" s="3">
         <f ca="1">K3+ SQRT( (I4-I3)^2 + (J4-J3)^2 )</f>
-        <v>19.902801873602684</v>
+        <v>19.902801545709476</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" ref="L4:L12" si="15" xml:space="preserve"> -(9.780327 * (1 + 0.0053024 * ((SIN($B$7))^2) - (5.8*10^(-6)) * (SIN(2*($B$7))^2) - (3.086*10^(-6)) * J4))</f>
-        <v>-9.8104083170766643</v>
+        <f t="shared" si="7"/>
+        <v>-9.8106739614160503</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.50643959223510326</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.50643947377798737</v>
       </c>
       <c r="N4" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>29.016844426305003</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>490381.80295809708</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" si="1"/>
+        <v>-9618.1747955757783</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" ca="1" si="10"/>
+        <v>499999.97775367287</v>
+      </c>
+      <c r="R4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>29.016851213397796</v>
-      </c>
-      <c r="O4" s="1">
-        <f ca="1">(0.5)*($B$8)*(H4^2)</f>
-        <v>490381.86740152189</v>
-      </c>
-      <c r="P4" s="1">
-        <f>($B$8)*L4*J4</f>
-        <v>-9617.9150215899699</v>
-      </c>
-      <c r="Q4" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>499999.78242311184</v>
-      </c>
-      <c r="R4" s="1">
-        <f ca="1" xml:space="preserve"> ($B$8)*H4</f>
-        <v>9903.3516286308022</v>
+        <v>9903.3509779073975</v>
       </c>
       <c r="S4" s="3">
-        <f t="shared" si="4"/>
-        <v>340.26014015633774</v>
+        <f t="shared" si="11"/>
+        <v>340.26014015906486</v>
       </c>
       <c r="T4" s="13">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.2910523584713906</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.29105233934476654</v>
       </c>
       <c r="U4" s="13">
-        <f t="shared" si="6"/>
-        <v>1.2030213763478994</v>
+        <f t="shared" si="13"/>
+        <v>1.2030213764234103</v>
       </c>
       <c r="V4" s="5" t="e">
         <f>IF(Mach&lt;cross, subsonic, IF(Mach&lt;cross, transonic, supersonic))</f>
         <v>#NAME?</v>
       </c>
       <c r="W4" s="3" t="e">
-        <f ca="1">(0.5)*(U4)*(H4)*(V4)*($B$17)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="X4" s="3" t="e">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="14"/>
         <v>#NAME?</v>
       </c>
       <c r="Y4" s="3" t="e">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#NAME?</v>
       </c>
       <c r="Z4" s="3" t="e">
-        <f ca="1" xml:space="preserve"> X4/($B$8)</f>
+        <f t="shared" ca="1" si="16"/>
         <v>#NAME?</v>
       </c>
       <c r="AA4" s="3" t="e">
-        <f ca="1" xml:space="preserve"> Y4/($B$8)</f>
+        <f t="shared" ca="1" si="17"/>
         <v>#NAME?</v>
       </c>
       <c r="AB4" s="1">
-        <f>IF(AB3 &gt;( $B$8 + $B$18*$B$2), AB3 -( $B$18*$B$2), $B$8)</f>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
       <c r="AC4" s="1">
-        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
-        <v>98066.5</v>
+        <f t="shared" ref="AC4:AC12" si="26">IF(J4&gt;($B$21), $B$19*$B$13*$B$18, 0)</f>
+        <v>0</v>
       </c>
       <c r="AD4" s="1">
-        <f ca="1" xml:space="preserve"> AC4*COS(M4)</f>
-        <v>85756.906797793345</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="AE4" s="1">
-        <f ca="1" xml:space="preserve"> AC4*SIN(M4)</f>
-        <v>47568.806572422916</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF4" s="1">
+        <f t="shared" si="19"/>
+        <v>101207.28106720161</v>
+      </c>
+      <c r="AG4" s="1">
+        <f t="shared" ca="1" si="19"/>
+        <v>101086.1329875744</v>
       </c>
       <c r="AJ4"/>
       <c r="AK4"/>
@@ -1751,120 +1819,128 @@
       <c r="B5" s="24">
         <v>100</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>3</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>0.4</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="22"/>
         <v>86.602540378443877</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" si="12"/>
-        <v>47.056833268115227</v>
+        <f t="shared" si="23"/>
+        <v>47.056793288551049</v>
       </c>
       <c r="H5" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>98.561360555754433</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" ca="1" si="24"/>
+        <v>25.98076211353316</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="25"/>
+        <v>14.558518690738424</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" ref="K5:K12" ca="1" si="27">K4+ SQRT( (I5-I4)^2 + (J5-J4)^2 )</f>
+        <v>29.782451490708912</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="7"/>
+        <v>-9.8106592883834551</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.49773492830705196</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>28.518110708240688</v>
+      </c>
+      <c r="O5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>98.561379643464804</v>
-      </c>
-      <c r="I5" s="3">
-        <f t="shared" ca="1" si="13"/>
-        <v>25.98076211353316</v>
-      </c>
-      <c r="J5" s="3">
-        <f t="shared" si="14"/>
-        <v>14.558522031229657</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" ref="K5:K12" ca="1" si="16">K4+ SQRT( (I5-I4)^2 + (J5-J4)^2 )</f>
-        <v>29.782453103453079</v>
-      </c>
-      <c r="L5" s="3">
-        <f t="shared" si="15"/>
-        <v>-9.8102648092300235</v>
-      </c>
-      <c r="M5" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.49773528472143636</v>
-      </c>
-      <c r="N5" s="3">
+        <v>485717.08973007125</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="1"/>
+        <v>-14282.866661839706</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" ca="1" si="10"/>
+        <v>499999.95639191096</v>
+      </c>
+      <c r="R5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>28.518131129280668</v>
-      </c>
-      <c r="O5" s="1">
-        <f ca="1">(0.5)*($B$8)*(H5^2)</f>
-        <v>485717.27786115988</v>
-      </c>
-      <c r="P5" s="1">
-        <f>($B$8)*L5*J5</f>
-        <v>-14282.295635737231</v>
-      </c>
-      <c r="Q5" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>499999.57349689712</v>
-      </c>
-      <c r="R5" s="1">
-        <f ca="1" xml:space="preserve"> ($B$8)*H5</f>
-        <v>9856.1379643464807</v>
+        <v>9856.1360555754436</v>
       </c>
       <c r="S5" s="3">
-        <f t="shared" si="4"/>
-        <v>340.2408085434663</v>
+        <f t="shared" si="11"/>
+        <v>340.24080855704796</v>
       </c>
       <c r="T5" s="13">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.28968124095811815</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.28968118484596395</v>
       </c>
       <c r="U5" s="13">
-        <f t="shared" si="6"/>
-        <v>1.2024861960387194</v>
+        <f t="shared" si="13"/>
+        <v>1.2024861964146523</v>
       </c>
       <c r="V5" s="5" t="e">
         <f>IF(Mach&lt;cross, subsonic, IF(Mach&lt;cross, transonic, supersonic))</f>
         <v>#NAME?</v>
       </c>
       <c r="W5" s="3" t="e">
-        <f ca="1">(0.5)*(U5)*(H5)*(V5)*($B$17)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="X5" s="3" t="e">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="14"/>
         <v>#NAME?</v>
       </c>
       <c r="Y5" s="3" t="e">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#NAME?</v>
       </c>
       <c r="Z5" s="3" t="e">
-        <f ca="1" xml:space="preserve"> X5/($B$8)</f>
+        <f t="shared" ca="1" si="16"/>
         <v>#NAME?</v>
       </c>
       <c r="AA5" s="3" t="e">
-        <f ca="1" xml:space="preserve"> Y5/($B$8)</f>
+        <f t="shared" ca="1" si="17"/>
         <v>#NAME?</v>
       </c>
       <c r="AB5" s="1">
-        <f>IF(AB4 &gt;( $B$8 + $B$18*$B$2), AB4 -( $B$18*$B$2), $B$8)</f>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
       <c r="AC5" s="1">
-        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
-        <v>98066.5</v>
+        <f t="shared" si="26"/>
+        <v>0</v>
       </c>
       <c r="AD5" s="1">
-        <f ca="1" xml:space="preserve"> AC5*COS(M5)</f>
-        <v>86167.706425625205</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="AE5" s="1">
-        <f ca="1" xml:space="preserve"> AC5*SIN(M5)</f>
-        <v>46820.559496841452</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1">
+        <f t="shared" si="19"/>
+        <v>101150.22852053362</v>
+      </c>
+      <c r="AG5" s="1">
+        <f t="shared" ca="1" si="19"/>
+        <v>100967.73007852238</v>
       </c>
       <c r="AJ5"/>
       <c r="AK5"/>
@@ -1876,120 +1952,128 @@
       <c r="B6" s="24">
         <v>50</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>0.5</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="22"/>
         <v>86.602540378443877</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="12"/>
-        <v>46.075806787192228</v>
+        <f t="shared" si="23"/>
+        <v>46.075727359712701</v>
       </c>
       <c r="H6" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>98.096751484065862</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" ca="1" si="24"/>
+        <v>34.641016151377549</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="25"/>
+        <v>19.21514472315161</v>
+      </c>
+      <c r="K6" s="25">
+        <f t="shared" ca="1" si="27"/>
+        <v>39.615262177676712</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" si="7"/>
+        <v>-9.8106449181339705</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.48894727126882392</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>28.014615048141788</v>
+      </c>
+      <c r="O6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>98.096788790921551</v>
-      </c>
-      <c r="I6" s="3">
-        <f t="shared" ca="1" si="13"/>
-        <v>34.641016151377549</v>
-      </c>
-      <c r="J6" s="14">
-        <f t="shared" si="14"/>
-        <v>19.215154033995031</v>
-      </c>
-      <c r="K6" s="25">
-        <f t="shared" ca="1" si="16"/>
-        <v>39.615266617863831</v>
-      </c>
-      <c r="L6" s="3">
-        <f t="shared" si="15"/>
-        <v>-9.8101242623479088</v>
-      </c>
-      <c r="M6" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.48894798608108997</v>
-      </c>
-      <c r="N6" s="3">
+        <v>481148.63258632884</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="1"/>
+        <v>-18851.296192939612</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" ca="1" si="10"/>
+        <v>499999.92877926846</v>
+      </c>
+      <c r="R6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>28.014656003867774</v>
-      </c>
-      <c r="O6" s="1">
-        <f ca="1">(0.5)*($B$8)*(H6^2)</f>
-        <v>481148.99855453358</v>
-      </c>
-      <c r="P6" s="1">
-        <f>($B$8)*L6*J6</f>
-        <v>-18850.304879364692</v>
-      </c>
-      <c r="Q6" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>499999.30343389825</v>
-      </c>
-      <c r="R6" s="1">
-        <f ca="1" xml:space="preserve"> ($B$8)*H6</f>
-        <v>9809.6788790921546</v>
+        <v>9809.6751484065862</v>
       </c>
       <c r="S6" s="3">
-        <f t="shared" si="4"/>
-        <v>340.22187579533477</v>
+        <f t="shared" si="11"/>
+        <v>340.22187583319044</v>
       </c>
       <c r="T6" s="13">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.28833180865163721</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.288331698965067</v>
       </c>
       <c r="U6" s="13">
-        <f t="shared" si="6"/>
-        <v>1.2019622347376375</v>
+        <f t="shared" si="13"/>
+        <v>1.201962235785113</v>
       </c>
       <c r="V6" s="5" t="e">
         <f>IF(Mach&lt;cross, subsonic, IF(Mach&lt;cross, transonic, supersonic))</f>
         <v>#NAME?</v>
       </c>
       <c r="W6" s="3" t="e">
-        <f ca="1">(0.5)*(U6)*(H6)*(V6)*($B$17)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="X6" s="3" t="e">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="14"/>
         <v>#NAME?</v>
       </c>
       <c r="Y6" s="3" t="e">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#NAME?</v>
       </c>
       <c r="Z6" s="3" t="e">
-        <f ca="1" xml:space="preserve"> X6/($B$8)</f>
+        <f t="shared" ca="1" si="16"/>
         <v>#NAME?</v>
       </c>
       <c r="AA6" s="3" t="e">
-        <f ca="1" xml:space="preserve"> Y6/($B$8)</f>
+        <f t="shared" ca="1" si="17"/>
         <v>#NAME?</v>
       </c>
       <c r="AB6" s="1">
-        <f>IF(AB5 &gt;( $B$8 + $B$18*$B$2), AB5 -( $B$18*$B$2), $B$8)</f>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
       <c r="AC6" s="1">
-        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
-        <v>98066.5</v>
+        <f t="shared" si="26"/>
+        <v>0</v>
       </c>
       <c r="AD6" s="1">
-        <f ca="1" xml:space="preserve"> AC6*COS(M6)</f>
-        <v>86575.800601626222</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="AE6" s="1">
-        <f ca="1" xml:space="preserve"> AC6*SIN(M6)</f>
-        <v>46061.580220802854</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
+        <f t="shared" si="19"/>
+        <v>101094.3784110229</v>
+      </c>
+      <c r="AG6" s="1">
+        <f t="shared" ca="1" si="19"/>
+        <v>100850.00004266192</v>
       </c>
       <c r="AJ6"/>
       <c r="AK6"/>
@@ -2002,120 +2086,128 @@
         <f xml:space="preserve"> B6 *(PI()/180)</f>
         <v>0.87266462599716477</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>5</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>0.6</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="22"/>
         <v>86.602540378443877</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="12"/>
-        <v>45.094794360957437</v>
+        <f t="shared" si="23"/>
+        <v>45.094662867899302</v>
       </c>
       <c r="H7" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>97.639790143002145</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" ca="1" si="24"/>
+        <v>43.301270189221938</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="25"/>
+        <v>23.773664234532212</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" ca="1" si="27"/>
+        <v>49.401992997293533</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="7"/>
+        <v>-9.8106308506654347</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.48007668300506151</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>27.506367778829919</v>
+      </c>
+      <c r="O7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>97.639850872771405</v>
-      </c>
-      <c r="I7" s="3">
-        <f t="shared" ca="1" si="13"/>
-        <v>43.301270189221938</v>
-      </c>
-      <c r="J7" s="3">
-        <f t="shared" si="14"/>
-        <v>23.773684091402515</v>
-      </c>
-      <c r="K7" s="3">
-        <f t="shared" ca="1" si="16"/>
-        <v>49.402002349673879</v>
-      </c>
-      <c r="L7" s="3">
-        <f t="shared" si="15"/>
-        <v>-9.8099866763874495</v>
-      </c>
-      <c r="M7" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.48007787748679526</v>
-      </c>
-      <c r="N7" s="3">
+        <v>476676.43095847499</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" si="1"/>
+        <v>-23323.464377266318</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" ca="1" si="10"/>
+        <v>499999.89533574128</v>
+      </c>
+      <c r="R7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>27.506436217591968</v>
-      </c>
-      <c r="O7" s="1">
-        <f ca="1">(0.5)*($B$8)*(H7^2)</f>
-        <v>476677.02392285189</v>
-      </c>
-      <c r="P7" s="1">
-        <f>($B$8)*L7*J7</f>
-        <v>-23321.952418530294</v>
-      </c>
-      <c r="Q7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>499998.97634138219</v>
-      </c>
-      <c r="R7" s="1">
-        <f ca="1" xml:space="preserve"> ($B$8)*H7</f>
-        <v>9763.9850872771403</v>
+        <v>9763.9790143002137</v>
       </c>
       <c r="S7" s="3">
-        <f t="shared" si="4"/>
-        <v>340.20334190616853</v>
+        <f t="shared" si="11"/>
+        <v>340.20334198690182</v>
       </c>
       <c r="T7" s="13">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.28700438486492424</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.28700420628660778</v>
       </c>
       <c r="U7" s="13">
-        <f t="shared" si="6"/>
-        <v>1.2014494811908036</v>
+        <f t="shared" si="13"/>
+        <v>1.2014494834239837</v>
       </c>
       <c r="V7" s="5" t="e">
         <f>IF(Mach&lt;cross, subsonic, IF(Mach&lt;cross, transonic, supersonic))</f>
         <v>#NAME?</v>
       </c>
       <c r="W7" s="3" t="e">
-        <f ca="1">(0.5)*(U7)*(H7)*(V7)*($B$17)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="X7" s="3" t="e">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="14"/>
         <v>#NAME?</v>
       </c>
       <c r="Y7" s="3" t="e">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#NAME?</v>
       </c>
       <c r="Z7" s="3" t="e">
-        <f ca="1" xml:space="preserve"> X7/($B$8)</f>
+        <f t="shared" ca="1" si="16"/>
         <v>#NAME?</v>
       </c>
       <c r="AA7" s="3" t="e">
-        <f ca="1" xml:space="preserve"> Y7/($B$8)</f>
+        <f t="shared" ca="1" si="17"/>
         <v>#NAME?</v>
       </c>
       <c r="AB7" s="1">
-        <f>IF(AB6 &gt;( $B$8 + $B$18*$B$2), AB6 -( $B$18*$B$2), $B$8)</f>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
       <c r="AC7" s="1">
-        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
-        <v>98066.5</v>
+        <f t="shared" si="26"/>
+        <v>0</v>
       </c>
       <c r="AD7" s="1">
-        <f ca="1" xml:space="preserve"> AC7*COS(M7)</f>
-        <v>86980.960643714323</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="AE7" s="1">
-        <f ca="1" xml:space="preserve"> AC7*SIN(M7)</f>
-        <v>45291.841514191263</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="1">
+        <f t="shared" si="19"/>
+        <v>101039.72914970007</v>
+      </c>
+      <c r="AG7" s="1">
+        <f t="shared" ca="1" si="19"/>
+        <v>100732.93213068502</v>
       </c>
       <c r="AJ7"/>
       <c r="AK7"/>
@@ -2127,120 +2219,128 @@
       <c r="B8" s="24">
         <v>100</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>6</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>0.7</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="22"/>
         <v>86.602540378443877</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="12"/>
-        <v>44.113795693318693</v>
+        <f t="shared" si="23"/>
+        <v>44.113599782832758</v>
       </c>
       <c r="H8" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>97.190584347455925</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" ca="1" si="24"/>
+        <v>51.961524227066327</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="25"/>
+        <v>28.234077367068817</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" ca="1" si="27"/>
+        <v>59.14341411091474</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="7"/>
+        <v>-9.8106170859757249</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.47112339947154724</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>26.993382419575575</v>
+      </c>
+      <c r="O8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>97.190673268950377</v>
-      </c>
-      <c r="I8" s="3">
-        <f t="shared" ca="1" si="13"/>
-        <v>51.961524227066327</v>
-      </c>
-      <c r="J8" s="3">
-        <f t="shared" si="14"/>
-        <v>28.234113594116323</v>
-      </c>
-      <c r="K8" s="3">
-        <f t="shared" ca="1" si="16"/>
-        <v>59.143430958901575</v>
-      </c>
-      <c r="L8" s="3">
-        <f t="shared" si="15"/>
-        <v>-9.8098520513066774</v>
-      </c>
-      <c r="M8" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.47112519560883803</v>
-      </c>
-      <c r="N8" s="3">
+        <v>472300.48428999726</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="1"/>
+        <v>-27699.372182412586</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" ca="1" si="10"/>
+        <v>499999.85647240985</v>
+      </c>
+      <c r="R8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>26.993485330661763</v>
-      </c>
-      <c r="O8" s="1">
-        <f ca="1">(0.5)*($B$8)*(H8^2)</f>
-        <v>472301.34852359322</v>
-      </c>
-      <c r="P8" s="1">
-        <f>($B$8)*L8*J8</f>
-        <v>-27697.247715806774</v>
-      </c>
-      <c r="Q8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>499998.59623939998</v>
-      </c>
-      <c r="R8" s="1">
-        <f ca="1" xml:space="preserve"> ($B$8)*H8</f>
-        <v>9719.0673268950377</v>
+        <v>9719.0584347455933</v>
       </c>
       <c r="S8" s="3">
-        <f t="shared" si="4"/>
-        <v>340.18520687031361</v>
+        <f t="shared" si="11"/>
+        <v>340.18520701760406</v>
       </c>
       <c r="T8" s="13">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.28569929352043133</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.28569903200531133</v>
       </c>
       <c r="U8" s="13">
-        <f t="shared" si="6"/>
-        <v>1.2009479243857608</v>
+        <f t="shared" si="13"/>
+        <v>1.2009479284586908</v>
       </c>
       <c r="V8" s="5" t="e">
         <f>IF(Mach&lt;cross, subsonic, IF(Mach&lt;cross, transonic, supersonic))</f>
         <v>#NAME?</v>
       </c>
       <c r="W8" s="3" t="e">
-        <f ca="1">(0.5)*(U8)*(H8)*(V8)*($B$17)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="X8" s="3" t="e">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="14"/>
         <v>#NAME?</v>
       </c>
       <c r="Y8" s="3" t="e">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#NAME?</v>
       </c>
       <c r="Z8" s="3" t="e">
-        <f ca="1" xml:space="preserve"> X8/($B$8)</f>
+        <f t="shared" ca="1" si="16"/>
         <v>#NAME?</v>
       </c>
       <c r="AA8" s="3" t="e">
-        <f ca="1" xml:space="preserve"> Y8/($B$8)</f>
+        <f t="shared" ca="1" si="17"/>
         <v>#NAME?</v>
       </c>
       <c r="AB8" s="1">
-        <f>IF(AB7 &gt;( $B$8 + $B$18*$B$2), AB7 -( $B$18*$B$2), $B$8)</f>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
       <c r="AC8" s="1">
-        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
-        <v>98066.5</v>
+        <f t="shared" si="26"/>
+        <v>0</v>
       </c>
       <c r="AD8" s="1">
-        <f ca="1" xml:space="preserve"> AC8*COS(M8)</f>
-        <v>87382.952914843889</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="AE8" s="1">
-        <f ca="1" xml:space="preserve"> AC8*SIN(M8)</f>
-        <v>44511.323976401523</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1">
+        <f t="shared" si="19"/>
+        <v>100986.27918194859</v>
+      </c>
+      <c r="AG8" s="1">
+        <f t="shared" ca="1" si="19"/>
+        <v>100616.51550850805</v>
       </c>
       <c r="AJ8"/>
       <c r="AK8"/>
@@ -2252,120 +2352,128 @@
       <c r="B9" s="24">
         <v>100</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>7</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>0.79999999999999993</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="22"/>
         <v>86.602540378443877</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="12"/>
-        <v>43.132810488188028</v>
+        <f t="shared" si="23"/>
+        <v>43.132538074235185</v>
       </c>
       <c r="H9" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>96.749242067963252</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" ca="1" si="24"/>
+        <v>60.621778264910716</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="25"/>
+        <v>32.596384259922218</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" ca="1" si="27"/>
+        <v>68.840306470193369</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="7"/>
+        <v>-9.8106036240627681</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.46208771406398158</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>26.47567578071412</v>
+      </c>
+      <c r="O9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>96.749363515270446</v>
-      </c>
-      <c r="I9" s="3">
-        <f t="shared" ca="1" si="13"/>
-        <v>60.621778264910716</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="14"/>
-        <v>32.596443903191663</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" ca="1" si="16"/>
-        <v>68.840333852376247</v>
-      </c>
-      <c r="L9" s="3">
-        <f t="shared" si="15"/>
-        <v>-9.8097203870645089</v>
-      </c>
-      <c r="M9" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.46209023443392433</v>
-      </c>
-      <c r="N9" s="3">
+        <v>468020.79203626752</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" si="1"/>
+        <v>-31979.020555173549</v>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" ca="1" si="10"/>
+        <v>499999.81259144109</v>
+      </c>
+      <c r="R9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>26.47582018727465</v>
-      </c>
-      <c r="O9" s="1">
-        <f ca="1">(0.5)*($B$8)*(H9^2)</f>
-        <v>468021.96703049721</v>
-      </c>
-      <c r="P9" s="1">
-        <f>($B$8)*L9*J9</f>
-        <v>-31976.200030294389</v>
-      </c>
-      <c r="Q9" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>499998.16706079157</v>
-      </c>
-      <c r="R9" s="1">
-        <f ca="1" xml:space="preserve"> ($B$8)*H9</f>
-        <v>9674.9363515270452</v>
+        <v>9674.924206796326</v>
       </c>
       <c r="S9" s="3">
-        <f t="shared" si="4"/>
-        <v>340.16747068223617</v>
+        <f t="shared" si="11"/>
+        <v>340.16747092473139</v>
       </c>
       <c r="T9" s="13">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.28441685891137969</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.28441650168652044</v>
       </c>
       <c r="U9" s="13">
-        <f t="shared" si="6"/>
-        <v>1.2004575535511621</v>
+        <f t="shared" si="13"/>
+        <v>1.200457560254631</v>
       </c>
       <c r="V9" s="5" t="e">
         <f>IF(Mach&lt;cross, subsonic, IF(Mach&lt;cross, transonic, supersonic))</f>
         <v>#NAME?</v>
       </c>
       <c r="W9" s="3" t="e">
-        <f ca="1">(0.5)*(U9)*(H9)*(V9)*($B$17)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="X9" s="3" t="e">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="14"/>
         <v>#NAME?</v>
       </c>
       <c r="Y9" s="3" t="e">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#NAME?</v>
       </c>
       <c r="Z9" s="3" t="e">
-        <f ca="1" xml:space="preserve"> X9/($B$8)</f>
+        <f t="shared" ca="1" si="16"/>
         <v>#NAME?</v>
       </c>
       <c r="AA9" s="3" t="e">
-        <f ca="1" xml:space="preserve"> Y9/($B$8)</f>
+        <f t="shared" ca="1" si="17"/>
         <v>#NAME?</v>
       </c>
       <c r="AB9" s="1">
-        <f>IF(AB8 &gt;( $B$8 + $B$18*$B$2), AB8 -( $B$18*$B$2), $B$8)</f>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
       <c r="AC9" s="1">
-        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
-        <v>98066.5</v>
+        <f t="shared" si="26"/>
+        <v>0</v>
       </c>
       <c r="AD9" s="1">
-        <f ca="1" xml:space="preserve"> AC9*COS(M9)</f>
-        <v>87781.53899361004</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="AE9" s="1">
-        <f ca="1" xml:space="preserve"> AC9*SIN(M9)</f>
-        <v>43720.016401681729</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF9" s="1">
+        <f t="shared" si="19"/>
+        <v>100934.02698744865</v>
+      </c>
+      <c r="AG9" s="1">
+        <f t="shared" ca="1" si="19"/>
+        <v>100500.7392571487</v>
       </c>
       <c r="AJ9"/>
       <c r="AK9"/>
@@ -2377,120 +2485,128 @@
       <c r="B10" s="16">
         <v>6378137</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>8</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="22"/>
         <v>86.602540378443877</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="12"/>
-        <v>42.151838449481573</v>
+        <f t="shared" si="23"/>
+        <v>42.15147771182891</v>
       </c>
       <c r="H10" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>96.315871346786935</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" ca="1" si="24"/>
+        <v>69.282032302755098</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="25"/>
+        <v>36.860585049225428</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" ca="1" si="27"/>
+        <v>78.493461828494304</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" si="7"/>
+        <v>-9.810590464924541</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.45296997941190875</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>25.953268066430162</v>
+      </c>
+      <c r="O10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>96.316029219809479</v>
-      </c>
-      <c r="I10" s="3">
-        <f t="shared" ca="1" si="13"/>
-        <v>69.282032302755098</v>
-      </c>
-      <c r="J10" s="3">
-        <f t="shared" si="14"/>
-        <v>36.860676350075138</v>
-      </c>
-      <c r="K10" s="3">
-        <f t="shared" ca="1" si="16"/>
-        <v>78.493503195190755</v>
-      </c>
-      <c r="L10" s="3">
-        <f t="shared" si="15"/>
-        <v>-9.8095916836207593</v>
-      </c>
-      <c r="M10" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.45297334705206066</v>
-      </c>
-      <c r="N10" s="3">
+        <v>463837.35366454069</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" si="1"/>
+        <v>-36162.410421547109</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" ca="1" si="10"/>
+        <v>499999.76408608782</v>
+      </c>
+      <c r="R10" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>25.953461017997785</v>
-      </c>
-      <c r="O10" s="1">
-        <f ca="1">(0.5)*($B$8)*(H10^2)</f>
-        <v>463838.87423355965</v>
-      </c>
-      <c r="P10" s="1">
-        <f>($B$8)*L10*J10</f>
-        <v>-36158.818417633353</v>
-      </c>
-      <c r="Q10" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>499997.69265119301</v>
-      </c>
-      <c r="R10" s="1">
-        <f ca="1" xml:space="preserve"> ($B$8)*H10</f>
-        <v>9631.6029219809479</v>
+        <v>9631.5871346786935</v>
       </c>
       <c r="S10" s="3">
-        <f t="shared" si="4"/>
-        <v>340.15013333652291</v>
+        <f t="shared" si="11"/>
+        <v>340.15013370773028</v>
       </c>
       <c r="T10" s="13">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.28315740545225809</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.28315694101577255</v>
       </c>
       <c r="U10" s="13">
-        <f t="shared" si="6"/>
-        <v>1.1999783581565004</v>
+        <f t="shared" si="13"/>
+        <v>1.1999783684149139</v>
       </c>
       <c r="V10" s="5" t="e">
         <f>IF(Mach&lt;cross, subsonic, IF(Mach&lt;cross, transonic, supersonic))</f>
         <v>#NAME?</v>
       </c>
       <c r="W10" s="3" t="e">
-        <f ca="1">(0.5)*(U10)*(H10)*(V10)*($B$17)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="X10" s="3" t="e">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="14"/>
         <v>#NAME?</v>
       </c>
       <c r="Y10" s="3" t="e">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#NAME?</v>
       </c>
       <c r="Z10" s="3" t="e">
-        <f ca="1" xml:space="preserve"> X10/($B$8)</f>
+        <f t="shared" ca="1" si="16"/>
         <v>#NAME?</v>
       </c>
       <c r="AA10" s="3" t="e">
-        <f ca="1" xml:space="preserve"> Y10/($B$8)</f>
+        <f t="shared" ca="1" si="17"/>
         <v>#NAME?</v>
       </c>
       <c r="AB10" s="1">
-        <f>IF(AB9 &gt;( $B$8 + $B$18*$B$2), AB9 -( $B$18*$B$2), $B$8)</f>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
       <c r="AC10" s="1">
-        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
-        <v>98066.5</v>
+        <f t="shared" si="26"/>
+        <v>0</v>
       </c>
       <c r="AD10" s="1">
-        <f ca="1" xml:space="preserve"> AC10*COS(M10)</f>
-        <v>88176.475866136883</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="AE10" s="1">
         <f ca="1" xml:space="preserve"> AC10*SIN(M10)</f>
-        <v>42917.916143244649</v>
+        <v>0</v>
+      </c>
+      <c r="AF10" s="1">
+        <f t="shared" si="19"/>
+        <v>100882.97108012233</v>
+      </c>
+      <c r="AG10" s="1">
+        <f t="shared" ca="1" si="19"/>
+        <v>100385.59237270131</v>
       </c>
       <c r="AJ10"/>
       <c r="AK10"/>
@@ -2502,120 +2618,128 @@
       <c r="B11" s="16">
         <v>6356752.2999999998</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>9</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="22"/>
         <v>86.602540378443877</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="12"/>
-        <v>41.170879281119497</v>
+        <f t="shared" si="23"/>
+        <v>41.170418665336456</v>
       </c>
       <c r="H11" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>95.890580210357925</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" ca="1" si="24"/>
+        <v>77.94228634059948</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="25"/>
+        <v>41.026679868083697</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" ca="1" si="27"/>
+        <v>88.103682743734367</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="7"/>
+        <v>-9.8105776085590577</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.44377060913325062</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>25.426182975284963</v>
+      </c>
+      <c r="O11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>95.890777975676656</v>
-      </c>
-      <c r="I11" s="3">
-        <f t="shared" ca="1" si="13"/>
-        <v>77.94228634059948</v>
-      </c>
-      <c r="J11" s="3">
-        <f t="shared" si="14"/>
-        <v>41.026812236605195</v>
-      </c>
-      <c r="K11" s="3">
-        <f t="shared" ca="1" si="16"/>
-        <v>88.103741913611515</v>
-      </c>
-      <c r="L11" s="3">
-        <f t="shared" si="15"/>
-        <v>-9.8094659409361373</v>
-      </c>
-      <c r="M11" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.44377494740405499</v>
-      </c>
-      <c r="N11" s="3">
+        <v>459750.16865395434</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="1"/>
+        <v>-40249.542686734261</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" ca="1" si="10"/>
+        <v>499999.71134068863</v>
+      </c>
+      <c r="R11" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>25.426431539892437</v>
-      </c>
-      <c r="O11" s="1">
-        <f ca="1">(0.5)*($B$8)*(H11^2)</f>
-        <v>459752.06503902574</v>
-      </c>
-      <c r="P11" s="1">
-        <f>($B$8)*L11*J11</f>
-        <v>-40245.111730016062</v>
-      </c>
-      <c r="Q11" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>499997.17676904181</v>
-      </c>
-      <c r="R11" s="1">
-        <f ca="1" xml:space="preserve"> ($B$8)*H11</f>
-        <v>9589.0777975676647</v>
+        <v>9589.058021035793</v>
       </c>
       <c r="S11" s="3">
-        <f t="shared" si="4"/>
-        <v>340.13319482788091</v>
+        <f t="shared" si="11"/>
+        <v>340.13319536605957</v>
       </c>
       <c r="T11" s="13">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.28192125741858476</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.28192067553758804</v>
       </c>
       <c r="U11" s="13">
-        <f t="shared" si="6"/>
-        <v>1.1995103279118349</v>
+        <f t="shared" si="13"/>
+        <v>1.1995103427801008</v>
       </c>
       <c r="V11" s="5" t="e">
         <f>IF(Mach&lt;cross, subsonic, IF(Mach&lt;cross, transonic, supersonic))</f>
         <v>#NAME?</v>
       </c>
       <c r="W11" s="3" t="e">
-        <f ca="1">(0.5)*(U11)*(H11)*(V11)*($B$17)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="X11" s="3" t="e">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="14"/>
         <v>#NAME?</v>
       </c>
       <c r="Y11" s="3" t="e">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#NAME?</v>
       </c>
       <c r="Z11" s="3" t="e">
-        <f ca="1" xml:space="preserve"> X11/($B$8)</f>
+        <f t="shared" ca="1" si="16"/>
         <v>#NAME?</v>
       </c>
       <c r="AA11" s="3" t="e">
-        <f ca="1" xml:space="preserve"> Y11/($B$8)</f>
+        <f t="shared" ca="1" si="17"/>
         <v>#NAME?</v>
       </c>
       <c r="AB11" s="1">
-        <f>IF(AB10 &gt;( $B$8 + $B$18*$B$2), AB10 -( $B$18*$B$2), $B$8)</f>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
       <c r="AC11" s="1">
-        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
-        <v>98066.5</v>
+        <f t="shared" si="26"/>
+        <v>0</v>
       </c>
       <c r="AD11" s="1">
-        <f ca="1" xml:space="preserve"> AC11*COS(M11)</f>
-        <v>88567.516139841144</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="AE11" s="1">
-        <f ca="1" xml:space="preserve"> AC11*SIN(M11)</f>
-        <v>42105.029474743023</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF11" s="1">
+        <f t="shared" si="19"/>
+        <v>100833.11000807921</v>
+      </c>
+      <c r="AG11" s="1">
+        <f t="shared" ca="1" si="19"/>
+        <v>100271.06376641487</v>
       </c>
       <c r="AJ11"/>
       <c r="AK11"/>
@@ -2627,120 +2751,128 @@
       <c r="B12" s="16">
         <v>6365755.0999999996</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>1.0999999999999999</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="22"/>
         <v>86.602540378443877</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="12"/>
-        <v>40.18993268702588</v>
+        <f t="shared" si="23"/>
+        <v>40.189360904480552</v>
       </c>
       <c r="H12" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>95.47347657810829</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" ca="1" si="24"/>
+        <v>86.602540378443862</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="25"/>
+        <v>45.09466884657455</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" ca="1" si="27"/>
+        <v>97.67178257228565</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="7"/>
+        <v>-9.8105650549643819</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.43449007954170649</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>24.894447798043217</v>
+      </c>
+      <c r="O12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>95.473717270187365</v>
-      </c>
-      <c r="I12" s="3">
-        <f t="shared" ca="1" si="13"/>
-        <v>86.602540378443862</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="14"/>
-        <v>45.094852835012468</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" ca="1" si="16"/>
-        <v>97.671863689084987</v>
-      </c>
-      <c r="L12" s="3">
-        <f t="shared" si="15"/>
-        <v>-9.8093431589722435</v>
-      </c>
-      <c r="M12" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.43449551198192587</v>
-      </c>
-      <c r="N12" s="3">
+        <v>455759.23649552959</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" si="1"/>
+        <v>-44240.418235139521</v>
+      </c>
+      <c r="Q12" s="1">
+        <f t="shared" ca="1" si="10"/>
+        <v>499999.65473066911</v>
+      </c>
+      <c r="R12" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>24.894759053940245</v>
-      </c>
-      <c r="O12" s="1">
-        <f ca="1">(0.5)*($B$8)*(H12^2)</f>
-        <v>455761.53446938371</v>
-      </c>
-      <c r="P12" s="1">
-        <f>($B$8)*L12*J12</f>
-        <v>-44235.088616198962</v>
-      </c>
-      <c r="Q12" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>499996.62308558269</v>
-      </c>
-      <c r="R12" s="1">
-        <f ca="1" xml:space="preserve"> ($B$8)*H12</f>
-        <v>9547.3717270187371</v>
+        <v>9547.3476578108293</v>
       </c>
       <c r="S12" s="3">
-        <f t="shared" si="4"/>
-        <v>340.11665515113754</v>
+        <f t="shared" si="11"/>
+        <v>340.11665589919033</v>
       </c>
       <c r="T12" s="13">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.2807087386760338</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.28070803038357045</v>
       </c>
       <c r="U12" s="13">
-        <f t="shared" si="6"/>
-        <v>1.1990534527675287</v>
+        <f t="shared" si="13"/>
+        <v>1.1990534734279625</v>
       </c>
       <c r="V12" s="5" t="e">
         <f>IF(Mach&lt;cross, subsonic, IF(Mach&lt;cross, transonic, supersonic))</f>
         <v>#NAME?</v>
       </c>
       <c r="W12" s="3" t="e">
-        <f ca="1">(0.5)*(U12)*(H12)*(V12)*($B$17)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="X12" s="3" t="e">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="14"/>
         <v>#NAME?</v>
       </c>
       <c r="Y12" s="3" t="e">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#NAME?</v>
       </c>
       <c r="Z12" s="3" t="e">
-        <f ca="1" xml:space="preserve"> X12/($B$8)</f>
+        <f t="shared" ca="1" si="16"/>
         <v>#NAME?</v>
       </c>
       <c r="AA12" s="3" t="e">
-        <f ca="1" xml:space="preserve"> Y12/($B$8)</f>
+        <f t="shared" ca="1" si="17"/>
         <v>#NAME?</v>
       </c>
       <c r="AB12" s="1">
-        <f>IF(AB11 &gt;( $B$8 + $B$18*$B$2), AB11 -( $B$18*$B$2), $B$8)</f>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
       <c r="AC12" s="1">
-        <f xml:space="preserve"> $B$19*$B$13*$B$18</f>
-        <v>98066.5</v>
+        <f t="shared" si="26"/>
+        <v>0</v>
       </c>
       <c r="AD12" s="1">
-        <f ca="1" xml:space="preserve"> AC12*COS(M12)</f>
-        <v>88954.408279592899</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="AE12" s="1">
-        <f ca="1" xml:space="preserve"> AC12*SIN(M12)</f>
-        <v>41281.371947616935</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF12" s="1">
+        <f>IF(J12&gt;38000,0,(101325*(1-(2.25577*10^(-5))*J12)^5.25588))</f>
+        <v>100784.44235356437</v>
+      </c>
+      <c r="AG12" s="1">
+        <f ca="1">IF(K12&gt;38000,0,(101325*(1-(2.25577*10^(-5))*K12)^5.25588))</f>
+        <v>100157.14226487692</v>
       </c>
       <c r="AJ12"/>
       <c r="AK12"/>
@@ -2749,10 +2881,10 @@
       <c r="A13" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="27">
         <v>9.8066499999999994</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="29" t="s">
         <v>44</v>
       </c>
       <c r="Q13" s="1"/>
@@ -2785,7 +2917,7 @@
       <c r="B16" s="24">
         <v>0.5</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="29" t="s">
         <v>5</v>
       </c>
       <c r="Q16" s="1"/>
@@ -2803,7 +2935,7 @@
         <f xml:space="preserve"> PI()*((B16/2)^2)</f>
         <v>0.19634954084936207</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="29" t="s">
         <v>45</v>
       </c>
       <c r="Q17" s="1"/>
@@ -2820,7 +2952,7 @@
       <c r="B18" s="24">
         <v>100</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="29" t="s">
         <v>46</v>
       </c>
       <c r="Q18" s="1"/>
@@ -2837,7 +2969,7 @@
       <c r="B19" s="24">
         <v>100</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="31" t="s">
         <v>1</v>
       </c>
       <c r="Q19" s="1"/>
@@ -2848,14 +2980,14 @@
       <c r="AK19"/>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="26">
         <f xml:space="preserve"> B19*B13*B18</f>
         <v>98066.5</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="31" t="s">
         <v>49</v>
       </c>
       <c r="Q20" s="1"/>
@@ -2866,6 +2998,15 @@
       <c r="AK20"/>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="24">
+        <v>100</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>5</v>
+      </c>
       <c r="Q21" s="1"/>
       <c r="S21" s="3"/>
       <c r="T21" s="13"/>

</xml_diff>

<commit_message>
Updated gravity model with mass of earth, grav constant, and r^2
</commit_message>
<xml_diff>
--- a/Aero210/dynamics_template.xlsx
+++ b/Aero210/dynamics_template.xlsx
@@ -60,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1172,8 +1172,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="104">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -1974,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP2691"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2001,11 +2001,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" s="40" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
       <c r="D1" s="32" t="s">
         <v>10</v>
       </c>
@@ -2016,10 +2016,10 @@
         <v>15</v>
       </c>
       <c r="G1" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>66</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>16</v>
       </c>
       <c r="I1" s="34" t="s">
         <v>67</v>
@@ -2144,27 +2144,27 @@
       <c r="F2" s="12">
         <v>0</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="12">
+        <v>0</v>
+      </c>
+      <c r="H2" s="13">
         <f xml:space="preserve"> (F2/1000)</f>
         <v>0</v>
       </c>
-      <c r="H2" s="12">
+      <c r="I2" s="13">
+        <f>G2/1000</f>
         <v>0</v>
       </c>
-      <c r="I2" s="13">
-        <f>H2/1000</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="43">
+      <c r="J2" s="42">
         <f xml:space="preserve"> 0</f>
         <v>0</v>
       </c>
       <c r="K2" s="41">
-        <f>SQRT((F2)^2 + (H2+$B$23)^2)</f>
+        <f>SQRT((F2)^2 + (G2+$B$23)^2)</f>
         <v>6378137</v>
       </c>
       <c r="L2" s="14">
-        <f>SQRT(F2^2 + H2^2)</f>
+        <f>SQRT(F2^2 + G2^2)</f>
         <v>0</v>
       </c>
       <c r="M2" s="15">
@@ -2200,7 +2200,7 @@
         <v>9.7803269999999998</v>
       </c>
       <c r="U2" s="15">
-        <f xml:space="preserve"> ATAN2($B$23+H2, F2)</f>
+        <f xml:space="preserve"> ATAN2($B$23+G2, F2)</f>
         <v>0</v>
       </c>
       <c r="V2" s="15">
@@ -2212,7 +2212,7 @@
         <v>200</v>
       </c>
       <c r="X2" s="16">
-        <f t="shared" ref="X2:X12" si="2" xml:space="preserve"> IF(H2&lt;30000, O2/AM2, "")</f>
+        <f xml:space="preserve"> IF(G2&lt;30000, O2/AM2, "")</f>
         <v>0</v>
       </c>
       <c r="Y2" s="15">
@@ -2220,35 +2220,35 @@
         <v>0.35</v>
       </c>
       <c r="Z2" s="15">
-        <f t="shared" ref="Z2:Z12" si="3">(0.5)*(AN2)*(O2^2)*(Y2)*($B$13)</f>
+        <f t="shared" ref="Z2:Z12" si="2">(0.5)*(AN2)*(O2^2)*(Y2)*($B$13)</f>
         <v>0</v>
       </c>
       <c r="AA2" s="15">
-        <f t="shared" ref="AA2:AA12" si="4" xml:space="preserve"> - Z2*COS(P2)</f>
+        <f t="shared" ref="AA2:AA12" si="3" xml:space="preserve"> - Z2*COS(P2)</f>
         <v>0</v>
       </c>
       <c r="AB2" s="15">
-        <f t="shared" ref="AB2:AB12" si="5" xml:space="preserve"> - Z2*SIN(P2)</f>
+        <f t="shared" ref="AB2:AB12" si="4" xml:space="preserve"> - Z2*SIN(P2)</f>
         <v>0</v>
       </c>
       <c r="AC2" s="10">
-        <f t="shared" ref="AC2:AC12" si="6">IF(E2 &gt;= $B$16, IF(E2 &lt; $B$17, B15, 0), 0)</f>
+        <f>IF(E2 &gt;= $B$16, IF(E2 &lt; $B$17, B15, 0), 0)</f>
         <v>0</v>
       </c>
       <c r="AD2" s="10">
-        <f t="shared" ref="AD2:AD12" si="7" xml:space="preserve"> AC2*COS(P2)</f>
+        <f t="shared" ref="AD2:AD12" si="5" xml:space="preserve"> AC2*COS(P2)</f>
         <v>0</v>
       </c>
       <c r="AE2" s="10">
-        <f t="shared" ref="AE2:AE12" si="8" xml:space="preserve"> AC2*SIN(P2)</f>
+        <f t="shared" ref="AE2:AE12" si="6" xml:space="preserve"> AC2*SIN(P2)</f>
         <v>0</v>
       </c>
       <c r="AF2" s="10">
-        <f t="shared" ref="AF2:AF12" si="9">(0.5)*($B$9)*(O2^2)</f>
+        <f t="shared" ref="AF2:AF12" si="7">(0.5)*($B$9)*(O2^2)</f>
         <v>0</v>
       </c>
       <c r="AG2" s="10">
-        <f t="shared" ref="AG2:AG12" si="10">($B$9)*AJ2*H2</f>
+        <f>($B$9)*AJ2*G2</f>
         <v>0</v>
       </c>
       <c r="AH2" s="10">
@@ -2256,11 +2256,11 @@
         <v>0</v>
       </c>
       <c r="AI2" s="10">
-        <f t="shared" ref="AI2:AI12" si="11" xml:space="preserve"> ($B$9)*O2</f>
+        <f t="shared" ref="AI2:AI12" si="8" xml:space="preserve"> ($B$9)*O2</f>
         <v>0</v>
       </c>
       <c r="AJ2" s="15">
-        <f t="shared" ref="AJ2:AJ12" si="12">IF(H2&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*H2)+((6.26*10^(-13))*(H2)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
+        <f>IF(G2&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G2)+((6.26*10^(-13))*(G2)^2))), ($B$25)*($B$20)*(K2)^(-2))</f>
         <v>-9.7803269999999998</v>
       </c>
       <c r="AK2" s="15">
@@ -2272,7 +2272,7 @@
         <v>-9.7803269999999998</v>
       </c>
       <c r="AM2" s="15">
-        <f t="shared" ref="AM2:AM12" si="13">IF(H2&lt;100000, IF(H2&gt;10000, (343.2)+(-4.313943*H2)+(-0.291943*H2^2)+(0.053721*H2^3)+((-3.039687*10^(-3))*H2^4)+((9.262166*10^(-5))*H2^5)+((-1.647967*10^(-6))*H2^6)+((1.694814*10^(-8))*H2^7)+((-9.299892*10^(-11))*H2^8)+((2.104694*10^(-13))*H2^9), ((-0.00406576*H2)+340.3)), "")</f>
+        <f>IF(G2&lt;100000, IF(G2&gt;10000, (343.2)+(-4.313943*G2)+(-0.291943*G2^2)+(0.053721*G2^3)+((-3.039687*10^(-3))*G2^4)+((9.262166*10^(-5))*G2^5)+((-1.647967*10^(-6))*G2^6)+((1.694814*10^(-8))*G2^7)+((-9.299892*10^(-11))*G2^8)+((2.104694*10^(-13))*G2^9), ((-0.00406576*G2)+340.3)), 0)</f>
         <v>340.3</v>
       </c>
       <c r="AN2" s="16">
@@ -2280,11 +2280,11 @@
         <v>1.2004891883138833</v>
       </c>
       <c r="AO2" s="10">
-        <f t="shared" ref="AO2:AO12" si="14">IF(H2&gt;38000,0,(101325*(1-(2.25577*10^(-5))*H2)^5.25588))</f>
+        <f>IF(G2&gt;38000,0,(101325*(1-(2.25577*10^(-5))*G2)^5.25588))</f>
         <v>101325</v>
       </c>
       <c r="AP2" s="15">
-        <f t="shared" ref="AP2:AP12" si="15">1.6667*AM2-273.15</f>
+        <f t="shared" ref="AP2:AP12" si="9">1.6667*AM2-273.15</f>
         <v>294.02801000000011</v>
       </c>
     </row>
@@ -2307,31 +2307,31 @@
         <v>0.1</v>
       </c>
       <c r="F3" s="15">
-        <f t="shared" ref="F3:F12" si="16">F2 + M2*($B$2) + (0.5)*(R2)*($B$2)^2</f>
+        <f>F2 + M2*($B$2) + (0.5)*(R2)*($B$2)^2</f>
         <v>0</v>
       </c>
-      <c r="G3" s="13">
-        <f t="shared" ref="G3:G12" si="17" xml:space="preserve"> (F3/1000)</f>
+      <c r="G3" s="18">
+        <f xml:space="preserve"> G2 + N2*($B$2) + (0.5)*(S2)*($B$2)^2</f>
+        <v>-4.8901635000000006E-2</v>
+      </c>
+      <c r="H3" s="13">
+        <f xml:space="preserve"> (F3/1000)</f>
         <v>0</v>
       </c>
-      <c r="H3" s="18">
-        <f t="shared" ref="H3:H12" si="18" xml:space="preserve"> H2 + N2*($B$2) + (0.5)*(S2)*($B$2)^2</f>
-        <v>-4.8901635000000006E-2</v>
-      </c>
       <c r="I3" s="13">
-        <f t="shared" ref="I3:I12" si="19">H3/1000</f>
+        <f>G3/1000</f>
         <v>-4.8901635000000009E-5</v>
       </c>
       <c r="J3" s="15">
-        <f t="shared" ref="J3:J12" si="20">J2 + SQRT( (F3-F2)^2 + (H3-H2)^2 )</f>
+        <f>J2 + SQRT( (F3-F2)^2 + (G3-G2)^2 )</f>
         <v>4.8901635000000006E-2</v>
       </c>
       <c r="K3" s="41">
-        <f t="shared" ref="K3:K12" si="21">SQRT((F3)^2 + (H3+$B$23)^2)</f>
+        <f>SQRT((F3)^2 + (G3+$B$23)^2)</f>
         <v>6378136.9510983648</v>
       </c>
       <c r="L3" s="14">
-        <f t="shared" ref="L3:L12" si="22">SQRT(F3^2 + H3^2)</f>
+        <f>SQRT(F3^2 + G3^2)</f>
         <v>4.8901635000000006E-2</v>
       </c>
       <c r="M3" s="15">
@@ -2343,7 +2343,7 @@
         <v>-0.97803269999999998</v>
       </c>
       <c r="O3" s="15">
-        <f t="shared" ref="O3:O12" si="23">SQRT(M3^2 + N3^2)</f>
+        <f t="shared" ref="O3:O12" si="10">SQRT(M3^2 + N3^2)</f>
         <v>0.97803269999999998</v>
       </c>
       <c r="P3" s="15">
@@ -2351,7 +2351,7 @@
         <v>-1.5707963267948966</v>
       </c>
       <c r="Q3" s="15">
-        <f t="shared" ref="Q3:Q12" si="24">P3*(180/PI())</f>
+        <f t="shared" ref="Q3:Q12" si="11">P3*(180/PI())</f>
         <v>-90</v>
       </c>
       <c r="R3" s="15">
@@ -2359,15 +2359,15 @@
         <v>-1.2085474226821971E-20</v>
       </c>
       <c r="S3" s="15">
-        <f t="shared" ref="S3:S12" si="25" xml:space="preserve"> ((AB3+AE3)/(W3)) + AL3</f>
+        <f t="shared" ref="S3:S12" si="12" xml:space="preserve"> ((AB3+AE3)/(W3)) + AL3</f>
         <v>-9.7801298609546308</v>
       </c>
       <c r="T3" s="15">
-        <f t="shared" ref="T3:T12" si="26">SQRT((R3^2)+(S3^2))</f>
+        <f t="shared" ref="T3:T12" si="13">SQRT((R3^2)+(S3^2))</f>
         <v>9.7801298609546308</v>
       </c>
       <c r="U3" s="15">
-        <f t="shared" ref="U3:U12" si="27" xml:space="preserve"> ATAN2($B$23+H3, F3)</f>
+        <f xml:space="preserve"> ATAN2($B$23+G3, F3)</f>
         <v>0</v>
       </c>
       <c r="V3" s="15">
@@ -2375,71 +2375,71 @@
         <v>0</v>
       </c>
       <c r="W3" s="15">
-        <f t="shared" ref="W3:W12" si="28">IF(AC2&gt;0, IF(W2 &gt;( $B$9 + $B$11*$B$2), W2 -( $B$11*$B$2), $B$9), W2)</f>
+        <f t="shared" ref="W3:W12" si="14">IF(AC2&gt;0, IF(W2 &gt;( $B$9 + $B$11*$B$2), W2 -( $B$11*$B$2), $B$9), W2)</f>
         <v>200</v>
       </c>
       <c r="X3" s="16">
+        <f xml:space="preserve"> IF(G3&lt;30000, O3/AM3, "")</f>
+        <v>2.8740291759590825E-3</v>
+      </c>
+      <c r="Y3" s="15">
+        <f t="shared" ref="Y3:Y12" si="15">0.35</f>
+        <v>0.35</v>
+      </c>
+      <c r="Z3" s="15">
         <f t="shared" si="2"/>
-        <v>2.8740291759590825E-3</v>
-      </c>
-      <c r="Y3" s="15">
-        <f t="shared" ref="Y3:Y12" si="29">0.35</f>
-        <v>0.35</v>
-      </c>
-      <c r="Z3" s="15">
+        <v>3.9457991163114638E-2</v>
+      </c>
+      <c r="AA3" s="15">
         <f t="shared" si="3"/>
+        <v>-2.417094845364394E-18</v>
+      </c>
+      <c r="AB3" s="15">
+        <f t="shared" si="4"/>
         <v>3.9457991163114638E-2</v>
       </c>
-      <c r="AA3" s="15">
-        <f t="shared" si="4"/>
-        <v>-2.417094845364394E-18</v>
-      </c>
-      <c r="AB3" s="15">
+      <c r="AC3" s="10">
+        <f>IF(E3 &gt;= $B$16, IF(E3 &lt; $B$17, B16, 0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD3" s="10">
         <f t="shared" si="5"/>
-        <v>3.9457991163114638E-2</v>
-      </c>
-      <c r="AC3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AD3" s="10">
+      <c r="AF3" s="10">
         <f t="shared" si="7"/>
+        <v>47.827398113464497</v>
+      </c>
+      <c r="AG3" s="10">
+        <f>($B$9)*AJ3*G3</f>
+        <v>47.827398851441266</v>
+      </c>
+      <c r="AH3" s="10">
+        <f t="shared" ref="AH3:AH12" si="16" xml:space="preserve"> ABS(AF3) + ABS(AG3)</f>
+        <v>95.654796964905756</v>
+      </c>
+      <c r="AI3" s="10">
+        <f t="shared" si="8"/>
+        <v>97.803269999999998</v>
+      </c>
+      <c r="AJ3" s="15">
+        <f>IF(G3&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G3)+((6.26*10^(-13))*(G3)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
+        <v>-9.7803271509104466</v>
+      </c>
+      <c r="AK3" s="15">
+        <f t="shared" ref="AK3:AK12" si="17" xml:space="preserve"> AJ3*SIN(U3)</f>
         <v>0</v>
       </c>
-      <c r="AE3" s="10">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF3" s="10">
-        <f t="shared" si="9"/>
-        <v>47.827398113464497</v>
-      </c>
-      <c r="AG3" s="10">
-        <f t="shared" si="10"/>
-        <v>47.827398851441266</v>
-      </c>
-      <c r="AH3" s="10">
-        <f t="shared" ref="AH3:AH12" si="30" xml:space="preserve"> ABS(AF3) + ABS(AG3)</f>
-        <v>95.654796964905756</v>
-      </c>
-      <c r="AI3" s="10">
-        <f t="shared" si="11"/>
-        <v>97.803269999999998</v>
-      </c>
-      <c r="AJ3" s="15">
-        <f t="shared" si="12"/>
+      <c r="AL3" s="15">
+        <f t="shared" ref="AL3:AL12" si="18" xml:space="preserve"> AJ3*COS(U3)</f>
         <v>-9.7803271509104466</v>
       </c>
-      <c r="AK3" s="15">
-        <f t="shared" ref="AK3:AK12" si="31" xml:space="preserve"> AJ3*SIN(U3)</f>
-        <v>0</v>
-      </c>
-      <c r="AL3" s="15">
-        <f t="shared" ref="AL3:AL12" si="32" xml:space="preserve"> AJ3*COS(U3)</f>
-        <v>-9.7803271509104466</v>
-      </c>
       <c r="AM3" s="15">
-        <f t="shared" si="13"/>
+        <f>IF(G3&lt;100000, IF(G3&gt;10000, (343.2)+(-4.313943*G3)+(-0.291943*G3^2)+(0.053721*G3^3)+((-3.039687*10^(-3))*G3^4)+((9.262166*10^(-5))*G3^5)+((-1.647967*10^(-6))*G3^6)+((1.694814*10^(-8))*G3^7)+((-9.299892*10^(-11))*G3^8)+((2.104694*10^(-13))*G3^9), ((-0.00406576*G3)+340.3)), 0)</f>
         <v>340.30019882231153</v>
       </c>
       <c r="AN3" s="16">
@@ -2447,11 +2447,11 @@
         <v>1.2004947955443879</v>
       </c>
       <c r="AO3" s="10">
-        <f t="shared" si="14"/>
+        <f>IF(G3&gt;38000,0,(101325*(1-(2.25577*10^(-5))*G3)^5.25588))</f>
         <v>101325.58746401522</v>
       </c>
       <c r="AP3" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>294.02834137714672</v>
       </c>
     </row>
@@ -2466,59 +2466,59 @@
         <v>2</v>
       </c>
       <c r="D4" s="10">
-        <f t="shared" ref="D4:D12" si="33">D3 + 1</f>
+        <f t="shared" ref="D4:D12" si="19">D3 + 1</f>
         <v>2</v>
       </c>
       <c r="E4" s="11">
-        <f t="shared" ref="E4:E12" si="34" xml:space="preserve"> E3 + $B$2</f>
+        <f t="shared" ref="E4:E12" si="20" xml:space="preserve"> E3 + $B$2</f>
         <v>0.2</v>
       </c>
       <c r="F4" s="15">
-        <f t="shared" si="16"/>
+        <f>F3 + M3*($B$2) + (0.5)*(R3)*($B$2)^2</f>
         <v>-6.0427371134109869E-23</v>
       </c>
-      <c r="G4" s="13">
-        <f t="shared" si="17"/>
+      <c r="G4" s="18">
+        <f xml:space="preserve"> G3 + N3*($B$2) + (0.5)*(S3)*($B$2)^2</f>
+        <v>-0.19560555430477317</v>
+      </c>
+      <c r="H4" s="13">
+        <f xml:space="preserve"> (F4/1000)</f>
         <v>-6.0427371134109865E-26</v>
       </c>
-      <c r="H4" s="18">
-        <f t="shared" si="18"/>
-        <v>-0.19560555430477317</v>
-      </c>
       <c r="I4" s="13">
-        <f t="shared" si="19"/>
+        <f>G4/1000</f>
         <v>-1.9560555430477318E-4</v>
       </c>
       <c r="J4" s="15">
-        <f t="shared" si="20"/>
+        <f>J3 + SQRT( (F4-F3)^2 + (G4-G3)^2 )</f>
         <v>0.19560555430477317</v>
       </c>
       <c r="K4" s="41">
-        <f t="shared" si="21"/>
+        <f>SQRT((F4)^2 + (G4+$B$23)^2)</f>
         <v>6378136.8043944454</v>
       </c>
       <c r="L4" s="14">
-        <f t="shared" si="22"/>
+        <f>SQRT(F4^2 + G4^2)</f>
         <v>0.19560555430477317</v>
       </c>
       <c r="M4" s="15">
-        <f t="shared" ref="M4:M12" si="35" xml:space="preserve"> M3 + R3*($B$2)</f>
+        <f t="shared" ref="M4:M12" si="21" xml:space="preserve"> M3 + R3*($B$2)</f>
         <v>-1.2085474226821972E-21</v>
       </c>
       <c r="N4" s="15">
-        <f t="shared" ref="N4:N12" si="36">N3 + S3*$B$2</f>
+        <f t="shared" ref="N4:N12" si="22">N3 + S3*$B$2</f>
         <v>-1.9560456860954631</v>
       </c>
       <c r="O4" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>1.9560456860954631</v>
       </c>
       <c r="P4" s="15">
-        <f t="shared" ref="P4:P12" si="37">ATAN2(M4,N4)</f>
+        <f t="shared" ref="P4:P12" si="23">ATAN2(M4,N4)</f>
         <v>-1.5707963267948966</v>
       </c>
       <c r="Q4" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>-90</v>
       </c>
       <c r="R4" s="15">
@@ -2526,15 +2526,15 @@
         <v>-4.8341599774508962E-20</v>
       </c>
       <c r="S4" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="12"/>
         <v>-9.7795384486645478</v>
       </c>
       <c r="T4" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="13"/>
         <v>9.7795384486645478</v>
       </c>
       <c r="U4" s="15">
-        <f t="shared" si="27"/>
+        <f xml:space="preserve"> ATAN2($B$23+G4, F4)</f>
         <v>-9.4741415851218922E-30</v>
       </c>
       <c r="V4" s="15">
@@ -2542,83 +2542,83 @@
         <v>-1.6535496446049164E-31</v>
       </c>
       <c r="W4" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="14"/>
         <v>200</v>
       </c>
       <c r="X4" s="16">
+        <f xml:space="preserve"> IF(G4&lt;30000, O4/AM4, "")</f>
+        <v>5.7479903461756972E-3</v>
+      </c>
+      <c r="Y4" s="15">
+        <f t="shared" si="15"/>
+        <v>0.35</v>
+      </c>
+      <c r="Z4" s="15">
         <f t="shared" si="2"/>
-        <v>5.7479903461756972E-3</v>
-      </c>
-      <c r="Y4" s="15">
-        <f t="shared" si="29"/>
-        <v>0.35</v>
-      </c>
-      <c r="Z4" s="15">
+        <v>0.15783099484306926</v>
+      </c>
+      <c r="AA4" s="15">
         <f t="shared" si="3"/>
+        <v>-9.6683199734338339E-18</v>
+      </c>
+      <c r="AB4" s="15">
+        <f t="shared" si="4"/>
         <v>0.15783099484306926</v>
       </c>
-      <c r="AA4" s="15">
-        <f t="shared" si="4"/>
-        <v>-9.6683199734338339E-18</v>
-      </c>
-      <c r="AB4" s="15">
+      <c r="AC4" s="10">
+        <f>IF(E4 &gt;= $B$16, IF(E4 &lt; $B$17, B17, 0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="10">
         <f t="shared" si="5"/>
-        <v>0.15783099484306926</v>
-      </c>
-      <c r="AC4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AD4" s="10">
+      <c r="AF4" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AE4" s="10">
+        <v>191.30573630463357</v>
+      </c>
+      <c r="AG4" s="10">
+        <f>($B$9)*AJ4*G4</f>
+        <v>191.30864021920343</v>
+      </c>
+      <c r="AH4" s="10">
+        <f t="shared" si="16"/>
+        <v>382.614376523837</v>
+      </c>
+      <c r="AI4" s="10">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF4" s="10">
+        <v>195.60456860954631</v>
+      </c>
+      <c r="AJ4" s="15">
+        <f>IF(G4&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G4)+((6.26*10^(-13))*(G4)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
+        <v>-9.7803276036387636</v>
+      </c>
+      <c r="AK4" s="15">
+        <f t="shared" si="17"/>
+        <v>9.2660208465749556E-29</v>
+      </c>
+      <c r="AL4" s="15">
+        <f t="shared" si="18"/>
+        <v>-9.7803276036387636</v>
+      </c>
+      <c r="AM4" s="15">
+        <f>IF(G4&lt;100000, IF(G4&gt;10000, (343.2)+(-4.313943*G4)+(-0.291943*G4^2)+(0.053721*G4^3)+((-3.039687*10^(-3))*G4^4)+((9.262166*10^(-5))*G4^5)+((-1.647967*10^(-6))*G4^6)+((1.694814*10^(-8))*G4^7)+((-9.299892*10^(-11))*G4^8)+((2.104694*10^(-13))*G4^9), ((-0.00406576*G4)+340.3)), 0)</f>
+        <v>340.30079528523851</v>
+      </c>
+      <c r="AN4" s="16">
+        <f t="shared" ref="AN4:AN12" si="24" xml:space="preserve"> AO4 / (287.058*AP4)</f>
+        <v>1.2005116172430963</v>
+      </c>
+      <c r="AO4" s="10">
+        <f>IF(G4&gt;38000,0,(101325*(1-(2.25577*10^(-5))*G4)^5.25588))</f>
+        <v>101327.34986076689</v>
+      </c>
+      <c r="AP4" s="15">
         <f t="shared" si="9"/>
-        <v>191.30573630463357</v>
-      </c>
-      <c r="AG4" s="10">
-        <f t="shared" si="10"/>
-        <v>191.30864021920343</v>
-      </c>
-      <c r="AH4" s="10">
-        <f t="shared" si="30"/>
-        <v>382.614376523837</v>
-      </c>
-      <c r="AI4" s="10">
-        <f t="shared" si="11"/>
-        <v>195.60456860954631</v>
-      </c>
-      <c r="AJ4" s="15">
-        <f t="shared" si="12"/>
-        <v>-9.7803276036387636</v>
-      </c>
-      <c r="AK4" s="15">
-        <f t="shared" si="31"/>
-        <v>9.2660208465749556E-29</v>
-      </c>
-      <c r="AL4" s="15">
-        <f t="shared" si="32"/>
-        <v>-9.7803276036387636</v>
-      </c>
-      <c r="AM4" s="15">
-        <f t="shared" si="13"/>
-        <v>340.30079528523851</v>
-      </c>
-      <c r="AN4" s="16">
-        <f t="shared" ref="AN4:AN12" si="38" xml:space="preserve"> AO4 / (287.058*AP4)</f>
-        <v>1.2005116172430963</v>
-      </c>
-      <c r="AO4" s="10">
-        <f t="shared" si="14"/>
-        <v>101327.34986076689</v>
-      </c>
-      <c r="AP4" s="15">
-        <f t="shared" si="15"/>
         <v>294.0293355019071</v>
       </c>
     </row>
@@ -2634,59 +2634,59 @@
         <v>3</v>
       </c>
       <c r="D5" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="E5" s="11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="20"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="F5" s="15">
-        <f t="shared" si="16"/>
+        <f>F4 + M4*($B$2) + (0.5)*(R4)*($B$2)^2</f>
         <v>-4.2299011227487443E-22</v>
       </c>
-      <c r="G5" s="13">
-        <f t="shared" si="17"/>
+      <c r="G5" s="18">
+        <f xml:space="preserve"> G4 + N4*($B$2) + (0.5)*(S4)*($B$2)^2</f>
+        <v>-0.44010781515764225</v>
+      </c>
+      <c r="H5" s="13">
+        <f xml:space="preserve"> (F5/1000)</f>
         <v>-4.2299011227487444E-25</v>
       </c>
-      <c r="H5" s="18">
-        <f t="shared" si="18"/>
-        <v>-0.44010781515764225</v>
-      </c>
       <c r="I5" s="13">
-        <f t="shared" si="19"/>
+        <f>G5/1000</f>
         <v>-4.4010781515764225E-4</v>
       </c>
       <c r="J5" s="15">
-        <f t="shared" si="20"/>
+        <f>J4 + SQRT( (F5-F4)^2 + (G5-G4)^2 )</f>
         <v>0.44010781515764225</v>
       </c>
       <c r="K5" s="41">
+        <f>SQRT((F5)^2 + (G5+$B$23)^2)</f>
+        <v>6378136.559892185</v>
+      </c>
+      <c r="L5" s="14">
+        <f>SQRT(F5^2 + G5^2)</f>
+        <v>0.44010781515764225</v>
+      </c>
+      <c r="M5" s="15">
         <f t="shared" si="21"/>
-        <v>6378136.559892185</v>
-      </c>
-      <c r="L5" s="14">
+        <v>-6.0427074001330938E-21</v>
+      </c>
+      <c r="N5" s="15">
         <f t="shared" si="22"/>
-        <v>0.44010781515764225</v>
-      </c>
-      <c r="M5" s="15">
-        <f t="shared" si="35"/>
-        <v>-6.0427074001330938E-21</v>
-      </c>
-      <c r="N5" s="15">
-        <f t="shared" si="36"/>
         <v>-2.933999530961918</v>
       </c>
       <c r="O5" s="15">
+        <f t="shared" si="10"/>
+        <v>2.933999530961918</v>
+      </c>
+      <c r="P5" s="15">
         <f t="shared" si="23"/>
-        <v>2.933999530961918</v>
-      </c>
-      <c r="P5" s="15">
-        <f t="shared" si="37"/>
         <v>-1.5707963267948966</v>
       </c>
       <c r="Q5" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>-90</v>
       </c>
       <c r="R5" s="15">
@@ -2694,15 +2694,15 @@
         <v>-1.0876602346293774E-19</v>
       </c>
       <c r="S5" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="12"/>
         <v>-9.7785528015261995</v>
       </c>
       <c r="T5" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="13"/>
         <v>9.7785528015261995</v>
       </c>
       <c r="U5" s="15">
-        <f t="shared" si="27"/>
+        <f xml:space="preserve"> ATAN2($B$23+G5, F5)</f>
         <v>-6.6318760707441573E-29</v>
       </c>
       <c r="V5" s="15">
@@ -2710,83 +2710,83 @@
         <v>-1.1574807301870994E-30</v>
       </c>
       <c r="W5" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="14"/>
         <v>200</v>
       </c>
       <c r="X5" s="16">
+        <f xml:space="preserve"> IF(G5&lt;30000, O5/AM5, "")</f>
+        <v>8.6217575769140398E-3</v>
+      </c>
+      <c r="Y5" s="15">
+        <f t="shared" si="15"/>
+        <v>0.35</v>
+      </c>
+      <c r="Z5" s="15">
         <f t="shared" si="2"/>
-        <v>8.6217575769140398E-3</v>
-      </c>
-      <c r="Y5" s="15">
-        <f t="shared" si="29"/>
-        <v>0.35</v>
-      </c>
-      <c r="Z5" s="15">
+        <v>0.35511132932757777</v>
+      </c>
+      <c r="AA5" s="15">
         <f t="shared" si="3"/>
+        <v>-2.1753204822311403E-17</v>
+      </c>
+      <c r="AB5" s="15">
+        <f t="shared" si="4"/>
         <v>0.35511132932757777</v>
       </c>
-      <c r="AA5" s="15">
-        <f t="shared" si="4"/>
-        <v>-2.1753204822311403E-17</v>
-      </c>
-      <c r="AB5" s="15">
+      <c r="AC5" s="10">
+        <f>IF(E5 &gt;= $B$16, IF(E5 &lt; $B$17, B18, 0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD5" s="10">
         <f t="shared" si="5"/>
-        <v>0.35511132932757777</v>
-      </c>
-      <c r="AC5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AD5" s="10">
+      <c r="AF5" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AE5" s="10">
+        <v>430.41766238423776</v>
+      </c>
+      <c r="AG5" s="10">
+        <f>($B$9)*AJ5*G5</f>
+        <v>430.43989452397778</v>
+      </c>
+      <c r="AH5" s="10">
+        <f t="shared" si="16"/>
+        <v>860.85755690821554</v>
+      </c>
+      <c r="AI5" s="10">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF5" s="10">
+        <v>293.39995309619178</v>
+      </c>
+      <c r="AJ5" s="15">
+        <f>IF(G5&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G5)+((6.26*10^(-13))*(G5)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
+        <v>-9.780328358172838</v>
+      </c>
+      <c r="AK5" s="15">
+        <f t="shared" si="17"/>
+        <v>6.4861925602586931E-28</v>
+      </c>
+      <c r="AL5" s="15">
+        <f t="shared" si="18"/>
+        <v>-9.780328358172838</v>
+      </c>
+      <c r="AM5" s="15">
+        <f>IF(G5&lt;100000, IF(G5&gt;10000, (343.2)+(-4.313943*G5)+(-0.291943*G5^2)+(0.053721*G5^3)+((-3.039687*10^(-3))*G5^4)+((9.262166*10^(-5))*G5^5)+((-1.647967*10^(-6))*G5^6)+((1.694814*10^(-8))*G5^7)+((-9.299892*10^(-11))*G5^8)+((2.104694*10^(-13))*G5^9), ((-0.00406576*G5)+340.3)), 0)</f>
+        <v>340.30178937275059</v>
+      </c>
+      <c r="AN5" s="16">
+        <f t="shared" si="24"/>
+        <v>1.2005396533185746</v>
+      </c>
+      <c r="AO5" s="10">
+        <f>IF(G5&gt;38000,0,(101325*(1-(2.25577*10^(-5))*G5)^5.25588))</f>
+        <v>101330.28719253176</v>
+      </c>
+      <c r="AP5" s="15">
         <f t="shared" si="9"/>
-        <v>430.41766238423776</v>
-      </c>
-      <c r="AG5" s="10">
-        <f t="shared" si="10"/>
-        <v>430.43989452397778</v>
-      </c>
-      <c r="AH5" s="10">
-        <f t="shared" si="30"/>
-        <v>860.85755690821554</v>
-      </c>
-      <c r="AI5" s="10">
-        <f t="shared" si="11"/>
-        <v>293.39995309619178</v>
-      </c>
-      <c r="AJ5" s="15">
-        <f t="shared" si="12"/>
-        <v>-9.780328358172838</v>
-      </c>
-      <c r="AK5" s="15">
-        <f t="shared" si="31"/>
-        <v>6.4861925602586931E-28</v>
-      </c>
-      <c r="AL5" s="15">
-        <f t="shared" si="32"/>
-        <v>-9.780328358172838</v>
-      </c>
-      <c r="AM5" s="15">
-        <f t="shared" si="13"/>
-        <v>340.30178937275059</v>
-      </c>
-      <c r="AN5" s="16">
-        <f t="shared" si="38"/>
-        <v>1.2005396533185746</v>
-      </c>
-      <c r="AO5" s="10">
-        <f t="shared" si="14"/>
-        <v>101330.28719253176</v>
-      </c>
-      <c r="AP5" s="15">
-        <f t="shared" si="15"/>
         <v>294.03099234756348</v>
       </c>
     </row>
@@ -2801,59 +2801,59 @@
         <v>2</v>
       </c>
       <c r="D6" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
       <c r="E6" s="11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="20"/>
         <v>0.4</v>
       </c>
       <c r="F6" s="15">
-        <f t="shared" si="16"/>
+        <f>F5 + M5*($B$2) + (0.5)*(R5)*($B$2)^2</f>
         <v>-1.5710909696028726E-21</v>
       </c>
-      <c r="G6" s="13">
-        <f t="shared" si="17"/>
+      <c r="G6" s="18">
+        <f xml:space="preserve"> G5 + N5*($B$2) + (0.5)*(S5)*($B$2)^2</f>
+        <v>-0.782400532261465</v>
+      </c>
+      <c r="H6" s="13">
+        <f xml:space="preserve"> (F6/1000)</f>
         <v>-1.5710909696028726E-24</v>
       </c>
-      <c r="H6" s="18">
-        <f t="shared" si="18"/>
-        <v>-0.782400532261465</v>
-      </c>
       <c r="I6" s="13">
-        <f t="shared" si="19"/>
+        <f>G6/1000</f>
         <v>-7.8240053226146498E-4</v>
       </c>
       <c r="J6" s="15">
-        <f t="shared" si="20"/>
+        <f>J5 + SQRT( (F6-F5)^2 + (G6-G5)^2 )</f>
         <v>0.782400532261465</v>
       </c>
       <c r="K6" s="41">
+        <f>SQRT((F6)^2 + (G6+$B$23)^2)</f>
+        <v>6378136.2175994674</v>
+      </c>
+      <c r="L6" s="14">
+        <f>SQRT(F6^2 + G6^2)</f>
+        <v>0.782400532261465</v>
+      </c>
+      <c r="M6" s="15">
         <f t="shared" si="21"/>
-        <v>6378136.2175994674</v>
-      </c>
-      <c r="L6" s="14">
+        <v>-1.6919309746426869E-20</v>
+      </c>
+      <c r="N6" s="15">
         <f t="shared" si="22"/>
-        <v>0.782400532261465</v>
-      </c>
-      <c r="M6" s="15">
-        <f t="shared" si="35"/>
-        <v>-1.6919309746426869E-20</v>
-      </c>
-      <c r="N6" s="15">
-        <f t="shared" si="36"/>
         <v>-3.9118548111145381</v>
       </c>
       <c r="O6" s="15">
+        <f t="shared" si="10"/>
+        <v>3.9118548111145381</v>
+      </c>
+      <c r="P6" s="15">
         <f t="shared" si="23"/>
-        <v>3.9118548111145381</v>
-      </c>
-      <c r="P6" s="15">
-        <f t="shared" si="37"/>
         <v>-1.5707963267948966</v>
       </c>
       <c r="Q6" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>-90</v>
       </c>
       <c r="R6" s="15">
@@ -2861,15 +2861,15 @@
         <v>-1.9335384882074849E-19</v>
       </c>
       <c r="S6" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="12"/>
         <v>-9.777172999435944</v>
       </c>
       <c r="T6" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="13"/>
         <v>9.777172999435944</v>
       </c>
       <c r="U6" s="15">
-        <f t="shared" si="27"/>
+        <f xml:space="preserve"> ATAN2($B$23+G6, F6)</f>
         <v>-2.4632446156726684E-28</v>
       </c>
       <c r="V6" s="15">
@@ -2877,83 +2877,83 @@
         <v>-4.2991728825510383E-30</v>
       </c>
       <c r="W6" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="14"/>
         <v>200</v>
       </c>
       <c r="X6" s="16">
+        <f xml:space="preserve"> IF(G6&lt;30000, O6/AM6, "")</f>
+        <v>1.1495204949341125E-2</v>
+      </c>
+      <c r="Y6" s="15">
+        <f t="shared" si="15"/>
+        <v>0.35</v>
+      </c>
+      <c r="Z6" s="15">
         <f t="shared" si="2"/>
-        <v>1.1495204949341125E-2</v>
-      </c>
-      <c r="Y6" s="15">
-        <f t="shared" si="29"/>
-        <v>0.35</v>
-      </c>
-      <c r="Z6" s="15">
+        <v>0.63128301049624069</v>
+      </c>
+      <c r="AA6" s="15">
         <f t="shared" si="3"/>
+        <v>-3.8670770245976572E-17</v>
+      </c>
+      <c r="AB6" s="15">
+        <f t="shared" si="4"/>
         <v>0.63128301049624069</v>
       </c>
-      <c r="AA6" s="15">
-        <f t="shared" si="4"/>
-        <v>-3.8670770245976572E-17</v>
-      </c>
-      <c r="AB6" s="15">
+      <c r="AC6" s="10">
+        <f>IF(E6 &gt;= $B$16, IF(E6 &lt; $B$17, B19, 0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="10">
         <f t="shared" si="5"/>
-        <v>0.63128301049624069</v>
-      </c>
-      <c r="AC6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="10">
+      <c r="AF6" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AE6" s="10">
+        <v>765.13040316199795</v>
+      </c>
+      <c r="AG6" s="10">
+        <f>($B$9)*AJ6*G6</f>
+        <v>765.21349395882066</v>
+      </c>
+      <c r="AH6" s="10">
+        <f t="shared" si="16"/>
+        <v>1530.3438971208186</v>
+      </c>
+      <c r="AI6" s="10">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF6" s="10">
+        <v>391.18548111145384</v>
+      </c>
+      <c r="AJ6" s="15">
+        <f>IF(G6&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G6)+((6.26*10^(-13))*(G6)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
+        <v>-9.7803294144884259</v>
+      </c>
+      <c r="AK6" s="15">
+        <f t="shared" si="17"/>
+        <v>2.4091343769743636E-27</v>
+      </c>
+      <c r="AL6" s="15">
+        <f t="shared" si="18"/>
+        <v>-9.7803294144884259</v>
+      </c>
+      <c r="AM6" s="15">
+        <f>IF(G6&lt;100000, IF(G6&gt;10000, (343.2)+(-4.313943*G6)+(-0.291943*G6^2)+(0.053721*G6^3)+((-3.039687*10^(-3))*G6^4)+((9.262166*10^(-5))*G6^5)+((-1.647967*10^(-6))*G6^6)+((1.694814*10^(-8))*G6^7)+((-9.299892*10^(-11))*G6^8)+((2.104694*10^(-13))*G6^9), ((-0.00406576*G6)+340.3)), 0)</f>
+        <v>340.30318105278803</v>
+      </c>
+      <c r="AN6" s="16">
+        <f t="shared" si="24"/>
+        <v>1.2005789034676997</v>
+      </c>
+      <c r="AO6" s="10">
+        <f>IF(G6&gt;38000,0,(101325*(1-(2.25577*10^(-5))*G6)^5.25588))</f>
+        <v>101334.39944731123</v>
+      </c>
+      <c r="AP6" s="15">
         <f t="shared" si="9"/>
-        <v>765.13040316199795</v>
-      </c>
-      <c r="AG6" s="10">
-        <f t="shared" si="10"/>
-        <v>765.21349395882066</v>
-      </c>
-      <c r="AH6" s="10">
-        <f t="shared" si="30"/>
-        <v>1530.3438971208186</v>
-      </c>
-      <c r="AI6" s="10">
-        <f t="shared" si="11"/>
-        <v>391.18548111145384</v>
-      </c>
-      <c r="AJ6" s="15">
-        <f t="shared" si="12"/>
-        <v>-9.7803294144884259</v>
-      </c>
-      <c r="AK6" s="15">
-        <f t="shared" si="31"/>
-        <v>2.4091343769743636E-27</v>
-      </c>
-      <c r="AL6" s="15">
-        <f t="shared" si="32"/>
-        <v>-9.7803294144884259</v>
-      </c>
-      <c r="AM6" s="15">
-        <f t="shared" si="13"/>
-        <v>340.30318105278803</v>
-      </c>
-      <c r="AN6" s="16">
-        <f t="shared" si="38"/>
-        <v>1.2005789034676997</v>
-      </c>
-      <c r="AO6" s="10">
-        <f t="shared" si="14"/>
-        <v>101334.39944731123</v>
-      </c>
-      <c r="AP6" s="15">
-        <f t="shared" si="15"/>
         <v>294.03331186068181</v>
       </c>
     </row>
@@ -2969,59 +2969,59 @@
         <v>3</v>
       </c>
       <c r="D7" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
       <c r="E7" s="11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
       <c r="F7" s="15">
-        <f t="shared" si="16"/>
+        <f>F6 + M6*($B$2) + (0.5)*(R6)*($B$2)^2</f>
         <v>-4.2297911883493018E-21</v>
       </c>
-      <c r="G7" s="13">
-        <f t="shared" si="17"/>
+      <c r="G7" s="18">
+        <f xml:space="preserve"> G6 + N6*($B$2) + (0.5)*(S6)*($B$2)^2</f>
+        <v>-1.2224718783700985</v>
+      </c>
+      <c r="H7" s="13">
+        <f xml:space="preserve"> (F7/1000)</f>
         <v>-4.229791188349302E-24</v>
       </c>
-      <c r="H7" s="18">
-        <f t="shared" si="18"/>
-        <v>-1.2224718783700985</v>
-      </c>
       <c r="I7" s="13">
-        <f t="shared" si="19"/>
+        <f>G7/1000</f>
         <v>-1.2224718783700986E-3</v>
       </c>
       <c r="J7" s="15">
-        <f t="shared" si="20"/>
+        <f>J6 + SQRT( (F7-F6)^2 + (G7-G6)^2 )</f>
         <v>1.2224718783700985</v>
       </c>
       <c r="K7" s="41">
+        <f>SQRT((F7)^2 + (G7+$B$23)^2)</f>
+        <v>6378135.7775281221</v>
+      </c>
+      <c r="L7" s="14">
+        <f>SQRT(F7^2 + G7^2)</f>
+        <v>1.2224718783700985</v>
+      </c>
+      <c r="M7" s="15">
         <f t="shared" si="21"/>
-        <v>6378135.7775281221</v>
-      </c>
-      <c r="L7" s="14">
+        <v>-3.625469462850172E-20</v>
+      </c>
+      <c r="N7" s="15">
         <f t="shared" si="22"/>
-        <v>1.2224718783700985</v>
-      </c>
-      <c r="M7" s="15">
-        <f t="shared" si="35"/>
-        <v>-3.625469462850172E-20</v>
-      </c>
-      <c r="N7" s="15">
-        <f t="shared" si="36"/>
         <v>-4.8895721110581327</v>
       </c>
       <c r="O7" s="15">
+        <f t="shared" si="10"/>
+        <v>4.8895721110581327</v>
+      </c>
+      <c r="P7" s="15">
         <f t="shared" si="23"/>
-        <v>4.8895721110581327</v>
-      </c>
-      <c r="P7" s="15">
-        <f t="shared" si="37"/>
         <v>-1.5707963267948966</v>
       </c>
       <c r="Q7" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>-90</v>
       </c>
       <c r="R7" s="15">
@@ -3029,15 +3029,15 @@
         <v>-3.0209763651539501E-19</v>
       </c>
       <c r="S7" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="12"/>
         <v>-9.77539916378303</v>
       </c>
       <c r="T7" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="13"/>
         <v>9.77539916378303</v>
       </c>
       <c r="U7" s="15">
-        <f t="shared" si="27"/>
+        <f xml:space="preserve"> ATAN2($B$23+G7, F7)</f>
         <v>-6.6317045228983475E-28</v>
       </c>
       <c r="V7" s="15">
@@ -3045,141 +3045,141 @@
         <v>-1.1574507894397586E-29</v>
       </c>
       <c r="W7" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="14"/>
         <v>200</v>
       </c>
       <c r="X7" s="16">
+        <f xml:space="preserve"> IF(G7&lt;30000, O7/AM7, "")</f>
+        <v>1.4368206573869148E-2</v>
+      </c>
+      <c r="Y7" s="15">
+        <f t="shared" si="15"/>
+        <v>0.35</v>
+      </c>
+      <c r="Z7" s="15">
         <f t="shared" si="2"/>
-        <v>1.4368206573869148E-2</v>
-      </c>
-      <c r="Y7" s="15">
-        <f t="shared" si="29"/>
-        <v>0.35</v>
-      </c>
-      <c r="Z7" s="15">
+        <v>0.9863217532244416</v>
+      </c>
+      <c r="AA7" s="15">
         <f t="shared" si="3"/>
+        <v>-6.0419528600284285E-17</v>
+      </c>
+      <c r="AB7" s="15">
+        <f t="shared" si="4"/>
         <v>0.9863217532244416</v>
       </c>
-      <c r="AA7" s="15">
-        <f t="shared" si="4"/>
-        <v>-6.0419528600284285E-17</v>
-      </c>
-      <c r="AB7" s="15">
+      <c r="AC7" s="10">
+        <f>IF(E7 &gt;= $B$16, IF(E7 &lt; $B$17, B20, 0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="10">
         <f t="shared" si="5"/>
-        <v>0.9863217532244416</v>
-      </c>
-      <c r="AC7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AD7" s="10">
+      <c r="AF7" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AE7" s="10">
+        <v>1195.3957714618741</v>
+      </c>
+      <c r="AG7" s="10">
+        <f>($B$9)*AJ7*G7</f>
+        <v>1195.6179330599039</v>
+      </c>
+      <c r="AH7" s="10">
+        <f t="shared" si="16"/>
+        <v>2391.013704521778</v>
+      </c>
+      <c r="AI7" s="10">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF7" s="10">
+        <v>488.95721110581326</v>
+      </c>
+      <c r="AJ7" s="15">
+        <f>IF(G7&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G7)+((6.26*10^(-13))*(G7)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
+        <v>-9.7803307725491528</v>
+      </c>
+      <c r="AK7" s="15">
+        <f t="shared" si="17"/>
+        <v>6.4860263819756101E-27</v>
+      </c>
+      <c r="AL7" s="15">
+        <f t="shared" si="18"/>
+        <v>-9.7803307725491528</v>
+      </c>
+      <c r="AM7" s="15">
+        <f>IF(G7&lt;100000, IF(G7&gt;10000, (343.2)+(-4.313943*G7)+(-0.291943*G7^2)+(0.053721*G7^3)+((-3.039687*10^(-3))*G7^4)+((9.262166*10^(-5))*G7^5)+((-1.647967*10^(-6))*G7^6)+((1.694814*10^(-8))*G7^7)+((-9.299892*10^(-11))*G7^8)+((2.104694*10^(-13))*G7^9), ((-0.00406576*G7)+340.3)), 0)</f>
+        <v>340.3049702772642</v>
+      </c>
+      <c r="AN7" s="16">
+        <f t="shared" si="24"/>
+        <v>1.2006293671756474</v>
+      </c>
+      <c r="AO7" s="10">
+        <f>IF(G7&gt;38000,0,(101325*(1-(2.25577*10^(-5))*G7)^5.25588))</f>
+        <v>101339.68659882821</v>
+      </c>
+      <c r="AP7" s="15">
         <f t="shared" si="9"/>
-        <v>1195.3957714618741</v>
-      </c>
-      <c r="AG7" s="10">
-        <f t="shared" si="10"/>
-        <v>1195.6179330599039</v>
-      </c>
-      <c r="AH7" s="10">
-        <f t="shared" si="30"/>
-        <v>2391.013704521778</v>
-      </c>
-      <c r="AI7" s="10">
-        <f t="shared" si="11"/>
-        <v>488.95721110581326</v>
-      </c>
-      <c r="AJ7" s="15">
-        <f t="shared" si="12"/>
-        <v>-9.7803307725491528</v>
-      </c>
-      <c r="AK7" s="15">
-        <f t="shared" si="31"/>
-        <v>6.4860263819756101E-27</v>
-      </c>
-      <c r="AL7" s="15">
-        <f t="shared" si="32"/>
-        <v>-9.7803307725491528</v>
-      </c>
-      <c r="AM7" s="15">
-        <f t="shared" si="13"/>
-        <v>340.3049702772642</v>
-      </c>
-      <c r="AN7" s="16">
-        <f t="shared" si="38"/>
-        <v>1.2006293671756474</v>
-      </c>
-      <c r="AO7" s="10">
-        <f t="shared" si="14"/>
-        <v>101339.68659882821</v>
-      </c>
-      <c r="AP7" s="15">
-        <f t="shared" si="15"/>
         <v>294.03629396111626</v>
       </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D8" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
       <c r="E8" s="11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="20"/>
         <v>0.6</v>
       </c>
       <c r="F8" s="15">
-        <f t="shared" si="16"/>
+        <f>F7 + M7*($B$2) + (0.5)*(R7)*($B$2)^2</f>
         <v>-9.3657488337764501E-21</v>
       </c>
-      <c r="G8" s="13">
-        <f t="shared" si="17"/>
+      <c r="G8" s="18">
+        <f xml:space="preserve"> G7 + N7*($B$2) + (0.5)*(S7)*($B$2)^2</f>
+        <v>-1.7603060852948271</v>
+      </c>
+      <c r="H8" s="13">
+        <f xml:space="preserve"> (F8/1000)</f>
         <v>-9.3657488337764501E-24</v>
       </c>
-      <c r="H8" s="18">
-        <f t="shared" si="18"/>
-        <v>-1.7603060852948271</v>
-      </c>
       <c r="I8" s="13">
-        <f t="shared" si="19"/>
+        <f>G8/1000</f>
         <v>-1.7603060852948271E-3</v>
       </c>
       <c r="J8" s="15">
-        <f t="shared" si="20"/>
+        <f>J7 + SQRT( (F8-F7)^2 + (G8-G7)^2 )</f>
         <v>1.7603060852948271</v>
       </c>
       <c r="K8" s="41">
+        <f>SQRT((F8)^2 + (G8+$B$23)^2)</f>
+        <v>6378135.2396939145</v>
+      </c>
+      <c r="L8" s="14">
+        <f>SQRT(F8^2 + G8^2)</f>
+        <v>1.7603060852948271</v>
+      </c>
+      <c r="M8" s="15">
         <f t="shared" si="21"/>
-        <v>6378135.2396939145</v>
-      </c>
-      <c r="L8" s="14">
+        <v>-6.6464458280041217E-20</v>
+      </c>
+      <c r="N8" s="15">
         <f t="shared" si="22"/>
-        <v>1.7603060852948271</v>
-      </c>
-      <c r="M8" s="15">
-        <f t="shared" si="35"/>
-        <v>-6.6464458280041217E-20</v>
-      </c>
-      <c r="N8" s="15">
-        <f t="shared" si="36"/>
         <v>-5.8671120274364359</v>
       </c>
       <c r="O8" s="15">
+        <f t="shared" si="10"/>
+        <v>5.8671120274364359</v>
+      </c>
+      <c r="P8" s="15">
         <f t="shared" si="23"/>
-        <v>5.8671120274364359</v>
-      </c>
-      <c r="P8" s="15">
-        <f t="shared" si="37"/>
         <v>-1.5707963267948966</v>
       </c>
       <c r="Q8" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>-90</v>
       </c>
       <c r="R8" s="15">
@@ -3187,15 +3187,15 @@
         <v>-4.3498740518162381E-19</v>
       </c>
       <c r="S8" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="12"/>
         <v>-9.7732314574360792</v>
       </c>
       <c r="T8" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="13"/>
         <v>9.7732314574360792</v>
       </c>
       <c r="U8" s="15">
-        <f t="shared" si="27"/>
+        <f xml:space="preserve"> ATAN2($B$23+G8, F8)</f>
         <v>-1.4684149021314747E-27</v>
       </c>
       <c r="V8" s="15">
@@ -3203,83 +3203,83 @@
         <v>-2.5628674827544532E-29</v>
       </c>
       <c r="W8" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="14"/>
         <v>200</v>
       </c>
       <c r="X8" s="16">
+        <f xml:space="preserve"> IF(G8&lt;30000, O8/AM8, "")</f>
+        <v>1.724063660449425E-2</v>
+      </c>
+      <c r="Y8" s="15">
+        <f t="shared" si="15"/>
+        <v>0.35</v>
+      </c>
+      <c r="Z8" s="15">
         <f t="shared" si="2"/>
-        <v>1.724063660449425E-2</v>
-      </c>
-      <c r="Y8" s="15">
-        <f t="shared" si="29"/>
-        <v>0.35</v>
-      </c>
-      <c r="Z8" s="15">
+        <v>1.4201949740879496</v>
+      </c>
+      <c r="AA8" s="15">
         <f t="shared" si="3"/>
+        <v>-8.6997483908641955E-17</v>
+      </c>
+      <c r="AB8" s="15">
+        <f t="shared" si="4"/>
         <v>1.4201949740879496</v>
       </c>
-      <c r="AA8" s="15">
-        <f t="shared" si="4"/>
-        <v>-8.6997483908641955E-17</v>
-      </c>
-      <c r="AB8" s="15">
+      <c r="AC8" s="10">
+        <f>IF(E8 &gt;= $B$16, IF(E8 &lt; $B$17, B21, 0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD8" s="10">
         <f t="shared" si="5"/>
-        <v>1.4201949740879496</v>
-      </c>
-      <c r="AC8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AD8" s="10">
+      <c r="AF8" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AE8" s="10">
+        <v>1721.1501771244641</v>
+      </c>
+      <c r="AG8" s="10">
+        <f>($B$9)*AJ8*G8</f>
+        <v>1721.6378696795523</v>
+      </c>
+      <c r="AH8" s="10">
+        <f t="shared" si="16"/>
+        <v>3442.7880468040166</v>
+      </c>
+      <c r="AI8" s="10">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF8" s="10">
+        <v>586.71120274364364</v>
+      </c>
+      <c r="AJ8" s="15">
+        <f>IF(G8&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G8)+((6.26*10^(-13))*(G8)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
+        <v>-9.7803324323065191</v>
+      </c>
+      <c r="AK8" s="15">
+        <f t="shared" si="17"/>
+        <v>1.4361585891398667E-26</v>
+      </c>
+      <c r="AL8" s="15">
+        <f t="shared" si="18"/>
+        <v>-9.7803324323065191</v>
+      </c>
+      <c r="AM8" s="15">
+        <f>IF(G8&lt;100000, IF(G8&gt;10000, (343.2)+(-4.313943*G8)+(-0.291943*G8^2)+(0.053721*G8^3)+((-3.039687*10^(-3))*G8^4)+((9.262166*10^(-5))*G8^5)+((-1.647967*10^(-6))*G8^6)+((1.694814*10^(-8))*G8^7)+((-9.299892*10^(-11))*G8^8)+((2.104694*10^(-13))*G8^9), ((-0.00406576*G8)+340.3)), 0)</f>
+        <v>340.30715698206939</v>
+      </c>
+      <c r="AN8" s="16">
+        <f t="shared" si="24"/>
+        <v>1.2006910437158671</v>
+      </c>
+      <c r="AO8" s="10">
+        <f>IF(G8&gt;38000,0,(101325*(1-(2.25577*10^(-5))*G8)^5.25588))</f>
+        <v>101346.14860652106</v>
+      </c>
+      <c r="AP8" s="15">
         <f t="shared" si="9"/>
-        <v>1721.1501771244641</v>
-      </c>
-      <c r="AG8" s="10">
-        <f t="shared" si="10"/>
-        <v>1721.6378696795523</v>
-      </c>
-      <c r="AH8" s="10">
-        <f t="shared" si="30"/>
-        <v>3442.7880468040166</v>
-      </c>
-      <c r="AI8" s="10">
-        <f t="shared" si="11"/>
-        <v>586.71120274364364</v>
-      </c>
-      <c r="AJ8" s="15">
-        <f t="shared" si="12"/>
-        <v>-9.7803324323065191</v>
-      </c>
-      <c r="AK8" s="15">
-        <f t="shared" si="31"/>
-        <v>1.4361585891398667E-26</v>
-      </c>
-      <c r="AL8" s="15">
-        <f t="shared" si="32"/>
-        <v>-9.7803324323065191</v>
-      </c>
-      <c r="AM8" s="15">
-        <f t="shared" si="13"/>
-        <v>340.30715698206939</v>
-      </c>
-      <c r="AN8" s="16">
-        <f t="shared" si="38"/>
-        <v>1.2006910437158671</v>
-      </c>
-      <c r="AO8" s="10">
-        <f t="shared" si="14"/>
-        <v>101346.14860652106</v>
-      </c>
-      <c r="AP8" s="15">
-        <f t="shared" si="15"/>
         <v>294.03993854201508</v>
       </c>
     </row>
@@ -3294,59 +3294,59 @@
         <v>22</v>
       </c>
       <c r="D9" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
       <c r="E9" s="11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="20"/>
         <v>0.7</v>
       </c>
       <c r="F9" s="15">
-        <f t="shared" si="16"/>
+        <f>F8 + M8*($B$2) + (0.5)*(R8)*($B$2)^2</f>
         <v>-1.8187131687688693E-20</v>
       </c>
-      <c r="G9" s="13">
-        <f t="shared" si="17"/>
+      <c r="G9" s="18">
+        <f xml:space="preserve"> G8 + N8*($B$2) + (0.5)*(S8)*($B$2)^2</f>
+        <v>-2.395883445325651</v>
+      </c>
+      <c r="H9" s="13">
+        <f xml:space="preserve"> (F9/1000)</f>
         <v>-1.8187131687688694E-23</v>
       </c>
-      <c r="H9" s="18">
-        <f t="shared" si="18"/>
-        <v>-2.395883445325651</v>
-      </c>
       <c r="I9" s="13">
-        <f t="shared" si="19"/>
+        <f>G9/1000</f>
         <v>-2.395883445325651E-3</v>
       </c>
       <c r="J9" s="15">
-        <f t="shared" si="20"/>
+        <f>J8 + SQRT( (F9-F8)^2 + (G9-G8)^2 )</f>
         <v>2.395883445325651</v>
       </c>
       <c r="K9" s="41">
+        <f>SQRT((F9)^2 + (G9+$B$23)^2)</f>
+        <v>6378134.6041165544</v>
+      </c>
+      <c r="L9" s="14">
+        <f>SQRT(F9^2 + G9^2)</f>
+        <v>2.395883445325651</v>
+      </c>
+      <c r="M9" s="15">
         <f t="shared" si="21"/>
-        <v>6378134.6041165544</v>
-      </c>
-      <c r="L9" s="14">
+        <v>-1.0996319879820359E-19</v>
+      </c>
+      <c r="N9" s="15">
         <f t="shared" si="22"/>
-        <v>2.395883445325651</v>
-      </c>
-      <c r="M9" s="15">
-        <f t="shared" si="35"/>
-        <v>-1.0996319879820359E-19</v>
-      </c>
-      <c r="N9" s="15">
-        <f t="shared" si="36"/>
         <v>-6.8444351731800435</v>
       </c>
       <c r="O9" s="15">
+        <f t="shared" si="10"/>
+        <v>6.8444351731800435</v>
+      </c>
+      <c r="P9" s="15">
         <f t="shared" si="23"/>
-        <v>6.8444351731800435</v>
-      </c>
-      <c r="P9" s="15">
-        <f t="shared" si="37"/>
         <v>-1.5707963267948966</v>
       </c>
       <c r="Q9" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>-90</v>
       </c>
       <c r="R9" s="15">
@@ -3354,15 +3354,15 @@
         <v>-5.9201063264844831E-19</v>
       </c>
       <c r="S9" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="12"/>
         <v>-9.7706700847230632</v>
       </c>
       <c r="T9" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="13"/>
         <v>9.7706700847230632</v>
       </c>
       <c r="U9" s="15">
-        <f t="shared" si="27"/>
+        <f xml:space="preserve"> ATAN2($B$23+G9, F9)</f>
         <v>-2.8514813211923144E-27</v>
       </c>
       <c r="V9" s="15">
@@ -3370,83 +3370,83 @@
         <v>-4.9767737613923847E-29</v>
       </c>
       <c r="W9" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="14"/>
         <v>200</v>
       </c>
       <c r="X9" s="16">
+        <f xml:space="preserve"> IF(G9&lt;30000, O9/AM9, "")</f>
+        <v>2.0112369253129092E-2</v>
+      </c>
+      <c r="Y9" s="15">
+        <f t="shared" si="15"/>
+        <v>0.35</v>
+      </c>
+      <c r="Z9" s="15">
         <f t="shared" si="2"/>
-        <v>2.0112369253129092E-2</v>
-      </c>
-      <c r="Y9" s="15">
-        <f t="shared" si="29"/>
-        <v>0.35</v>
-      </c>
-      <c r="Z9" s="15">
+        <v>1.932861795368449</v>
+      </c>
+      <c r="AA9" s="15">
         <f t="shared" si="3"/>
+        <v>-1.1840213210737784E-16</v>
+      </c>
+      <c r="AB9" s="15">
+        <f t="shared" si="4"/>
         <v>1.932861795368449</v>
       </c>
-      <c r="AA9" s="15">
-        <f t="shared" si="4"/>
-        <v>-1.1840213210737784E-16</v>
-      </c>
-      <c r="AB9" s="15">
+      <c r="AC9" s="10">
+        <f>IF(E9 &gt;= $B$16, IF(E9 &lt; $B$17, B22, 0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD9" s="10">
         <f t="shared" si="5"/>
-        <v>1.932861795368449</v>
-      </c>
-      <c r="AC9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AD9" s="10">
+      <c r="AF9" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AE9" s="10">
+        <v>2342.3146419932068</v>
+      </c>
+      <c r="AG9" s="10">
+        <f>($B$9)*AJ9*G9</f>
+        <v>2343.2541263614694</v>
+      </c>
+      <c r="AH9" s="10">
+        <f t="shared" si="16"/>
+        <v>4685.5687683546766</v>
+      </c>
+      <c r="AI9" s="10">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF9" s="10">
+        <v>684.4435173180043</v>
+      </c>
+      <c r="AJ9" s="15">
+        <f>IF(G9&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G9)+((6.26*10^(-13))*(G9)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
+        <v>-9.7803343936999063</v>
+      </c>
+      <c r="AK9" s="15">
+        <f t="shared" si="17"/>
+        <v>2.7888440838650042E-26</v>
+      </c>
+      <c r="AL9" s="15">
+        <f t="shared" si="18"/>
+        <v>-9.7803343936999063</v>
+      </c>
+      <c r="AM9" s="15">
+        <f>IF(G9&lt;100000, IF(G9&gt;10000, (343.2)+(-4.313943*G9)+(-0.291943*G9^2)+(0.053721*G9^3)+((-3.039687*10^(-3))*G9^4)+((9.262166*10^(-5))*G9^5)+((-1.647967*10^(-6))*G9^6)+((1.694814*10^(-8))*G9^7)+((-9.299892*10^(-11))*G9^8)+((2.104694*10^(-13))*G9^9), ((-0.00406576*G9)+340.3)), 0)</f>
+        <v>340.3097410870767</v>
+      </c>
+      <c r="AN9" s="16">
+        <f t="shared" si="24"/>
+        <v>1.2007639321500814</v>
+      </c>
+      <c r="AO9" s="10">
+        <f>IF(G9&gt;38000,0,(101325*(1-(2.25577*10^(-5))*G9)^5.25588))</f>
+        <v>101353.78541553953</v>
+      </c>
+      <c r="AP9" s="15">
         <f t="shared" si="9"/>
-        <v>2342.3146419932068</v>
-      </c>
-      <c r="AG9" s="10">
-        <f t="shared" si="10"/>
-        <v>2343.2541263614694</v>
-      </c>
-      <c r="AH9" s="10">
-        <f t="shared" si="30"/>
-        <v>4685.5687683546766</v>
-      </c>
-      <c r="AI9" s="10">
-        <f t="shared" si="11"/>
-        <v>684.4435173180043</v>
-      </c>
-      <c r="AJ9" s="15">
-        <f t="shared" si="12"/>
-        <v>-9.7803343936999063</v>
-      </c>
-      <c r="AK9" s="15">
-        <f t="shared" si="31"/>
-        <v>2.7888440838650042E-26</v>
-      </c>
-      <c r="AL9" s="15">
-        <f t="shared" si="32"/>
-        <v>-9.7803343936999063</v>
-      </c>
-      <c r="AM9" s="15">
-        <f t="shared" si="13"/>
-        <v>340.3097410870767</v>
-      </c>
-      <c r="AN9" s="16">
-        <f t="shared" si="38"/>
-        <v>1.2007639321500814</v>
-      </c>
-      <c r="AO9" s="10">
-        <f t="shared" si="14"/>
-        <v>101353.78541553953</v>
-      </c>
-      <c r="AP9" s="15">
-        <f t="shared" si="15"/>
         <v>294.0442454698308</v>
       </c>
     </row>
@@ -3461,59 +3461,59 @@
         <v>22</v>
       </c>
       <c r="D10" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
       <c r="E10" s="11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="20"/>
         <v>0.79999999999999993</v>
       </c>
       <c r="F10" s="15">
-        <f t="shared" si="16"/>
+        <f>F9 + M9*($B$2) + (0.5)*(R9)*($B$2)^2</f>
         <v>-3.21435047307513E-20</v>
       </c>
-      <c r="G10" s="13">
-        <f t="shared" si="17"/>
+      <c r="G10" s="18">
+        <f xml:space="preserve"> G9 + N9*($B$2) + (0.5)*(S9)*($B$2)^2</f>
+        <v>-3.1291803130672706</v>
+      </c>
+      <c r="H10" s="13">
+        <f xml:space="preserve"> (F10/1000)</f>
         <v>-3.2143504730751302E-23</v>
       </c>
-      <c r="H10" s="18">
-        <f t="shared" si="18"/>
-        <v>-3.1291803130672706</v>
-      </c>
       <c r="I10" s="13">
-        <f t="shared" si="19"/>
+        <f>G10/1000</f>
         <v>-3.1291803130672705E-3</v>
       </c>
       <c r="J10" s="15">
-        <f t="shared" si="20"/>
+        <f>J9 + SQRT( (F10-F9)^2 + (G10-G9)^2 )</f>
         <v>3.1291803130672706</v>
       </c>
       <c r="K10" s="41">
+        <f>SQRT((F10)^2 + (G10+$B$23)^2)</f>
+        <v>6378133.8708196869</v>
+      </c>
+      <c r="L10" s="14">
+        <f>SQRT(F10^2 + G10^2)</f>
+        <v>3.1291803130672706</v>
+      </c>
+      <c r="M10" s="15">
         <f t="shared" si="21"/>
-        <v>6378133.8708196869</v>
-      </c>
-      <c r="L10" s="14">
+        <v>-1.6916426206304844E-19</v>
+      </c>
+      <c r="N10" s="15">
         <f t="shared" si="22"/>
-        <v>3.1291803130672706</v>
-      </c>
-      <c r="M10" s="15">
-        <f t="shared" si="35"/>
-        <v>-1.6916426206304844E-19</v>
-      </c>
-      <c r="N10" s="15">
-        <f t="shared" si="36"/>
         <v>-7.8215021816523498</v>
       </c>
       <c r="O10" s="15">
+        <f t="shared" si="10"/>
+        <v>7.8215021816523498</v>
+      </c>
+      <c r="P10" s="15">
         <f t="shared" si="23"/>
-        <v>7.8215021816523498</v>
-      </c>
-      <c r="P10" s="15">
-        <f t="shared" si="37"/>
         <v>-1.5707963267948966</v>
       </c>
       <c r="Q10" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>-90</v>
       </c>
       <c r="R10" s="15">
@@ -3521,15 +3521,15 @@
         <v>-7.7315225756461974E-19</v>
       </c>
       <c r="S10" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="12"/>
         <v>-9.7677152914047767</v>
       </c>
       <c r="T10" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="13"/>
         <v>9.7677152914047767</v>
       </c>
       <c r="U10" s="15">
-        <f t="shared" si="27"/>
+        <f xml:space="preserve"> ATAN2($B$23+G10, F10)</f>
         <v>-5.0396409642340058E-27</v>
       </c>
       <c r="V10" s="15">
@@ -3537,83 +3537,83 @@
         <v>-8.7958327944265185E-29</v>
       </c>
       <c r="W10" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="14"/>
         <v>200</v>
       </c>
       <c r="X10" s="16">
+        <f xml:space="preserve"> IF(G10&lt;30000, O10/AM10, "")</f>
+        <v>2.2983278803926713E-2</v>
+      </c>
+      <c r="Y10" s="15">
+        <f t="shared" si="15"/>
+        <v>0.35</v>
+      </c>
+      <c r="Z10" s="15">
         <f t="shared" si="2"/>
-        <v>2.2983278803926713E-2</v>
-      </c>
-      <c r="Y10" s="15">
-        <f t="shared" si="29"/>
-        <v>0.35</v>
-      </c>
-      <c r="Z10" s="15">
+        <v>2.5242730503599971</v>
+      </c>
+      <c r="AA10" s="15">
         <f t="shared" si="3"/>
+        <v>-1.5463046137080098E-16</v>
+      </c>
+      <c r="AB10" s="15">
+        <f t="shared" si="4"/>
         <v>2.5242730503599971</v>
       </c>
-      <c r="AA10" s="15">
-        <f t="shared" si="4"/>
-        <v>-1.5463046137080098E-16</v>
-      </c>
-      <c r="AB10" s="15">
+      <c r="AC10" s="10">
+        <f>IF(E10 &gt;= $B$16, IF(E10 &lt; $B$17, B23, 0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD10" s="10">
         <f t="shared" si="5"/>
-        <v>2.5242730503599971</v>
-      </c>
-      <c r="AC10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AD10" s="10">
+      <c r="AF10" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AE10" s="10">
+        <v>3058.7948188796231</v>
+      </c>
+      <c r="AG10" s="10">
+        <f>($B$9)*AJ10*G10</f>
+        <v>3060.4436921179927</v>
+      </c>
+      <c r="AH10" s="10">
+        <f t="shared" si="16"/>
+        <v>6119.2385109976158</v>
+      </c>
+      <c r="AI10" s="10">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF10" s="10">
+        <v>782.15021816523495</v>
+      </c>
+      <c r="AJ10" s="15">
+        <f>IF(G10&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G10)+((6.26*10^(-13))*(G10)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
+        <v>-9.7803366566565764</v>
+      </c>
+      <c r="AK10" s="15">
+        <f t="shared" si="17"/>
+        <v>4.9289385258885939E-26</v>
+      </c>
+      <c r="AL10" s="15">
+        <f t="shared" si="18"/>
+        <v>-9.7803366566565764</v>
+      </c>
+      <c r="AM10" s="15">
+        <f>IF(G10&lt;100000, IF(G10&gt;10000, (343.2)+(-4.313943*G10)+(-0.291943*G10^2)+(0.053721*G10^3)+((-3.039687*10^(-3))*G10^4)+((9.262166*10^(-5))*G10^5)+((-1.647967*10^(-6))*G10^6)+((1.694814*10^(-8))*G10^7)+((-9.299892*10^(-11))*G10^8)+((2.104694*10^(-13))*G10^9), ((-0.00406576*G10)+340.3)), 0)</f>
+        <v>340.31272249614966</v>
+      </c>
+      <c r="AN10" s="16">
+        <f t="shared" si="24"/>
+        <v>1.2008480313282641</v>
+      </c>
+      <c r="AO10" s="10">
+        <f>IF(G10&gt;38000,0,(101325*(1-(2.25577*10^(-5))*G10)^5.25588))</f>
+        <v>101362.59695673757</v>
+      </c>
+      <c r="AP10" s="15">
         <f t="shared" si="9"/>
-        <v>3058.7948188796231</v>
-      </c>
-      <c r="AG10" s="10">
-        <f t="shared" si="10"/>
-        <v>3060.4436921179927</v>
-      </c>
-      <c r="AH10" s="10">
-        <f t="shared" si="30"/>
-        <v>6119.2385109976158</v>
-      </c>
-      <c r="AI10" s="10">
-        <f t="shared" si="11"/>
-        <v>782.15021816523495</v>
-      </c>
-      <c r="AJ10" s="15">
-        <f t="shared" si="12"/>
-        <v>-9.7803366566565764</v>
-      </c>
-      <c r="AK10" s="15">
-        <f t="shared" si="31"/>
-        <v>4.9289385258885939E-26</v>
-      </c>
-      <c r="AL10" s="15">
-        <f t="shared" si="32"/>
-        <v>-9.7803366566565764</v>
-      </c>
-      <c r="AM10" s="15">
-        <f t="shared" si="13"/>
-        <v>340.31272249614966</v>
-      </c>
-      <c r="AN10" s="16">
-        <f t="shared" si="38"/>
-        <v>1.2008480313282641</v>
-      </c>
-      <c r="AO10" s="10">
-        <f t="shared" si="14"/>
-        <v>101362.59695673757</v>
-      </c>
-      <c r="AP10" s="15">
-        <f t="shared" si="15"/>
         <v>294.04921458433273</v>
       </c>
     </row>
@@ -3628,59 +3628,59 @@
         <v>45</v>
       </c>
       <c r="D11" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="E11" s="11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="20"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="F11" s="15">
-        <f t="shared" si="16"/>
+        <f>F10 + M10*($B$2) + (0.5)*(R10)*($B$2)^2</f>
         <v>-5.2925692224879245E-20</v>
       </c>
-      <c r="G11" s="13">
-        <f t="shared" si="17"/>
+      <c r="G11" s="18">
+        <f xml:space="preserve"> G10 + N10*($B$2) + (0.5)*(S10)*($B$2)^2</f>
+        <v>-3.9601691076895293</v>
+      </c>
+      <c r="H11" s="13">
+        <f xml:space="preserve"> (F11/1000)</f>
         <v>-5.2925692224879247E-23</v>
       </c>
-      <c r="H11" s="18">
-        <f t="shared" si="18"/>
-        <v>-3.9601691076895293</v>
-      </c>
       <c r="I11" s="13">
-        <f t="shared" si="19"/>
+        <f>G11/1000</f>
         <v>-3.9601691076895295E-3</v>
       </c>
       <c r="J11" s="15">
-        <f t="shared" si="20"/>
+        <f>J10 + SQRT( (F11-F10)^2 + (G11-G10)^2 )</f>
         <v>3.9601691076895293</v>
       </c>
       <c r="K11" s="41">
+        <f>SQRT((F11)^2 + (G11+$B$23)^2)</f>
+        <v>6378133.0398308923</v>
+      </c>
+      <c r="L11" s="14">
+        <f>SQRT(F11^2 + G11^2)</f>
+        <v>3.9601691076895293</v>
+      </c>
+      <c r="M11" s="15">
         <f t="shared" si="21"/>
-        <v>6378133.0398308923</v>
-      </c>
-      <c r="L11" s="14">
+        <v>-2.4647948781951042E-19</v>
+      </c>
+      <c r="N11" s="15">
         <f t="shared" si="22"/>
-        <v>3.9601691076895293</v>
-      </c>
-      <c r="M11" s="15">
-        <f t="shared" si="35"/>
-        <v>-2.4647948781951042E-19</v>
-      </c>
-      <c r="N11" s="15">
-        <f t="shared" si="36"/>
         <v>-8.7982737107928273</v>
       </c>
       <c r="O11" s="15">
+        <f t="shared" si="10"/>
+        <v>8.7982737107928273</v>
+      </c>
+      <c r="P11" s="15">
         <f t="shared" si="23"/>
-        <v>8.7982737107928273</v>
-      </c>
-      <c r="P11" s="15">
-        <f t="shared" si="37"/>
         <v>-1.5707963267948966</v>
       </c>
       <c r="Q11" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>-90</v>
       </c>
       <c r="R11" s="15">
@@ -3688,15 +3688,15 @@
         <v>-9.7839468142257834E-19</v>
       </c>
       <c r="S11" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="12"/>
         <v>-9.7643673646418012</v>
       </c>
       <c r="T11" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="13"/>
         <v>9.7643673646418012</v>
       </c>
       <c r="U11" s="15">
-        <f t="shared" si="27"/>
+        <f xml:space="preserve"> ATAN2($B$23+G11, F11)</f>
         <v>-8.2979912608223828E-27</v>
       </c>
       <c r="V11" s="15">
@@ -3704,83 +3704,83 @@
         <v>-1.4482726880306613E-28</v>
       </c>
       <c r="W11" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="14"/>
         <v>200</v>
       </c>
       <c r="X11" s="16">
+        <f xml:space="preserve"> IF(G11&lt;30000, O11/AM11, "")</f>
+        <v>2.5853239627593026E-2</v>
+      </c>
+      <c r="Y11" s="15">
+        <f t="shared" si="15"/>
+        <v>0.35</v>
+      </c>
+      <c r="Z11" s="15">
         <f t="shared" si="2"/>
-        <v>2.5853239627593026E-2</v>
-      </c>
-      <c r="Y11" s="15">
-        <f t="shared" si="29"/>
-        <v>0.35</v>
-      </c>
-      <c r="Z11" s="15">
+        <v>3.1943712899763588</v>
+      </c>
+      <c r="AA11" s="15">
         <f t="shared" si="3"/>
+        <v>-1.9567895251594956E-16</v>
+      </c>
+      <c r="AB11" s="15">
+        <f t="shared" si="4"/>
         <v>3.1943712899763588</v>
       </c>
-      <c r="AA11" s="15">
-        <f t="shared" si="4"/>
-        <v>-1.9567895251594956E-16</v>
-      </c>
-      <c r="AB11" s="15">
+      <c r="AC11" s="10">
+        <f>IF(E11 &gt;= $B$16, IF(E11 &lt; $B$17, B24, 0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="10">
         <f t="shared" si="5"/>
-        <v>3.1943712899763588</v>
-      </c>
-      <c r="AC11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AD11" s="10">
+      <c r="AF11" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AE11" s="10">
+        <v>3870.4810145014094</v>
+      </c>
+      <c r="AG11" s="10">
+        <f>($B$9)*AJ11*G11</f>
+        <v>3873.1797246091555</v>
+      </c>
+      <c r="AH11" s="10">
+        <f t="shared" si="16"/>
+        <v>7743.6607391105645</v>
+      </c>
+      <c r="AI11" s="10">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF11" s="10">
+        <v>879.82737107928278</v>
+      </c>
+      <c r="AJ11" s="15">
+        <f>IF(G11&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G11)+((6.26*10^(-13))*(G11)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
+        <v>-9.7803392210916833</v>
+      </c>
+      <c r="AK11" s="15">
+        <f t="shared" si="17"/>
+        <v>8.1157169384497179E-26</v>
+      </c>
+      <c r="AL11" s="15">
+        <f t="shared" si="18"/>
+        <v>-9.7803392210916833</v>
+      </c>
+      <c r="AM11" s="15">
+        <f>IF(G11&lt;100000, IF(G11&gt;10000, (343.2)+(-4.313943*G11)+(-0.291943*G11^2)+(0.053721*G11^3)+((-3.039687*10^(-3))*G11^4)+((9.262166*10^(-5))*G11^5)+((-1.647967*10^(-6))*G11^6)+((1.694814*10^(-8))*G11^7)+((-9.299892*10^(-11))*G11^8)+((2.104694*10^(-13))*G11^9), ((-0.00406576*G11)+340.3)), 0)</f>
+        <v>340.31610109715132</v>
+      </c>
+      <c r="AN11" s="16">
+        <f t="shared" si="24"/>
+        <v>1.2009433398886522</v>
+      </c>
+      <c r="AO11" s="10">
+        <f>IF(G11&gt;38000,0,(101325*(1-(2.25577*10^(-5))*G11)^5.25588))</f>
+        <v>101372.58314666818</v>
+      </c>
+      <c r="AP11" s="15">
         <f t="shared" si="9"/>
-        <v>3870.4810145014094</v>
-      </c>
-      <c r="AG11" s="10">
-        <f t="shared" si="10"/>
-        <v>3873.1797246091555</v>
-      </c>
-      <c r="AH11" s="10">
-        <f t="shared" si="30"/>
-        <v>7743.6607391105645</v>
-      </c>
-      <c r="AI11" s="10">
-        <f t="shared" si="11"/>
-        <v>879.82737107928278</v>
-      </c>
-      <c r="AJ11" s="15">
-        <f t="shared" si="12"/>
-        <v>-9.7803392210916833</v>
-      </c>
-      <c r="AK11" s="15">
-        <f t="shared" si="31"/>
-        <v>8.1157169384497179E-26</v>
-      </c>
-      <c r="AL11" s="15">
-        <f t="shared" si="32"/>
-        <v>-9.7803392210916833</v>
-      </c>
-      <c r="AM11" s="15">
-        <f t="shared" si="13"/>
-        <v>340.31610109715132</v>
-      </c>
-      <c r="AN11" s="16">
-        <f t="shared" si="38"/>
-        <v>1.2009433398886522</v>
-      </c>
-      <c r="AO11" s="10">
-        <f t="shared" si="14"/>
-        <v>101372.58314666818</v>
-      </c>
-      <c r="AP11" s="15">
-        <f t="shared" si="15"/>
         <v>294.0548456986221</v>
       </c>
     </row>
@@ -3795,59 +3795,59 @@
         <v>5</v>
       </c>
       <c r="D12" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
       <c r="E12" s="11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="20"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="F12" s="15">
-        <f t="shared" si="16"/>
+        <f>F11 + M11*($B$2) + (0.5)*(R11)*($B$2)^2</f>
         <v>-8.2465614413943178E-20</v>
       </c>
-      <c r="G12" s="13">
-        <f t="shared" si="17"/>
+      <c r="G12" s="18">
+        <f xml:space="preserve"> G11 + N11*($B$2) + (0.5)*(S11)*($B$2)^2</f>
+        <v>-4.8888183155920215</v>
+      </c>
+      <c r="H12" s="13">
+        <f xml:space="preserve"> (F12/1000)</f>
         <v>-8.2465614413943177E-23</v>
       </c>
-      <c r="H12" s="18">
-        <f t="shared" si="18"/>
-        <v>-4.8888183155920215</v>
-      </c>
       <c r="I12" s="13">
-        <f t="shared" si="19"/>
+        <f>G12/1000</f>
         <v>-4.8888183155920218E-3</v>
       </c>
       <c r="J12" s="15">
-        <f t="shared" si="20"/>
+        <f>J11 + SQRT( (F12-F11)^2 + (G12-G11)^2 )</f>
         <v>4.8888183155920215</v>
       </c>
       <c r="K12" s="41">
+        <f>SQRT((F12)^2 + (G12+$B$23)^2)</f>
+        <v>6378132.1111816848</v>
+      </c>
+      <c r="L12" s="14">
+        <f>SQRT(F12^2 + G12^2)</f>
+        <v>4.8888183155920215</v>
+      </c>
+      <c r="M12" s="15">
         <f t="shared" si="21"/>
-        <v>6378132.1111816848</v>
-      </c>
-      <c r="L12" s="14">
+        <v>-3.4431895596176826E-19</v>
+      </c>
+      <c r="N12" s="15">
         <f t="shared" si="22"/>
-        <v>4.8888183155920215</v>
-      </c>
-      <c r="M12" s="15">
-        <f t="shared" si="35"/>
-        <v>-3.4431895596176826E-19</v>
-      </c>
-      <c r="N12" s="15">
-        <f t="shared" si="36"/>
         <v>-9.7747104472570072</v>
       </c>
       <c r="O12" s="15">
+        <f t="shared" si="10"/>
+        <v>9.7747104472570072</v>
+      </c>
+      <c r="P12" s="15">
         <f t="shared" si="23"/>
-        <v>9.7747104472570072</v>
-      </c>
-      <c r="P12" s="15">
-        <f t="shared" si="37"/>
         <v>-1.5707963267948966</v>
       </c>
       <c r="Q12" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>-90</v>
       </c>
       <c r="R12" s="15">
@@ -3855,15 +3855,15 @@
         <v>-1.2077177709807872E-18</v>
       </c>
       <c r="S12" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="12"/>
         <v>-9.76062663295499</v>
       </c>
       <c r="T12" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="13"/>
         <v>9.76062663295499</v>
       </c>
       <c r="U12" s="15">
-        <f t="shared" si="27"/>
+        <f xml:space="preserve"> ATAN2($B$23+G12, F12)</f>
         <v>-1.292943027463642E-26</v>
       </c>
       <c r="V12" s="15">
@@ -3871,83 +3871,83 @@
         <v>-2.2566112869944024E-28</v>
       </c>
       <c r="W12" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="14"/>
         <v>200</v>
       </c>
       <c r="X12" s="16">
+        <f xml:space="preserve"> IF(G12&lt;30000, O12/AM12, "")</f>
+        <v>2.8722126195685514E-2</v>
+      </c>
+      <c r="Y12" s="15">
+        <f t="shared" si="15"/>
+        <v>0.35</v>
+      </c>
+      <c r="Z12" s="15">
         <f t="shared" si="2"/>
-        <v>2.8722126195685514E-2</v>
-      </c>
-      <c r="Y12" s="15">
-        <f t="shared" si="29"/>
-        <v>0.35</v>
-      </c>
-      <c r="Z12" s="15">
+        <v>3.9430907906588941</v>
+      </c>
+      <c r="AA12" s="15">
         <f t="shared" si="3"/>
+        <v>-2.4154357948700767E-16</v>
+      </c>
+      <c r="AB12" s="15">
+        <f t="shared" si="4"/>
         <v>3.9430907906588941</v>
       </c>
-      <c r="AA12" s="15">
-        <f t="shared" si="4"/>
-        <v>-2.4154357948700767E-16</v>
-      </c>
-      <c r="AB12" s="15">
+      <c r="AC12" s="10">
+        <f>IF(E12 &gt;= $B$16, IF(E12 &lt; $B$17, B25, 0), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD12" s="10">
         <f t="shared" si="5"/>
-        <v>3.9430907906588941</v>
-      </c>
-      <c r="AC12" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AD12" s="10">
+      <c r="AF12" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AE12" s="10">
+        <v>4777.248216385764</v>
+      </c>
+      <c r="AG12" s="10">
+        <f>($B$9)*AJ12*G12</f>
+        <v>4781.431552723272</v>
+      </c>
+      <c r="AH12" s="10">
+        <f t="shared" si="16"/>
+        <v>9558.679769109036</v>
+      </c>
+      <c r="AI12" s="10">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF12" s="10">
+        <v>977.47104472570072</v>
+      </c>
+      <c r="AJ12" s="15">
+        <f>IF(G12&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G12)+((6.26*10^(-13))*(G12)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
+        <v>-9.7803420869082842</v>
+      </c>
+      <c r="AK12" s="15">
+        <f t="shared" si="17"/>
+        <v>1.2645425107477272E-25</v>
+      </c>
+      <c r="AL12" s="15">
+        <f t="shared" si="18"/>
+        <v>-9.7803420869082842</v>
+      </c>
+      <c r="AM12" s="15">
+        <f>IF(G12&lt;100000, IF(G12&gt;10000, (343.2)+(-4.313943*G12)+(-0.291943*G12^2)+(0.053721*G12^3)+((-3.039687*10^(-3))*G12^4)+((9.262166*10^(-5))*G12^5)+((-1.647967*10^(-6))*G12^6)+((1.694814*10^(-8))*G12^7)+((-9.299892*10^(-11))*G12^8)+((2.104694*10^(-13))*G12^9), ((-0.00406576*G12)+340.3)), 0)</f>
+        <v>340.31987676195479</v>
+      </c>
+      <c r="AN12" s="16">
+        <f t="shared" si="24"/>
+        <v>1.2010498562577365</v>
+      </c>
+      <c r="AO12" s="10">
+        <f>IF(G12&gt;38000,0,(101325*(1-(2.25577*10^(-5))*G12)^5.25588))</f>
+        <v>101383.74388757549</v>
+      </c>
+      <c r="AP12" s="15">
         <f t="shared" si="9"/>
-        <v>4777.248216385764</v>
-      </c>
-      <c r="AG12" s="10">
-        <f t="shared" si="10"/>
-        <v>4781.431552723272</v>
-      </c>
-      <c r="AH12" s="10">
-        <f t="shared" si="30"/>
-        <v>9558.679769109036</v>
-      </c>
-      <c r="AI12" s="10">
-        <f t="shared" si="11"/>
-        <v>977.47104472570072</v>
-      </c>
-      <c r="AJ12" s="15">
-        <f t="shared" si="12"/>
-        <v>-9.7803420869082842</v>
-      </c>
-      <c r="AK12" s="15">
-        <f t="shared" si="31"/>
-        <v>1.2645425107477272E-25</v>
-      </c>
-      <c r="AL12" s="15">
-        <f t="shared" si="32"/>
-        <v>-9.7803420869082842</v>
-      </c>
-      <c r="AM12" s="15">
-        <f t="shared" si="13"/>
-        <v>340.31987676195479</v>
-      </c>
-      <c r="AN12" s="16">
-        <f t="shared" si="38"/>
-        <v>1.2010498562577365</v>
-      </c>
-      <c r="AO12" s="10">
-        <f t="shared" si="14"/>
-        <v>101383.74388757549</v>
-      </c>
-      <c r="AP12" s="15">
-        <f t="shared" si="15"/>
         <v>294.06113859915013</v>
       </c>
     </row>
@@ -36620,7 +36620,7 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H3:H400">
+  <conditionalFormatting sqref="H13:H400 G3:G12">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
fixed newtonian grgravity bug
</commit_message>
<xml_diff>
--- a/Aero210/dynamics_template.xlsx
+++ b/Aero210/dynamics_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -702,7 +702,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
   <si>
     <t>Constants</t>
   </si>
@@ -893,13 +893,7 @@
     <t>x (km)</t>
   </si>
   <si>
-    <t>6.67408*10^(-11)</t>
-  </si>
-  <si>
     <t>m3 kg-1 s2</t>
-  </si>
-  <si>
-    <t>5.972*10^24</t>
   </si>
   <si>
     <t>rAB</t>
@@ -1307,7 +1301,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1396,10 +1390,6 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1410,6 +1400,9 @@
     <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="6" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="104">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -2215,8 +2208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC2691"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AN15" sqref="AN15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2244,11 +2237,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55" s="35" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
       <c r="D1" s="28" t="s">
         <v>10</v>
       </c>
@@ -2259,13 +2252,13 @@
         <v>15</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H1" s="27" t="s">
         <v>62</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J1" s="27" t="s">
         <v>16</v>
@@ -2274,7 +2267,7 @@
         <v>57</v>
       </c>
       <c r="L1" s="27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M1" s="27" t="s">
         <v>12</v>
@@ -2292,50 +2285,50 @@
         <v>34</v>
       </c>
       <c r="R1" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="T1" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" s="27" t="s">
         <v>67</v>
-      </c>
-      <c r="S1" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="T1" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="U1" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="V1" s="27" t="s">
-        <v>69</v>
       </c>
       <c r="W1" s="37"/>
       <c r="X1" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z1" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA1" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB1" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC1" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD1" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="Y1" s="36" t="s">
+      <c r="AE1" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="Z1" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA1" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB1" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC1" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD1" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE1" s="36" t="s">
-        <v>79</v>
-      </c>
       <c r="AF1" s="36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AG1" s="36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AH1" s="37"/>
       <c r="AI1" s="30" t="s">
@@ -2410,17 +2403,17 @@
       <c r="C2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="46">
+      <c r="D2" s="44">
         <v>0</v>
       </c>
-      <c r="E2" s="47">
+      <c r="E2" s="45">
         <f xml:space="preserve"> 0</f>
         <v>0</v>
       </c>
-      <c r="F2" s="48">
+      <c r="F2" s="46">
         <v>0</v>
       </c>
-      <c r="G2" s="48">
+      <c r="G2" s="46">
         <v>0</v>
       </c>
       <c r="H2" s="24">
@@ -2435,174 +2428,174 @@
         <f xml:space="preserve"> 0</f>
         <v>0</v>
       </c>
-      <c r="K2" s="49">
+      <c r="K2" s="47">
         <f t="shared" ref="K2:K12" si="2">SQRT((F2)^2 + (G2+$B$23)^2)</f>
         <v>6378137</v>
       </c>
-      <c r="L2" s="50">
+      <c r="L2" s="48">
         <f t="shared" ref="L2:L12" si="3">SQRT(F2^2 + G2^2)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="51">
+      <c r="M2" s="49">
         <f>B3*COS(B5)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="51">
+      <c r="N2" s="49">
         <f>B3*SIN(B5)</f>
         <v>0</v>
       </c>
-      <c r="O2" s="51">
+      <c r="O2" s="49">
         <f>SQRT(M2^2 + N2^2)</f>
         <v>0</v>
       </c>
-      <c r="P2" s="51">
+      <c r="P2" s="49">
         <f t="shared" ref="P2:P12" si="4" xml:space="preserve"> ((AM2+AP2)/(AI2)) + AX2</f>
         <v>0</v>
       </c>
-      <c r="Q2" s="51">
+      <c r="Q2" s="49">
         <f t="shared" ref="Q2:Q12" si="5" xml:space="preserve"> ((AN2+AQ2)/(AI2)) + AY2</f>
         <v>-9.7803269999999998</v>
       </c>
-      <c r="R2" s="51">
+      <c r="R2" s="49">
         <f>SQRT((P2^2)+(Q2^2))</f>
         <v>9.7803269999999998</v>
       </c>
-      <c r="S2" s="51">
+      <c r="S2" s="49">
         <f xml:space="preserve"> T2 * (PI()/180)</f>
         <v>0</v>
       </c>
-      <c r="T2" s="51">
+      <c r="T2" s="49">
         <f xml:space="preserve"> $B$4</f>
         <v>0</v>
       </c>
-      <c r="U2" s="51">
+      <c r="U2" s="49">
         <f t="shared" ref="U2:U12" si="6" xml:space="preserve"> ATAN2($B$23+G2, F2)</f>
         <v>0</v>
       </c>
-      <c r="V2" s="51">
+      <c r="V2" s="49">
         <f t="shared" ref="V2:V12" si="7" xml:space="preserve"> U2 * (PI()/180)</f>
         <v>0</v>
       </c>
-      <c r="W2" s="52"/>
-      <c r="X2" s="50">
+      <c r="W2" s="50"/>
+      <c r="X2" s="48">
         <f xml:space="preserve"> 0</f>
         <v>0</v>
       </c>
-      <c r="Y2" s="49">
+      <c r="Y2" s="47">
         <f xml:space="preserve"> 0</f>
         <v>0</v>
       </c>
-      <c r="Z2" s="51">
+      <c r="Z2" s="49">
         <f xml:space="preserve"> X2</f>
         <v>0</v>
       </c>
-      <c r="AA2" s="46">
+      <c r="AA2" s="44">
         <f t="shared" ref="AA2:AA12" si="8">K2*AD2</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="51">
+      <c r="AB2" s="49">
         <f t="shared" ref="AB2:AB12" si="9" xml:space="preserve"> Y2 - (K2)*(AD2)^2</f>
         <v>0</v>
       </c>
-      <c r="AC2" s="51">
+      <c r="AC2" s="49">
         <f t="shared" ref="AC2:AC12" si="10" xml:space="preserve"> (K2)*(AE2) + (2)*(X2)*(AD2)</f>
         <v>0</v>
       </c>
-      <c r="AD2" s="51">
+      <c r="AD2" s="49">
         <f xml:space="preserve"> 0</f>
         <v>0</v>
       </c>
-      <c r="AE2" s="51">
+      <c r="AE2" s="49">
         <f xml:space="preserve"> 0</f>
         <v>0</v>
       </c>
-      <c r="AF2" s="51">
+      <c r="AF2" s="49">
         <f xml:space="preserve"> 0</f>
         <v>0</v>
       </c>
-      <c r="AG2" s="51">
+      <c r="AG2" s="49">
         <f xml:space="preserve"> 0</f>
         <v>0</v>
       </c>
-      <c r="AH2" s="52"/>
-      <c r="AI2" s="50">
+      <c r="AH2" s="50"/>
+      <c r="AI2" s="48">
         <f xml:space="preserve"> ($B$9+$B$10)</f>
         <v>200</v>
       </c>
-      <c r="AJ2" s="53">
+      <c r="AJ2" s="51">
         <f t="shared" ref="AJ2:AJ12" si="11" xml:space="preserve"> IF(G2&lt;30000, O2/AZ2, "")</f>
         <v>0</v>
       </c>
-      <c r="AK2" s="51">
+      <c r="AK2" s="49">
         <f>0.35</f>
         <v>0.35</v>
       </c>
-      <c r="AL2" s="51">
+      <c r="AL2" s="49">
         <f t="shared" ref="AL2:AL12" si="12">(0.5)*(BA2)*(O2^2)*(AK2)*($B$13)</f>
         <v>0</v>
       </c>
-      <c r="AM2" s="51">
+      <c r="AM2" s="49">
         <f t="shared" ref="AM2:AM12" si="13" xml:space="preserve"> - AL2*COS(S2)</f>
         <v>0</v>
       </c>
-      <c r="AN2" s="51">
+      <c r="AN2" s="49">
         <f t="shared" ref="AN2:AN12" si="14" xml:space="preserve"> - AL2*SIN(S2)</f>
         <v>0</v>
       </c>
-      <c r="AO2" s="46">
+      <c r="AO2" s="44">
         <f>IF(E2 &gt;= $B$16, IF(E2 &lt; $B$17, $B$15, 0), 0)</f>
         <v>0</v>
       </c>
-      <c r="AP2" s="46">
+      <c r="AP2" s="44">
         <f t="shared" ref="AP2:AP12" si="15" xml:space="preserve"> AO2*COS(S2)</f>
         <v>0</v>
       </c>
-      <c r="AQ2" s="46">
+      <c r="AQ2" s="44">
         <f t="shared" ref="AQ2:AQ12" si="16" xml:space="preserve"> AO2*SIN(S2)</f>
         <v>0</v>
       </c>
-      <c r="AR2" s="46">
+      <c r="AR2" s="44">
         <f t="shared" ref="AR2:AR12" si="17">(0.5)*($B$9)*(O2^2)</f>
         <v>0</v>
       </c>
-      <c r="AS2" s="46">
+      <c r="AS2" s="44">
         <f t="shared" ref="AS2:AS12" si="18">($B$9)*AW2*G2</f>
         <v>0</v>
       </c>
-      <c r="AT2" s="46">
+      <c r="AT2" s="44">
         <f t="shared" ref="AT2:AT12" si="19" xml:space="preserve"> ABS(AR2) + ABS(AS2)</f>
         <v>0</v>
       </c>
-      <c r="AU2" s="46">
+      <c r="AU2" s="44">
         <f t="shared" ref="AU2:AU12" si="20" xml:space="preserve"> ($B$9)*O2</f>
         <v>0</v>
       </c>
-      <c r="AV2" s="52"/>
-      <c r="AW2" s="51">
+      <c r="AV2" s="50"/>
+      <c r="AW2" s="49">
         <f>IF(G2&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G2)+((6.26*10^(-13))*(G2)^2))), ($B$25)*($B$20)*(K2)^(-2))</f>
         <v>-9.7803269999999998</v>
       </c>
-      <c r="AX2" s="51">
+      <c r="AX2" s="49">
         <f t="shared" ref="AX2:AX12" si="21" xml:space="preserve"> AW2*SIN(U2)</f>
         <v>0</v>
       </c>
-      <c r="AY2" s="51">
+      <c r="AY2" s="49">
         <f t="shared" ref="AY2:AY12" si="22" xml:space="preserve"> AW2*COS(U2)</f>
         <v>-9.7803269999999998</v>
       </c>
-      <c r="AZ2" s="51">
+      <c r="AZ2" s="49">
         <f t="shared" ref="AZ2:AZ12" si="23">IF(G2&lt;100000, IF(G2&gt;10000, (343.2)+(-4.313943*G2)+(-0.291943*G2^2)+(0.053721*G2^3)+((-3.039687*10^(-3))*G2^4)+((9.262166*10^(-5))*G2^5)+((-1.647967*10^(-6))*G2^6)+((1.694814*10^(-8))*G2^7)+((-9.299892*10^(-11))*G2^8)+((2.104694*10^(-13))*G2^9), ((-0.00406576*G2)+340.3)), 0)</f>
         <v>340.3</v>
       </c>
-      <c r="BA2" s="53">
+      <c r="BA2" s="51">
         <f t="shared" ref="BA2:BA12" si="24" xml:space="preserve"> BB2 / (287.058*BC2)</f>
         <v>1.2004891883138833</v>
       </c>
-      <c r="BB2" s="46">
+      <c r="BB2" s="44">
         <f t="shared" ref="BB2:BB12" si="25">IF(G2&gt;38000,0,(101325*(1-(2.25577*10^(-5))*G2)^5.25588))</f>
         <v>101325</v>
       </c>
-      <c r="BC2" s="51">
+      <c r="BC2" s="49">
         <f t="shared" ref="BC2:BC12" si="26">1.6667*AZ2-273.15</f>
         <v>294.02801000000011</v>
       </c>
@@ -2617,19 +2610,19 @@
       <c r="C3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="44">
         <f>D2 + 1</f>
         <v>1</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="45">
         <f xml:space="preserve"> E2 + $B$2</f>
         <v>0.1</v>
       </c>
-      <c r="F3" s="51">
+      <c r="F3" s="49">
         <f t="shared" ref="F3:F12" si="27">F2 + M2*($B$2) + (0.5)*(P2)*($B$2)^2</f>
         <v>0</v>
       </c>
-      <c r="G3" s="54">
+      <c r="G3" s="52">
         <f t="shared" ref="G3:G12" si="28" xml:space="preserve"> G2 + N2*($B$2) + (0.5)*(Q2)*($B$2)^2</f>
         <v>-4.8901635000000006E-2</v>
       </c>
@@ -2641,178 +2634,178 @@
         <f t="shared" si="1"/>
         <v>-4.8901635000000009E-5</v>
       </c>
-      <c r="J3" s="51">
+      <c r="J3" s="49">
         <f t="shared" ref="J3:J12" si="29">J2 + SQRT( (F3-F2)^2 + (G3-G2)^2 )</f>
         <v>4.8901635000000006E-2</v>
       </c>
-      <c r="K3" s="49">
+      <c r="K3" s="47">
         <f t="shared" si="2"/>
         <v>6378136.9510983648</v>
       </c>
-      <c r="L3" s="50">
+      <c r="L3" s="48">
         <f t="shared" si="3"/>
         <v>4.8901635000000006E-2</v>
       </c>
-      <c r="M3" s="51">
+      <c r="M3" s="49">
         <f t="shared" ref="M3:M12" si="30" xml:space="preserve"> M2 + P2*($B$2)</f>
         <v>0</v>
       </c>
-      <c r="N3" s="51">
+      <c r="N3" s="49">
         <f t="shared" ref="N3:N12" si="31">N2 + Q2*$B$2</f>
         <v>-0.97803269999999998</v>
       </c>
-      <c r="O3" s="51">
+      <c r="O3" s="49">
         <f t="shared" ref="O3:O12" si="32">SQRT(M3^2 + N3^2)</f>
         <v>0.97803269999999998</v>
       </c>
-      <c r="P3" s="51">
+      <c r="P3" s="49">
         <f t="shared" si="4"/>
         <v>-1.2085474226821971E-20</v>
       </c>
-      <c r="Q3" s="51">
+      <c r="Q3" s="49">
         <f t="shared" si="5"/>
         <v>-9.7801298609546308</v>
       </c>
-      <c r="R3" s="51">
+      <c r="R3" s="49">
         <f t="shared" ref="R3:R12" si="33">SQRT((P3^2)+(Q3^2))</f>
         <v>9.7801298609546308</v>
       </c>
-      <c r="S3" s="51">
+      <c r="S3" s="49">
         <f t="shared" ref="S3:S12" si="34">ATAN2(M3,N3)</f>
         <v>-1.5707963267948966</v>
       </c>
-      <c r="T3" s="51">
+      <c r="T3" s="49">
         <f t="shared" ref="T3:T12" si="35">S3*(180/PI())</f>
         <v>-90</v>
       </c>
-      <c r="U3" s="51">
+      <c r="U3" s="49">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="V3" s="51">
+      <c r="V3" s="49">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="W3" s="52"/>
-      <c r="X3" s="50">
+      <c r="W3" s="50"/>
+      <c r="X3" s="48">
         <f t="shared" ref="X3:X12" si="36" xml:space="preserve"> (K4-K2)/(2*$B$2)</f>
         <v>-0.9780277730897069</v>
       </c>
-      <c r="Y3" s="49">
+      <c r="Y3" s="47">
         <f t="shared" ref="Y3:Y11" si="37" xml:space="preserve"> (X4-X2)/(2*$B$2)</f>
         <v>-9.780154493637383</v>
       </c>
-      <c r="Z3" s="51">
+      <c r="Z3" s="49">
         <f t="shared" ref="Z3:Z12" si="38" xml:space="preserve"> X3</f>
         <v>-0.9780277730897069</v>
       </c>
-      <c r="AA3" s="46">
+      <c r="AA3" s="44">
         <f t="shared" si="8"/>
         <v>50093770.472900562</v>
       </c>
-      <c r="AB3" s="47">
+      <c r="AB3" s="45">
         <f t="shared" si="9"/>
         <v>-393435563.05084872</v>
       </c>
-      <c r="AC3" s="51">
+      <c r="AC3" s="49">
         <f t="shared" si="10"/>
         <v>-15.362824334727042</v>
       </c>
-      <c r="AD3" s="51">
+      <c r="AD3" s="49">
         <f t="shared" ref="AD3:AD12" si="39" xml:space="preserve"> (S2-S4)/(2*$B$2)</f>
         <v>7.8539816339744828</v>
       </c>
-      <c r="AE3" s="51">
+      <c r="AE3" s="49">
         <f t="shared" ref="AE3:AE11" si="40" xml:space="preserve"> (AD4-AD2)/(2*$B$2)</f>
         <v>0</v>
       </c>
-      <c r="AF3" s="51">
+      <c r="AF3" s="49">
         <f t="shared" ref="AF3:AF12" si="41" xml:space="preserve"> (U4-U2)/(2*$B$2)</f>
         <v>-4.7370707925609457E-29</v>
       </c>
-      <c r="AG3" s="51">
+      <c r="AG3" s="49">
         <f t="shared" ref="AG3:AG11" si="42" xml:space="preserve"> (AF4-AF2)/(2*$B$2)</f>
         <v>-1.6579690176860392E-27</v>
       </c>
-      <c r="AH3" s="52"/>
-      <c r="AI3" s="51">
+      <c r="AH3" s="50"/>
+      <c r="AI3" s="49">
         <f t="shared" ref="AI3:AI12" si="43">IF(AO2&gt;0, IF(AI2 &gt;( $B$9 + $B$11*$B$2), AI2 -( $B$11*$B$2), $B$9), AI2)</f>
         <v>200</v>
       </c>
-      <c r="AJ3" s="53">
+      <c r="AJ3" s="51">
         <f t="shared" si="11"/>
         <v>2.8740291759590825E-3</v>
       </c>
-      <c r="AK3" s="51">
+      <c r="AK3" s="49">
         <f t="shared" ref="AK3:AK12" si="44">0.35</f>
         <v>0.35</v>
       </c>
-      <c r="AL3" s="51">
+      <c r="AL3" s="49">
         <f t="shared" si="12"/>
         <v>3.9457991163114638E-2</v>
       </c>
-      <c r="AM3" s="51">
+      <c r="AM3" s="49">
         <f t="shared" si="13"/>
         <v>-2.417094845364394E-18</v>
       </c>
-      <c r="AN3" s="51">
+      <c r="AN3" s="49">
         <f t="shared" si="14"/>
         <v>3.9457991163114638E-2</v>
       </c>
-      <c r="AO3" s="46">
+      <c r="AO3" s="44">
         <f t="shared" ref="AO3:AO12" si="45">IF(E3 &gt;= $B$16, IF(E3 &lt; $B$17, $B$15, 0), 0)</f>
         <v>0</v>
       </c>
-      <c r="AP3" s="46">
+      <c r="AP3" s="44">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AQ3" s="46">
+      <c r="AQ3" s="44">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AR3" s="46">
+      <c r="AR3" s="44">
         <f t="shared" si="17"/>
         <v>47.827398113464497</v>
       </c>
-      <c r="AS3" s="46">
+      <c r="AS3" s="44">
         <f t="shared" si="18"/>
         <v>47.827398851441266</v>
       </c>
-      <c r="AT3" s="46">
+      <c r="AT3" s="44">
         <f t="shared" si="19"/>
         <v>95.654796964905756</v>
       </c>
-      <c r="AU3" s="46">
+      <c r="AU3" s="44">
         <f t="shared" si="20"/>
         <v>97.803269999999998</v>
       </c>
-      <c r="AV3" s="52"/>
-      <c r="AW3" s="51">
-        <f t="shared" ref="AW3:AW12" si="46">IF(G3&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G3)+((6.26*10^(-13))*(G3)^2))), (6.674*10^(-11))*(5.972*10^(24))*(1)^(-2))</f>
+      <c r="AV3" s="50"/>
+      <c r="AW3" s="49">
+        <f t="shared" ref="AW3:AW12" si="46">IF(G3&lt;10^6, (-(9.780327*(1+0.0053024*((SIN($B$7))^2) - (5.8*10^(-6))*(SIN(2*($B$7))^2)) - ((3.086*10^(-6))*G3)+((6.26*10^(-13))*(G3)^2))), ($B$25)*($B$20)*(K3)^(-2))</f>
         <v>-9.7803271509104466</v>
       </c>
-      <c r="AX3" s="51">
+      <c r="AX3" s="49">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AY3" s="51">
+      <c r="AY3" s="49">
         <f t="shared" si="22"/>
         <v>-9.7803271509104466</v>
       </c>
-      <c r="AZ3" s="51">
+      <c r="AZ3" s="49">
         <f t="shared" si="23"/>
         <v>340.30019882231153</v>
       </c>
-      <c r="BA3" s="53">
+      <c r="BA3" s="51">
         <f t="shared" si="24"/>
         <v>1.2004947955443879</v>
       </c>
-      <c r="BB3" s="46">
+      <c r="BB3" s="44">
         <f t="shared" si="25"/>
         <v>101325.58746401522</v>
       </c>
-      <c r="BC3" s="51">
+      <c r="BC3" s="49">
         <f t="shared" si="26"/>
         <v>294.02834137714672</v>
       </c>
@@ -2827,19 +2820,19 @@
       <c r="C4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="44">
         <f t="shared" ref="D4:D12" si="47">D3 + 1</f>
         <v>2</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="45">
         <f t="shared" ref="E4:E12" si="48" xml:space="preserve"> E3 + $B$2</f>
         <v>0.2</v>
       </c>
-      <c r="F4" s="51">
+      <c r="F4" s="49">
         <f t="shared" si="27"/>
         <v>-6.0427371134109869E-23</v>
       </c>
-      <c r="G4" s="54">
+      <c r="G4" s="52">
         <f t="shared" si="28"/>
         <v>-0.19560555430477317</v>
       </c>
@@ -2851,178 +2844,178 @@
         <f t="shared" si="1"/>
         <v>-1.9560555430477318E-4</v>
       </c>
-      <c r="J4" s="51">
+      <c r="J4" s="49">
         <f t="shared" si="29"/>
         <v>0.19560555430477317</v>
       </c>
-      <c r="K4" s="49">
+      <c r="K4" s="47">
         <f t="shared" si="2"/>
         <v>6378136.8043944454</v>
       </c>
-      <c r="L4" s="50">
+      <c r="L4" s="48">
         <f t="shared" si="3"/>
         <v>0.19560555430477317</v>
       </c>
-      <c r="M4" s="51">
+      <c r="M4" s="49">
         <f t="shared" si="30"/>
         <v>-1.2085474226821972E-21</v>
       </c>
-      <c r="N4" s="51">
+      <c r="N4" s="49">
         <f t="shared" si="31"/>
         <v>-1.9560456860954631</v>
       </c>
-      <c r="O4" s="51">
+      <c r="O4" s="49">
         <f t="shared" si="32"/>
         <v>1.9560456860954631</v>
       </c>
-      <c r="P4" s="51">
+      <c r="P4" s="49">
         <f t="shared" si="4"/>
         <v>-4.8341599774508962E-20</v>
       </c>
-      <c r="Q4" s="51">
+      <c r="Q4" s="49">
         <f t="shared" si="5"/>
         <v>-9.7795384486645478</v>
       </c>
-      <c r="R4" s="51">
+      <c r="R4" s="49">
         <f t="shared" si="33"/>
         <v>9.7795384486645478</v>
       </c>
-      <c r="S4" s="51">
+      <c r="S4" s="49">
         <f t="shared" si="34"/>
         <v>-1.5707963267948966</v>
       </c>
-      <c r="T4" s="51">
+      <c r="T4" s="49">
         <f t="shared" si="35"/>
         <v>-90</v>
       </c>
-      <c r="U4" s="51">
+      <c r="U4" s="49">
         <f t="shared" si="6"/>
         <v>-9.4741415851218922E-30</v>
       </c>
-      <c r="V4" s="51">
+      <c r="V4" s="49">
         <f t="shared" si="7"/>
         <v>-1.6535496446049164E-31</v>
       </c>
-      <c r="W4" s="52"/>
-      <c r="X4" s="50">
+      <c r="W4" s="50"/>
+      <c r="X4" s="48">
         <f t="shared" si="36"/>
         <v>-1.9560308987274766</v>
       </c>
-      <c r="Y4" s="49">
+      <c r="Y4" s="47">
         <f t="shared" si="37"/>
         <v>-9.7797355847433209</v>
       </c>
-      <c r="Z4" s="51">
+      <c r="Z4" s="49">
         <f t="shared" si="38"/>
         <v>-1.9560308987274766</v>
       </c>
-      <c r="AA4" s="46">
+      <c r="AA4" s="44">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AB4" s="51">
+      <c r="AB4" s="49">
         <f t="shared" si="9"/>
         <v>-9.7797355847433209</v>
       </c>
-      <c r="AC4" s="51">
+      <c r="AC4" s="49">
         <f t="shared" si="10"/>
         <v>-250468846.60345334</v>
       </c>
-      <c r="AD4" s="51">
+      <c r="AD4" s="49">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AE4" s="51">
+      <c r="AE4" s="49">
         <f t="shared" si="40"/>
         <v>-39.269908169872409</v>
       </c>
-      <c r="AF4" s="51">
+      <c r="AF4" s="49">
         <f t="shared" si="41"/>
         <v>-3.3159380353720786E-28</v>
       </c>
-      <c r="AG4" s="51">
+      <c r="AG4" s="49">
         <f t="shared" si="42"/>
         <v>-5.6844044599255765E-27</v>
       </c>
-      <c r="AH4" s="52"/>
-      <c r="AI4" s="51">
+      <c r="AH4" s="50"/>
+      <c r="AI4" s="49">
         <f t="shared" si="43"/>
         <v>200</v>
       </c>
-      <c r="AJ4" s="53">
+      <c r="AJ4" s="51">
         <f t="shared" si="11"/>
         <v>5.7479903461756972E-3</v>
       </c>
-      <c r="AK4" s="51">
+      <c r="AK4" s="49">
         <f t="shared" si="44"/>
         <v>0.35</v>
       </c>
-      <c r="AL4" s="51">
+      <c r="AL4" s="49">
         <f t="shared" si="12"/>
         <v>0.15783099484306926</v>
       </c>
-      <c r="AM4" s="51">
+      <c r="AM4" s="49">
         <f t="shared" si="13"/>
         <v>-9.6683199734338339E-18</v>
       </c>
-      <c r="AN4" s="51">
+      <c r="AN4" s="49">
         <f t="shared" si="14"/>
         <v>0.15783099484306926</v>
       </c>
-      <c r="AO4" s="46">
+      <c r="AO4" s="44">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="AP4" s="46">
+      <c r="AP4" s="44">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AQ4" s="46">
+      <c r="AQ4" s="44">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AR4" s="46">
+      <c r="AR4" s="44">
         <f t="shared" si="17"/>
         <v>191.30573630463357</v>
       </c>
-      <c r="AS4" s="46">
+      <c r="AS4" s="44">
         <f t="shared" si="18"/>
         <v>191.30864021920343</v>
       </c>
-      <c r="AT4" s="46">
+      <c r="AT4" s="44">
         <f t="shared" si="19"/>
         <v>382.614376523837</v>
       </c>
-      <c r="AU4" s="46">
+      <c r="AU4" s="44">
         <f t="shared" si="20"/>
         <v>195.60456860954631</v>
       </c>
-      <c r="AV4" s="52"/>
-      <c r="AW4" s="51">
+      <c r="AV4" s="50"/>
+      <c r="AW4" s="49">
         <f t="shared" si="46"/>
         <v>-9.7803276036387636</v>
       </c>
-      <c r="AX4" s="51">
+      <c r="AX4" s="49">
         <f t="shared" si="21"/>
         <v>9.2660208465749556E-29</v>
       </c>
-      <c r="AY4" s="51">
+      <c r="AY4" s="49">
         <f t="shared" si="22"/>
         <v>-9.7803276036387636</v>
       </c>
-      <c r="AZ4" s="51">
+      <c r="AZ4" s="49">
         <f t="shared" si="23"/>
         <v>340.30079528523851</v>
       </c>
-      <c r="BA4" s="53">
+      <c r="BA4" s="51">
         <f t="shared" si="24"/>
         <v>1.2005116172430963</v>
       </c>
-      <c r="BB4" s="46">
+      <c r="BB4" s="44">
         <f t="shared" si="25"/>
         <v>101327.34986076689</v>
       </c>
-      <c r="BC4" s="51">
+      <c r="BC4" s="49">
         <f t="shared" si="26"/>
         <v>294.0293355019071</v>
       </c>
@@ -3038,19 +3031,19 @@
       <c r="C5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="44">
         <f t="shared" si="47"/>
         <v>3</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="45">
         <f t="shared" si="48"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="F5" s="51">
+      <c r="F5" s="49">
         <f t="shared" si="27"/>
         <v>-4.2299011227487443E-22</v>
       </c>
-      <c r="G5" s="54">
+      <c r="G5" s="52">
         <f t="shared" si="28"/>
         <v>-0.44010781515764225</v>
       </c>
@@ -3062,178 +3055,178 @@
         <f t="shared" si="1"/>
         <v>-4.4010781515764225E-4</v>
       </c>
-      <c r="J5" s="51">
+      <c r="J5" s="49">
         <f t="shared" si="29"/>
         <v>0.44010781515764225</v>
       </c>
-      <c r="K5" s="49">
+      <c r="K5" s="47">
         <f t="shared" si="2"/>
         <v>6378136.559892185</v>
       </c>
-      <c r="L5" s="50">
+      <c r="L5" s="48">
         <f t="shared" si="3"/>
         <v>0.44010781515764225</v>
       </c>
-      <c r="M5" s="51">
+      <c r="M5" s="49">
         <f t="shared" si="30"/>
         <v>-6.0427074001330938E-21</v>
       </c>
-      <c r="N5" s="51">
+      <c r="N5" s="49">
         <f t="shared" si="31"/>
         <v>-2.933999530961918</v>
       </c>
-      <c r="O5" s="51">
+      <c r="O5" s="49">
         <f t="shared" si="32"/>
         <v>2.933999530961918</v>
       </c>
-      <c r="P5" s="51">
+      <c r="P5" s="49">
         <f t="shared" si="4"/>
         <v>-1.0876602346293774E-19</v>
       </c>
-      <c r="Q5" s="51">
+      <c r="Q5" s="49">
         <f t="shared" si="5"/>
         <v>-9.7785528015261995</v>
       </c>
-      <c r="R5" s="51">
+      <c r="R5" s="49">
         <f t="shared" si="33"/>
         <v>9.7785528015261995</v>
       </c>
-      <c r="S5" s="51">
+      <c r="S5" s="49">
         <f t="shared" si="34"/>
         <v>-1.5707963267948966</v>
       </c>
-      <c r="T5" s="51">
+      <c r="T5" s="49">
         <f t="shared" si="35"/>
         <v>-90</v>
       </c>
-      <c r="U5" s="51">
+      <c r="U5" s="49">
         <f t="shared" si="6"/>
         <v>-6.6318760707441573E-29</v>
       </c>
-      <c r="V5" s="51">
+      <c r="V5" s="49">
         <f t="shared" si="7"/>
         <v>-1.1574807301870994E-30</v>
       </c>
-      <c r="W5" s="52"/>
-      <c r="X5" s="50">
+      <c r="W5" s="50"/>
+      <c r="X5" s="48">
         <f t="shared" si="36"/>
         <v>-2.9339748900383711</v>
       </c>
-      <c r="Y5" s="49">
+      <c r="Y5" s="47">
         <f t="shared" si="37"/>
         <v>-9.7789470804855227</v>
       </c>
-      <c r="Z5" s="51">
+      <c r="Z5" s="49">
         <f t="shared" si="38"/>
         <v>-2.9339748900383711</v>
       </c>
-      <c r="AA5" s="46">
+      <c r="AA5" s="44">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AB5" s="51">
+      <c r="AB5" s="49">
         <f t="shared" si="9"/>
         <v>-9.7789470804855227</v>
       </c>
-      <c r="AC5" s="51">
+      <c r="AC5" s="49">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AD5" s="51">
+      <c r="AD5" s="49">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AE5" s="51">
+      <c r="AE5" s="49">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AF5" s="51">
+      <c r="AF5" s="49">
         <f t="shared" si="41"/>
         <v>-1.1842515999107248E-27</v>
       </c>
-      <c r="AG5" s="51">
+      <c r="AG5" s="49">
         <f t="shared" si="42"/>
         <v>-1.3263323271873791E-26</v>
       </c>
-      <c r="AH5" s="52"/>
-      <c r="AI5" s="51">
+      <c r="AH5" s="50"/>
+      <c r="AI5" s="49">
         <f t="shared" si="43"/>
         <v>200</v>
       </c>
-      <c r="AJ5" s="53">
+      <c r="AJ5" s="51">
         <f t="shared" si="11"/>
         <v>8.6217575769140398E-3</v>
       </c>
-      <c r="AK5" s="51">
+      <c r="AK5" s="49">
         <f t="shared" si="44"/>
         <v>0.35</v>
       </c>
-      <c r="AL5" s="51">
+      <c r="AL5" s="49">
         <f t="shared" si="12"/>
         <v>0.35511132932757777</v>
       </c>
-      <c r="AM5" s="51">
+      <c r="AM5" s="49">
         <f t="shared" si="13"/>
         <v>-2.1753204822311403E-17</v>
       </c>
-      <c r="AN5" s="51">
+      <c r="AN5" s="49">
         <f t="shared" si="14"/>
         <v>0.35511132932757777</v>
       </c>
-      <c r="AO5" s="46">
+      <c r="AO5" s="44">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="AP5" s="46">
+      <c r="AP5" s="44">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AQ5" s="46">
+      <c r="AQ5" s="44">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AR5" s="46">
+      <c r="AR5" s="44">
         <f t="shared" si="17"/>
         <v>430.41766238423776</v>
       </c>
-      <c r="AS5" s="46">
+      <c r="AS5" s="44">
         <f t="shared" si="18"/>
         <v>430.43989452397778</v>
       </c>
-      <c r="AT5" s="46">
+      <c r="AT5" s="44">
         <f t="shared" si="19"/>
         <v>860.85755690821554</v>
       </c>
-      <c r="AU5" s="46">
+      <c r="AU5" s="44">
         <f t="shared" si="20"/>
         <v>293.39995309619178</v>
       </c>
-      <c r="AV5" s="52"/>
-      <c r="AW5" s="51">
+      <c r="AV5" s="50"/>
+      <c r="AW5" s="49">
         <f t="shared" si="46"/>
         <v>-9.780328358172838</v>
       </c>
-      <c r="AX5" s="51">
+      <c r="AX5" s="49">
         <f t="shared" si="21"/>
         <v>6.4861925602586931E-28</v>
       </c>
-      <c r="AY5" s="51">
+      <c r="AY5" s="49">
         <f t="shared" si="22"/>
         <v>-9.780328358172838</v>
       </c>
-      <c r="AZ5" s="51">
+      <c r="AZ5" s="49">
         <f t="shared" si="23"/>
         <v>340.30178937275059</v>
       </c>
-      <c r="BA5" s="53">
+      <c r="BA5" s="51">
         <f t="shared" si="24"/>
         <v>1.2005396533185746</v>
       </c>
-      <c r="BB5" s="46">
+      <c r="BB5" s="44">
         <f t="shared" si="25"/>
         <v>101330.28719253176</v>
       </c>
-      <c r="BC5" s="51">
+      <c r="BC5" s="49">
         <f t="shared" si="26"/>
         <v>294.03099234756348</v>
       </c>
@@ -3248,19 +3241,19 @@
       <c r="C6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="44">
         <f t="shared" si="47"/>
         <v>4</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="45">
         <f t="shared" si="48"/>
         <v>0.4</v>
       </c>
-      <c r="F6" s="51">
+      <c r="F6" s="49">
         <f t="shared" si="27"/>
         <v>-1.5710909696028726E-21</v>
       </c>
-      <c r="G6" s="54">
+      <c r="G6" s="52">
         <f t="shared" si="28"/>
         <v>-0.782400532261465</v>
       </c>
@@ -3272,178 +3265,178 @@
         <f t="shared" si="1"/>
         <v>-7.8240053226146498E-4</v>
       </c>
-      <c r="J6" s="51">
+      <c r="J6" s="49">
         <f t="shared" si="29"/>
         <v>0.782400532261465</v>
       </c>
-      <c r="K6" s="49">
+      <c r="K6" s="47">
         <f t="shared" si="2"/>
         <v>6378136.2175994674</v>
       </c>
-      <c r="L6" s="50">
+      <c r="L6" s="48">
         <f t="shared" si="3"/>
         <v>0.782400532261465</v>
       </c>
-      <c r="M6" s="51">
+      <c r="M6" s="49">
         <f t="shared" si="30"/>
         <v>-1.6919309746426869E-20</v>
       </c>
-      <c r="N6" s="51">
+      <c r="N6" s="49">
         <f t="shared" si="31"/>
         <v>-3.9118548111145381</v>
       </c>
-      <c r="O6" s="51">
+      <c r="O6" s="49">
         <f t="shared" si="32"/>
         <v>3.9118548111145381</v>
       </c>
-      <c r="P6" s="51">
+      <c r="P6" s="49">
         <f t="shared" si="4"/>
         <v>-1.9335384882074849E-19</v>
       </c>
-      <c r="Q6" s="51">
+      <c r="Q6" s="49">
         <f t="shared" si="5"/>
         <v>-9.777172999435944</v>
       </c>
-      <c r="R6" s="51">
+      <c r="R6" s="49">
         <f t="shared" si="33"/>
         <v>9.777172999435944</v>
       </c>
-      <c r="S6" s="51">
+      <c r="S6" s="49">
         <f t="shared" si="34"/>
         <v>-1.5707963267948966</v>
       </c>
-      <c r="T6" s="51">
+      <c r="T6" s="49">
         <f t="shared" si="35"/>
         <v>-90</v>
       </c>
-      <c r="U6" s="51">
+      <c r="U6" s="49">
         <f t="shared" si="6"/>
         <v>-2.4632446156726684E-28</v>
       </c>
-      <c r="V6" s="51">
+      <c r="V6" s="49">
         <f t="shared" si="7"/>
         <v>-4.2991728825510383E-30</v>
       </c>
-      <c r="W6" s="52"/>
-      <c r="X6" s="50">
+      <c r="W6" s="50"/>
+      <c r="X6" s="48">
         <f t="shared" si="36"/>
         <v>-3.9118203148245811</v>
       </c>
-      <c r="Y6" s="49">
+      <c r="Y6" s="47">
         <f t="shared" si="37"/>
         <v>-9.7777643706649542</v>
       </c>
-      <c r="Z6" s="51">
+      <c r="Z6" s="49">
         <f t="shared" si="38"/>
         <v>-3.9118203148245811</v>
       </c>
-      <c r="AA6" s="46">
+      <c r="AA6" s="44">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AB6" s="51">
+      <c r="AB6" s="49">
         <f t="shared" si="9"/>
         <v>-9.7777643706649542</v>
       </c>
-      <c r="AC6" s="51">
+      <c r="AC6" s="49">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="51">
+      <c r="AD6" s="49">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AE6" s="51">
+      <c r="AE6" s="49">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AF6" s="51">
+      <c r="AF6" s="49">
         <f t="shared" si="41"/>
         <v>-2.9842584579119661E-27</v>
       </c>
-      <c r="AG6" s="51">
+      <c r="AG6" s="49">
         <f t="shared" si="42"/>
         <v>-2.463100301455157E-26</v>
       </c>
-      <c r="AH6" s="52"/>
-      <c r="AI6" s="51">
+      <c r="AH6" s="50"/>
+      <c r="AI6" s="49">
         <f t="shared" si="43"/>
         <v>200</v>
       </c>
-      <c r="AJ6" s="53">
+      <c r="AJ6" s="51">
         <f t="shared" si="11"/>
         <v>1.1495204949341125E-2</v>
       </c>
-      <c r="AK6" s="51">
+      <c r="AK6" s="49">
         <f t="shared" si="44"/>
         <v>0.35</v>
       </c>
-      <c r="AL6" s="51">
+      <c r="AL6" s="49">
         <f t="shared" si="12"/>
         <v>0.63128301049624069</v>
       </c>
-      <c r="AM6" s="51">
+      <c r="AM6" s="49">
         <f t="shared" si="13"/>
         <v>-3.8670770245976572E-17</v>
       </c>
-      <c r="AN6" s="51">
+      <c r="AN6" s="49">
         <f t="shared" si="14"/>
         <v>0.63128301049624069</v>
       </c>
-      <c r="AO6" s="46">
+      <c r="AO6" s="44">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="AP6" s="46">
+      <c r="AP6" s="44">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AQ6" s="46">
+      <c r="AQ6" s="44">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AR6" s="46">
+      <c r="AR6" s="44">
         <f t="shared" si="17"/>
         <v>765.13040316199795</v>
       </c>
-      <c r="AS6" s="46">
+      <c r="AS6" s="44">
         <f t="shared" si="18"/>
         <v>765.21349395882066</v>
       </c>
-      <c r="AT6" s="46">
+      <c r="AT6" s="44">
         <f t="shared" si="19"/>
         <v>1530.3438971208186</v>
       </c>
-      <c r="AU6" s="46">
+      <c r="AU6" s="44">
         <f t="shared" si="20"/>
         <v>391.18548111145384</v>
       </c>
-      <c r="AV6" s="52"/>
-      <c r="AW6" s="51">
+      <c r="AV6" s="50"/>
+      <c r="AW6" s="49">
         <f t="shared" si="46"/>
         <v>-9.7803294144884259</v>
       </c>
-      <c r="AX6" s="51">
+      <c r="AX6" s="49">
         <f t="shared" si="21"/>
         <v>2.4091343769743636E-27</v>
       </c>
-      <c r="AY6" s="51">
+      <c r="AY6" s="49">
         <f t="shared" si="22"/>
         <v>-9.7803294144884259</v>
       </c>
-      <c r="AZ6" s="51">
+      <c r="AZ6" s="49">
         <f t="shared" si="23"/>
         <v>340.30318105278803</v>
       </c>
-      <c r="BA6" s="53">
+      <c r="BA6" s="51">
         <f t="shared" si="24"/>
         <v>1.2005789034676997</v>
       </c>
-      <c r="BB6" s="46">
+      <c r="BB6" s="44">
         <f t="shared" si="25"/>
         <v>101334.39944731123</v>
       </c>
-      <c r="BC6" s="51">
+      <c r="BC6" s="49">
         <f t="shared" si="26"/>
         <v>294.03331186068181</v>
       </c>
@@ -3459,19 +3452,19 @@
       <c r="C7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="44">
         <f t="shared" si="47"/>
         <v>5</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="45">
         <f t="shared" si="48"/>
         <v>0.5</v>
       </c>
-      <c r="F7" s="51">
+      <c r="F7" s="49">
         <f t="shared" si="27"/>
         <v>-4.2297911883493018E-21</v>
       </c>
-      <c r="G7" s="54">
+      <c r="G7" s="52">
         <f t="shared" si="28"/>
         <v>-1.2224718783700985</v>
       </c>
@@ -3483,197 +3476,197 @@
         <f t="shared" si="1"/>
         <v>-1.2224718783700986E-3</v>
       </c>
-      <c r="J7" s="51">
+      <c r="J7" s="49">
         <f t="shared" si="29"/>
         <v>1.2224718783700985</v>
       </c>
-      <c r="K7" s="49">
+      <c r="K7" s="47">
         <f t="shared" si="2"/>
         <v>6378135.7775281221</v>
       </c>
-      <c r="L7" s="50">
+      <c r="L7" s="48">
         <f t="shared" si="3"/>
         <v>1.2224718783700985</v>
       </c>
-      <c r="M7" s="51">
+      <c r="M7" s="49">
         <f t="shared" si="30"/>
         <v>-3.625469462850172E-20</v>
       </c>
-      <c r="N7" s="51">
+      <c r="N7" s="49">
         <f t="shared" si="31"/>
         <v>-4.8895721110581327</v>
       </c>
-      <c r="O7" s="51">
+      <c r="O7" s="49">
         <f t="shared" si="32"/>
         <v>4.8895721110581327</v>
       </c>
-      <c r="P7" s="51">
+      <c r="P7" s="49">
         <f t="shared" si="4"/>
         <v>-3.0209763651539501E-19</v>
       </c>
-      <c r="Q7" s="51">
+      <c r="Q7" s="49">
         <f t="shared" si="5"/>
         <v>-9.77539916378303</v>
       </c>
-      <c r="R7" s="51">
+      <c r="R7" s="49">
         <f t="shared" si="33"/>
         <v>9.77539916378303</v>
       </c>
-      <c r="S7" s="51">
+      <c r="S7" s="49">
         <f t="shared" si="34"/>
         <v>-1.5707963267948966</v>
       </c>
-      <c r="T7" s="51">
+      <c r="T7" s="49">
         <f t="shared" si="35"/>
         <v>-90</v>
       </c>
-      <c r="U7" s="51">
+      <c r="U7" s="49">
         <f t="shared" si="6"/>
         <v>-6.6317045228983475E-28</v>
       </c>
-      <c r="V7" s="51">
+      <c r="V7" s="49">
         <f t="shared" si="7"/>
         <v>-1.1574507894397586E-29</v>
       </c>
-      <c r="W7" s="52"/>
-      <c r="X7" s="50">
+      <c r="W7" s="50"/>
+      <c r="X7" s="48">
         <f t="shared" si="36"/>
         <v>-4.8895277641713619</v>
       </c>
-      <c r="Y7" s="49">
+      <c r="Y7" s="47">
         <f t="shared" si="37"/>
         <v>-9.7761876182630658</v>
       </c>
-      <c r="Z7" s="51">
+      <c r="Z7" s="49">
         <f t="shared" si="38"/>
         <v>-4.8895277641713619</v>
       </c>
-      <c r="AA7" s="46">
+      <c r="AA7" s="44">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AB7" s="51">
+      <c r="AB7" s="49">
         <f t="shared" si="9"/>
         <v>-9.7761876182630658</v>
       </c>
-      <c r="AC7" s="51">
+      <c r="AC7" s="49">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AD7" s="51">
+      <c r="AD7" s="49">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AE7" s="51">
+      <c r="AE7" s="49">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AF7" s="51">
+      <c r="AF7" s="49">
         <f t="shared" si="41"/>
         <v>-6.1104522028210392E-27</v>
       </c>
-      <c r="AG7" s="51">
+      <c r="AG7" s="49">
         <f t="shared" si="42"/>
         <v>-3.978647943300216E-26</v>
       </c>
-      <c r="AH7" s="52"/>
-      <c r="AI7" s="51">
+      <c r="AH7" s="50"/>
+      <c r="AI7" s="49">
         <f t="shared" si="43"/>
         <v>200</v>
       </c>
-      <c r="AJ7" s="53">
+      <c r="AJ7" s="51">
         <f t="shared" si="11"/>
         <v>1.4368206573869148E-2</v>
       </c>
-      <c r="AK7" s="51">
+      <c r="AK7" s="49">
         <f t="shared" si="44"/>
         <v>0.35</v>
       </c>
-      <c r="AL7" s="51">
+      <c r="AL7" s="49">
         <f t="shared" si="12"/>
         <v>0.9863217532244416</v>
       </c>
-      <c r="AM7" s="51">
+      <c r="AM7" s="49">
         <f t="shared" si="13"/>
         <v>-6.0419528600284285E-17</v>
       </c>
-      <c r="AN7" s="51">
+      <c r="AN7" s="49">
         <f t="shared" si="14"/>
         <v>0.9863217532244416</v>
       </c>
-      <c r="AO7" s="46">
+      <c r="AO7" s="44">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="AP7" s="46">
+      <c r="AP7" s="44">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AQ7" s="46">
+      <c r="AQ7" s="44">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AR7" s="46">
+      <c r="AR7" s="44">
         <f t="shared" si="17"/>
         <v>1195.3957714618741</v>
       </c>
-      <c r="AS7" s="46">
+      <c r="AS7" s="44">
         <f t="shared" si="18"/>
         <v>1195.6179330599039</v>
       </c>
-      <c r="AT7" s="46">
+      <c r="AT7" s="44">
         <f t="shared" si="19"/>
         <v>2391.013704521778</v>
       </c>
-      <c r="AU7" s="46">
+      <c r="AU7" s="44">
         <f t="shared" si="20"/>
         <v>488.95721110581326</v>
       </c>
-      <c r="AV7" s="52"/>
-      <c r="AW7" s="51">
+      <c r="AV7" s="50"/>
+      <c r="AW7" s="49">
         <f t="shared" si="46"/>
         <v>-9.7803307725491528</v>
       </c>
-      <c r="AX7" s="51">
+      <c r="AX7" s="49">
         <f t="shared" si="21"/>
         <v>6.4860263819756101E-27</v>
       </c>
-      <c r="AY7" s="51">
+      <c r="AY7" s="49">
         <f t="shared" si="22"/>
         <v>-9.7803307725491528</v>
       </c>
-      <c r="AZ7" s="51">
+      <c r="AZ7" s="49">
         <f t="shared" si="23"/>
         <v>340.3049702772642</v>
       </c>
-      <c r="BA7" s="53">
+      <c r="BA7" s="51">
         <f t="shared" si="24"/>
         <v>1.2006293671756474</v>
       </c>
-      <c r="BB7" s="46">
+      <c r="BB7" s="44">
         <f t="shared" si="25"/>
         <v>101339.68659882821</v>
       </c>
-      <c r="BC7" s="51">
+      <c r="BC7" s="49">
         <f t="shared" si="26"/>
         <v>294.03629396111626</v>
       </c>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.2">
       <c r="B8" s="43"/>
-      <c r="D8" s="46">
+      <c r="D8" s="44">
         <f t="shared" si="47"/>
         <v>6</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="45">
         <f t="shared" si="48"/>
         <v>0.6</v>
       </c>
-      <c r="F8" s="51">
+      <c r="F8" s="49">
         <f t="shared" si="27"/>
         <v>-9.3657488337764501E-21</v>
       </c>
-      <c r="G8" s="54">
+      <c r="G8" s="52">
         <f t="shared" si="28"/>
         <v>-1.7603060852948271</v>
       </c>
@@ -3685,178 +3678,178 @@
         <f t="shared" si="1"/>
         <v>-1.7603060852948271E-3</v>
       </c>
-      <c r="J8" s="51">
+      <c r="J8" s="49">
         <f t="shared" si="29"/>
         <v>1.7603060852948271</v>
       </c>
-      <c r="K8" s="49">
+      <c r="K8" s="47">
         <f t="shared" si="2"/>
         <v>6378135.2396939145</v>
       </c>
-      <c r="L8" s="50">
+      <c r="L8" s="48">
         <f t="shared" si="3"/>
         <v>1.7603060852948271</v>
       </c>
-      <c r="M8" s="51">
+      <c r="M8" s="49">
         <f t="shared" si="30"/>
         <v>-6.6464458280041217E-20</v>
       </c>
-      <c r="N8" s="51">
+      <c r="N8" s="49">
         <f t="shared" si="31"/>
         <v>-5.8671120274364359</v>
       </c>
-      <c r="O8" s="51">
+      <c r="O8" s="49">
         <f t="shared" si="32"/>
         <v>5.8671120274364359</v>
       </c>
-      <c r="P8" s="51">
+      <c r="P8" s="49">
         <f t="shared" si="4"/>
         <v>-4.3498740518162381E-19</v>
       </c>
-      <c r="Q8" s="51">
+      <c r="Q8" s="49">
         <f t="shared" si="5"/>
         <v>-9.7732314574360792</v>
       </c>
-      <c r="R8" s="51">
+      <c r="R8" s="49">
         <f t="shared" si="33"/>
         <v>9.7732314574360792</v>
       </c>
-      <c r="S8" s="51">
+      <c r="S8" s="49">
         <f t="shared" si="34"/>
         <v>-1.5707963267948966</v>
       </c>
-      <c r="T8" s="51">
+      <c r="T8" s="49">
         <f t="shared" si="35"/>
         <v>-90</v>
       </c>
-      <c r="U8" s="51">
+      <c r="U8" s="49">
         <f t="shared" si="6"/>
         <v>-1.4684149021314747E-27</v>
       </c>
-      <c r="V8" s="51">
+      <c r="V8" s="49">
         <f t="shared" si="7"/>
         <v>-2.5628674827544532E-29</v>
       </c>
-      <c r="W8" s="52"/>
-      <c r="X8" s="50">
+      <c r="W8" s="50"/>
+      <c r="X8" s="48">
         <f t="shared" si="36"/>
         <v>-5.8670578384771943</v>
       </c>
-      <c r="Y8" s="49">
+      <c r="Y8" s="47">
         <f t="shared" si="37"/>
         <v>-9.7742168698459864</v>
       </c>
-      <c r="Z8" s="51">
+      <c r="Z8" s="49">
         <f t="shared" si="38"/>
         <v>-5.8670578384771943</v>
       </c>
-      <c r="AA8" s="46">
+      <c r="AA8" s="44">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AB8" s="51">
+      <c r="AB8" s="49">
         <f t="shared" si="9"/>
         <v>-9.7742168698459864</v>
       </c>
-      <c r="AC8" s="51">
+      <c r="AC8" s="49">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AD8" s="51">
+      <c r="AD8" s="49">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AE8" s="51">
+      <c r="AE8" s="49">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AF8" s="51">
+      <c r="AF8" s="49">
         <f t="shared" si="41"/>
         <v>-1.0941554344512399E-26</v>
       </c>
-      <c r="AG8" s="51">
+      <c r="AG8" s="49">
         <f t="shared" si="42"/>
         <v>-5.8728390538458076E-26</v>
       </c>
-      <c r="AH8" s="52"/>
-      <c r="AI8" s="51">
+      <c r="AH8" s="50"/>
+      <c r="AI8" s="49">
         <f t="shared" si="43"/>
         <v>200</v>
       </c>
-      <c r="AJ8" s="53">
+      <c r="AJ8" s="51">
         <f t="shared" si="11"/>
         <v>1.724063660449425E-2</v>
       </c>
-      <c r="AK8" s="51">
+      <c r="AK8" s="49">
         <f t="shared" si="44"/>
         <v>0.35</v>
       </c>
-      <c r="AL8" s="51">
+      <c r="AL8" s="49">
         <f t="shared" si="12"/>
         <v>1.4201949740879496</v>
       </c>
-      <c r="AM8" s="51">
+      <c r="AM8" s="49">
         <f t="shared" si="13"/>
         <v>-8.6997483908641955E-17</v>
       </c>
-      <c r="AN8" s="51">
+      <c r="AN8" s="49">
         <f t="shared" si="14"/>
         <v>1.4201949740879496</v>
       </c>
-      <c r="AO8" s="46">
+      <c r="AO8" s="44">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="AP8" s="46">
+      <c r="AP8" s="44">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AQ8" s="46">
+      <c r="AQ8" s="44">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AR8" s="46">
+      <c r="AR8" s="44">
         <f t="shared" si="17"/>
         <v>1721.1501771244641</v>
       </c>
-      <c r="AS8" s="46">
+      <c r="AS8" s="44">
         <f t="shared" si="18"/>
         <v>1721.6378696795523</v>
       </c>
-      <c r="AT8" s="46">
+      <c r="AT8" s="44">
         <f t="shared" si="19"/>
         <v>3442.7880468040166</v>
       </c>
-      <c r="AU8" s="46">
+      <c r="AU8" s="44">
         <f t="shared" si="20"/>
         <v>586.71120274364364</v>
       </c>
-      <c r="AV8" s="52"/>
-      <c r="AW8" s="51">
+      <c r="AV8" s="50"/>
+      <c r="AW8" s="49">
         <f t="shared" si="46"/>
         <v>-9.7803324323065191</v>
       </c>
-      <c r="AX8" s="51">
+      <c r="AX8" s="49">
         <f t="shared" si="21"/>
         <v>1.4361585891398667E-26</v>
       </c>
-      <c r="AY8" s="51">
+      <c r="AY8" s="49">
         <f t="shared" si="22"/>
         <v>-9.7803324323065191</v>
       </c>
-      <c r="AZ8" s="51">
+      <c r="AZ8" s="49">
         <f t="shared" si="23"/>
         <v>340.30715698206939</v>
       </c>
-      <c r="BA8" s="53">
+      <c r="BA8" s="51">
         <f t="shared" si="24"/>
         <v>1.2006910437158671</v>
       </c>
-      <c r="BB8" s="46">
+      <c r="BB8" s="44">
         <f t="shared" si="25"/>
         <v>101346.14860652106</v>
       </c>
-      <c r="BC8" s="51">
+      <c r="BC8" s="49">
         <f t="shared" si="26"/>
         <v>294.03993854201508</v>
       </c>
@@ -3871,19 +3864,19 @@
       <c r="C9" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="44">
         <f t="shared" si="47"/>
         <v>7</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="45">
         <f t="shared" si="48"/>
         <v>0.7</v>
       </c>
-      <c r="F9" s="51">
+      <c r="F9" s="49">
         <f t="shared" si="27"/>
         <v>-1.8187131687688693E-20</v>
       </c>
-      <c r="G9" s="54">
+      <c r="G9" s="52">
         <f t="shared" si="28"/>
         <v>-2.395883445325651</v>
       </c>
@@ -3895,178 +3888,178 @@
         <f t="shared" si="1"/>
         <v>-2.395883445325651E-3</v>
       </c>
-      <c r="J9" s="51">
+      <c r="J9" s="49">
         <f t="shared" si="29"/>
         <v>2.395883445325651</v>
       </c>
-      <c r="K9" s="49">
+      <c r="K9" s="47">
         <f t="shared" si="2"/>
         <v>6378134.6041165544</v>
       </c>
-      <c r="L9" s="50">
+      <c r="L9" s="48">
         <f t="shared" si="3"/>
         <v>2.395883445325651</v>
       </c>
-      <c r="M9" s="51">
+      <c r="M9" s="49">
         <f t="shared" si="30"/>
         <v>-1.0996319879820359E-19</v>
       </c>
-      <c r="N9" s="51">
+      <c r="N9" s="49">
         <f t="shared" si="31"/>
         <v>-6.8444351731800435</v>
       </c>
-      <c r="O9" s="51">
+      <c r="O9" s="49">
         <f t="shared" si="32"/>
         <v>6.8444351731800435</v>
       </c>
-      <c r="P9" s="51">
+      <c r="P9" s="49">
         <f t="shared" si="4"/>
         <v>-5.9201063264844831E-19</v>
       </c>
-      <c r="Q9" s="51">
+      <c r="Q9" s="49">
         <f t="shared" si="5"/>
         <v>-9.7706700847230632</v>
       </c>
-      <c r="R9" s="51">
+      <c r="R9" s="49">
         <f t="shared" si="33"/>
         <v>9.7706700847230632</v>
       </c>
-      <c r="S9" s="51">
+      <c r="S9" s="49">
         <f t="shared" si="34"/>
         <v>-1.5707963267948966</v>
       </c>
-      <c r="T9" s="51">
+      <c r="T9" s="49">
         <f t="shared" si="35"/>
         <v>-90</v>
       </c>
-      <c r="U9" s="51">
+      <c r="U9" s="49">
         <f t="shared" si="6"/>
         <v>-2.8514813211923144E-27</v>
       </c>
-      <c r="V9" s="51">
+      <c r="V9" s="49">
         <f t="shared" si="7"/>
         <v>-4.9767737613923847E-29</v>
       </c>
-      <c r="W9" s="52"/>
-      <c r="X9" s="50">
+      <c r="W9" s="50"/>
+      <c r="X9" s="48">
         <f t="shared" si="36"/>
         <v>-6.8443711381405592</v>
       </c>
-      <c r="Y9" s="49">
+      <c r="Y9" s="47">
         <f t="shared" si="37"/>
         <v>-9.7718523582443595</v>
       </c>
-      <c r="Z9" s="51">
+      <c r="Z9" s="49">
         <f t="shared" si="38"/>
         <v>-6.8443711381405592</v>
       </c>
-      <c r="AA9" s="46">
+      <c r="AA9" s="44">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AB9" s="51">
+      <c r="AB9" s="49">
         <f t="shared" si="9"/>
         <v>-9.7718523582443595</v>
       </c>
-      <c r="AC9" s="51">
+      <c r="AC9" s="49">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AD9" s="51">
+      <c r="AD9" s="49">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AE9" s="51">
+      <c r="AE9" s="49">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AF9" s="51">
+      <c r="AF9" s="49">
         <f t="shared" si="41"/>
         <v>-1.7856130310512655E-26</v>
       </c>
-      <c r="AG9" s="51">
+      <c r="AG9" s="49">
         <f t="shared" si="42"/>
         <v>-8.1454976768189708E-26</v>
       </c>
-      <c r="AH9" s="52"/>
-      <c r="AI9" s="51">
+      <c r="AH9" s="50"/>
+      <c r="AI9" s="49">
         <f t="shared" si="43"/>
         <v>200</v>
       </c>
-      <c r="AJ9" s="53">
+      <c r="AJ9" s="51">
         <f t="shared" si="11"/>
         <v>2.0112369253129092E-2</v>
       </c>
-      <c r="AK9" s="51">
+      <c r="AK9" s="49">
         <f t="shared" si="44"/>
         <v>0.35</v>
       </c>
-      <c r="AL9" s="51">
+      <c r="AL9" s="49">
         <f t="shared" si="12"/>
         <v>1.932861795368449</v>
       </c>
-      <c r="AM9" s="51">
+      <c r="AM9" s="49">
         <f t="shared" si="13"/>
         <v>-1.1840213210737784E-16</v>
       </c>
-      <c r="AN9" s="51">
+      <c r="AN9" s="49">
         <f t="shared" si="14"/>
         <v>1.932861795368449</v>
       </c>
-      <c r="AO9" s="46">
+      <c r="AO9" s="44">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="AP9" s="46">
+      <c r="AP9" s="44">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AQ9" s="46">
+      <c r="AQ9" s="44">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AR9" s="46">
+      <c r="AR9" s="44">
         <f t="shared" si="17"/>
         <v>2342.3146419932068</v>
       </c>
-      <c r="AS9" s="46">
+      <c r="AS9" s="44">
         <f t="shared" si="18"/>
         <v>2343.2541263614694</v>
       </c>
-      <c r="AT9" s="46">
+      <c r="AT9" s="44">
         <f t="shared" si="19"/>
         <v>4685.5687683546766</v>
       </c>
-      <c r="AU9" s="46">
+      <c r="AU9" s="44">
         <f t="shared" si="20"/>
         <v>684.4435173180043</v>
       </c>
-      <c r="AV9" s="52"/>
-      <c r="AW9" s="51">
+      <c r="AV9" s="50"/>
+      <c r="AW9" s="49">
         <f t="shared" si="46"/>
         <v>-9.7803343936999063</v>
       </c>
-      <c r="AX9" s="51">
+      <c r="AX9" s="49">
         <f t="shared" si="21"/>
         <v>2.7888440838650042E-26</v>
       </c>
-      <c r="AY9" s="51">
+      <c r="AY9" s="49">
         <f t="shared" si="22"/>
         <v>-9.7803343936999063</v>
       </c>
-      <c r="AZ9" s="51">
+      <c r="AZ9" s="49">
         <f t="shared" si="23"/>
         <v>340.3097410870767</v>
       </c>
-      <c r="BA9" s="53">
+      <c r="BA9" s="51">
         <f t="shared" si="24"/>
         <v>1.2007639321500814</v>
       </c>
-      <c r="BB9" s="46">
+      <c r="BB9" s="44">
         <f t="shared" si="25"/>
         <v>101353.78541553953</v>
       </c>
-      <c r="BC9" s="51">
+      <c r="BC9" s="49">
         <f t="shared" si="26"/>
         <v>294.0442454698308</v>
       </c>
@@ -4081,19 +4074,19 @@
       <c r="C10" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="44">
         <f t="shared" si="47"/>
         <v>8</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="45">
         <f t="shared" si="48"/>
         <v>0.79999999999999993</v>
       </c>
-      <c r="F10" s="51">
+      <c r="F10" s="49">
         <f t="shared" si="27"/>
         <v>-3.21435047307513E-20</v>
       </c>
-      <c r="G10" s="54">
+      <c r="G10" s="52">
         <f t="shared" si="28"/>
         <v>-3.1291803130672706</v>
       </c>
@@ -4105,178 +4098,178 @@
         <f t="shared" si="1"/>
         <v>-3.1291803130672705E-3</v>
       </c>
-      <c r="J10" s="51">
+      <c r="J10" s="49">
         <f t="shared" si="29"/>
         <v>3.1291803130672706</v>
       </c>
-      <c r="K10" s="49">
+      <c r="K10" s="47">
         <f t="shared" si="2"/>
         <v>6378133.8708196869</v>
       </c>
-      <c r="L10" s="50">
+      <c r="L10" s="48">
         <f t="shared" si="3"/>
         <v>3.1291803130672706</v>
       </c>
-      <c r="M10" s="51">
+      <c r="M10" s="49">
         <f t="shared" si="30"/>
         <v>-1.6916426206304844E-19</v>
       </c>
-      <c r="N10" s="51">
+      <c r="N10" s="49">
         <f t="shared" si="31"/>
         <v>-7.8215021816523498</v>
       </c>
-      <c r="O10" s="51">
+      <c r="O10" s="49">
         <f t="shared" si="32"/>
         <v>7.8215021816523498</v>
       </c>
-      <c r="P10" s="51">
+      <c r="P10" s="49">
         <f t="shared" si="4"/>
         <v>-7.7315225756461974E-19</v>
       </c>
-      <c r="Q10" s="51">
+      <c r="Q10" s="49">
         <f t="shared" si="5"/>
         <v>-9.7677152914047767</v>
       </c>
-      <c r="R10" s="51">
+      <c r="R10" s="49">
         <f t="shared" si="33"/>
         <v>9.7677152914047767</v>
       </c>
-      <c r="S10" s="51">
+      <c r="S10" s="49">
         <f t="shared" si="34"/>
         <v>-1.5707963267948966</v>
       </c>
-      <c r="T10" s="51">
+      <c r="T10" s="49">
         <f t="shared" si="35"/>
         <v>-90</v>
       </c>
-      <c r="U10" s="51">
+      <c r="U10" s="49">
         <f t="shared" si="6"/>
         <v>-5.0396409642340058E-27</v>
       </c>
-      <c r="V10" s="51">
+      <c r="V10" s="49">
         <f t="shared" si="7"/>
         <v>-8.7958327944265185E-29</v>
       </c>
-      <c r="W10" s="52"/>
-      <c r="X10" s="50">
+      <c r="W10" s="50"/>
+      <c r="X10" s="48">
         <f t="shared" si="36"/>
         <v>-7.8214283101260662</v>
       </c>
-      <c r="Y10" s="49">
+      <c r="Y10" s="47">
         <f t="shared" si="37"/>
         <v>-9.7690943628549576</v>
       </c>
-      <c r="Z10" s="51">
+      <c r="Z10" s="49">
         <f t="shared" si="38"/>
         <v>-7.8214283101260662</v>
       </c>
-      <c r="AA10" s="46">
+      <c r="AA10" s="44">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AB10" s="51">
+      <c r="AB10" s="49">
         <f t="shared" si="9"/>
         <v>-9.7690943628549576</v>
       </c>
-      <c r="AC10" s="51">
+      <c r="AC10" s="49">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AD10" s="51">
+      <c r="AD10" s="49">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AE10" s="51">
+      <c r="AE10" s="49">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AF10" s="51">
+      <c r="AF10" s="49">
         <f t="shared" si="41"/>
         <v>-2.7232549698150339E-26</v>
       </c>
-      <c r="AG10" s="51">
+      <c r="AG10" s="49">
         <f t="shared" si="42"/>
         <v>-1.0796408120749707E-25</v>
       </c>
-      <c r="AH10" s="52"/>
-      <c r="AI10" s="51">
+      <c r="AH10" s="50"/>
+      <c r="AI10" s="49">
         <f t="shared" si="43"/>
         <v>200</v>
       </c>
-      <c r="AJ10" s="53">
+      <c r="AJ10" s="51">
         <f t="shared" si="11"/>
         <v>2.2983278803926713E-2</v>
       </c>
-      <c r="AK10" s="51">
+      <c r="AK10" s="49">
         <f t="shared" si="44"/>
         <v>0.35</v>
       </c>
-      <c r="AL10" s="51">
+      <c r="AL10" s="49">
         <f t="shared" si="12"/>
         <v>2.5242730503599971</v>
       </c>
-      <c r="AM10" s="51">
+      <c r="AM10" s="49">
         <f t="shared" si="13"/>
         <v>-1.5463046137080098E-16</v>
       </c>
-      <c r="AN10" s="51">
+      <c r="AN10" s="49">
         <f t="shared" si="14"/>
         <v>2.5242730503599971</v>
       </c>
-      <c r="AO10" s="46">
+      <c r="AO10" s="44">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="AP10" s="46">
+      <c r="AP10" s="44">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AQ10" s="46">
+      <c r="AQ10" s="44">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AR10" s="46">
+      <c r="AR10" s="44">
         <f t="shared" si="17"/>
         <v>3058.7948188796231</v>
       </c>
-      <c r="AS10" s="46">
+      <c r="AS10" s="44">
         <f t="shared" si="18"/>
         <v>3060.4436921179927</v>
       </c>
-      <c r="AT10" s="46">
+      <c r="AT10" s="44">
         <f t="shared" si="19"/>
         <v>6119.2385109976158</v>
       </c>
-      <c r="AU10" s="46">
+      <c r="AU10" s="44">
         <f t="shared" si="20"/>
         <v>782.15021816523495</v>
       </c>
-      <c r="AV10" s="52"/>
-      <c r="AW10" s="51">
+      <c r="AV10" s="50"/>
+      <c r="AW10" s="49">
         <f t="shared" si="46"/>
         <v>-9.7803366566565764</v>
       </c>
-      <c r="AX10" s="51">
+      <c r="AX10" s="49">
         <f t="shared" si="21"/>
         <v>4.9289385258885939E-26</v>
       </c>
-      <c r="AY10" s="51">
+      <c r="AY10" s="49">
         <f t="shared" si="22"/>
         <v>-9.7803366566565764</v>
       </c>
-      <c r="AZ10" s="51">
+      <c r="AZ10" s="49">
         <f t="shared" si="23"/>
         <v>340.31272249614966</v>
       </c>
-      <c r="BA10" s="53">
+      <c r="BA10" s="51">
         <f t="shared" si="24"/>
         <v>1.2008480313282641</v>
       </c>
-      <c r="BB10" s="46">
+      <c r="BB10" s="44">
         <f t="shared" si="25"/>
         <v>101362.59695673757</v>
       </c>
-      <c r="BC10" s="51">
+      <c r="BC10" s="49">
         <f t="shared" si="26"/>
         <v>294.04921458433273</v>
       </c>
@@ -4291,19 +4284,19 @@
       <c r="C11" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="44">
         <f t="shared" si="47"/>
         <v>9</v>
       </c>
-      <c r="E11" s="47">
+      <c r="E11" s="45">
         <f t="shared" si="48"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="F11" s="51">
+      <c r="F11" s="49">
         <f t="shared" si="27"/>
         <v>-5.2925692224879245E-20</v>
       </c>
-      <c r="G11" s="54">
+      <c r="G11" s="52">
         <f t="shared" si="28"/>
         <v>-3.9601691076895293</v>
       </c>
@@ -4315,178 +4308,178 @@
         <f t="shared" si="1"/>
         <v>-3.9601691076895295E-3</v>
       </c>
-      <c r="J11" s="51">
+      <c r="J11" s="49">
         <f t="shared" si="29"/>
         <v>3.9601691076895293</v>
       </c>
-      <c r="K11" s="49">
+      <c r="K11" s="47">
         <f t="shared" si="2"/>
         <v>6378133.0398308923</v>
       </c>
-      <c r="L11" s="50">
+      <c r="L11" s="48">
         <f t="shared" si="3"/>
         <v>3.9601691076895293</v>
       </c>
-      <c r="M11" s="51">
+      <c r="M11" s="49">
         <f t="shared" si="30"/>
         <v>-2.4647948781951042E-19</v>
       </c>
-      <c r="N11" s="51">
+      <c r="N11" s="49">
         <f t="shared" si="31"/>
         <v>-8.7982737107928273</v>
       </c>
-      <c r="O11" s="51">
+      <c r="O11" s="49">
         <f t="shared" si="32"/>
         <v>8.7982737107928273</v>
       </c>
-      <c r="P11" s="51">
+      <c r="P11" s="49">
         <f t="shared" si="4"/>
         <v>-9.7839468142257834E-19</v>
       </c>
-      <c r="Q11" s="51">
+      <c r="Q11" s="49">
         <f t="shared" si="5"/>
         <v>-9.7643673646418012</v>
       </c>
-      <c r="R11" s="51">
+      <c r="R11" s="49">
         <f t="shared" si="33"/>
         <v>9.7643673646418012</v>
       </c>
-      <c r="S11" s="51">
+      <c r="S11" s="49">
         <f t="shared" si="34"/>
         <v>-1.5707963267948966</v>
       </c>
-      <c r="T11" s="51">
+      <c r="T11" s="49">
         <f t="shared" si="35"/>
         <v>-90</v>
       </c>
-      <c r="U11" s="51">
+      <c r="U11" s="49">
         <f t="shared" si="6"/>
         <v>-8.2979912608223828E-27</v>
       </c>
-      <c r="V11" s="51">
+      <c r="V11" s="49">
         <f t="shared" si="7"/>
         <v>-1.4482726880306613E-28</v>
       </c>
-      <c r="W11" s="52"/>
-      <c r="X11" s="50">
+      <c r="W11" s="50"/>
+      <c r="X11" s="48">
         <f t="shared" si="36"/>
         <v>-8.7981900107115507</v>
       </c>
-      <c r="Y11" s="49">
+      <c r="Y11" s="47">
         <f t="shared" si="37"/>
         <v>-159453286.88863075</v>
       </c>
-      <c r="Z11" s="51">
+      <c r="Z11" s="49">
         <f t="shared" si="38"/>
         <v>-8.7981900107115507</v>
       </c>
-      <c r="AA11" s="46">
+      <c r="AA11" s="44">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AB11" s="51">
+      <c r="AB11" s="49">
         <f t="shared" si="9"/>
         <v>-159453286.88863075</v>
       </c>
-      <c r="AC11" s="51">
+      <c r="AC11" s="49">
         <f t="shared" si="10"/>
         <v>-250468698.76938829</v>
       </c>
-      <c r="AD11" s="51">
+      <c r="AD11" s="49">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AE11" s="51">
+      <c r="AE11" s="49">
         <f t="shared" si="40"/>
         <v>-39.269908169872409</v>
       </c>
-      <c r="AF11" s="51">
+      <c r="AF11" s="49">
         <f t="shared" si="41"/>
         <v>-3.9448946552012071E-26</v>
       </c>
-      <c r="AG11" s="51">
+      <c r="AG11" s="49">
         <f t="shared" si="42"/>
         <v>3.4361253001131122E-25</v>
       </c>
-      <c r="AH11" s="52"/>
-      <c r="AI11" s="51">
+      <c r="AH11" s="50"/>
+      <c r="AI11" s="49">
         <f t="shared" si="43"/>
         <v>200</v>
       </c>
-      <c r="AJ11" s="53">
+      <c r="AJ11" s="51">
         <f t="shared" si="11"/>
         <v>2.5853239627593026E-2</v>
       </c>
-      <c r="AK11" s="51">
+      <c r="AK11" s="49">
         <f t="shared" si="44"/>
         <v>0.35</v>
       </c>
-      <c r="AL11" s="51">
+      <c r="AL11" s="49">
         <f t="shared" si="12"/>
         <v>3.1943712899763588</v>
       </c>
-      <c r="AM11" s="51">
+      <c r="AM11" s="49">
         <f t="shared" si="13"/>
         <v>-1.9567895251594956E-16</v>
       </c>
-      <c r="AN11" s="51">
+      <c r="AN11" s="49">
         <f t="shared" si="14"/>
         <v>3.1943712899763588</v>
       </c>
-      <c r="AO11" s="46">
+      <c r="AO11" s="44">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="AP11" s="46">
+      <c r="AP11" s="44">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AQ11" s="46">
+      <c r="AQ11" s="44">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AR11" s="46">
+      <c r="AR11" s="44">
         <f t="shared" si="17"/>
         <v>3870.4810145014094</v>
       </c>
-      <c r="AS11" s="46">
+      <c r="AS11" s="44">
         <f t="shared" si="18"/>
         <v>3873.1797246091555</v>
       </c>
-      <c r="AT11" s="46">
+      <c r="AT11" s="44">
         <f t="shared" si="19"/>
         <v>7743.6607391105645</v>
       </c>
-      <c r="AU11" s="46">
+      <c r="AU11" s="44">
         <f t="shared" si="20"/>
         <v>879.82737107928278</v>
       </c>
-      <c r="AV11" s="52"/>
-      <c r="AW11" s="51">
+      <c r="AV11" s="50"/>
+      <c r="AW11" s="49">
         <f t="shared" si="46"/>
         <v>-9.7803392210916833</v>
       </c>
-      <c r="AX11" s="51">
+      <c r="AX11" s="49">
         <f t="shared" si="21"/>
         <v>8.1157169384497179E-26</v>
       </c>
-      <c r="AY11" s="51">
+      <c r="AY11" s="49">
         <f t="shared" si="22"/>
         <v>-9.7803392210916833</v>
       </c>
-      <c r="AZ11" s="51">
+      <c r="AZ11" s="49">
         <f t="shared" si="23"/>
         <v>340.31610109715132</v>
       </c>
-      <c r="BA11" s="53">
+      <c r="BA11" s="51">
         <f t="shared" si="24"/>
         <v>1.2009433398886522</v>
       </c>
-      <c r="BB11" s="46">
+      <c r="BB11" s="44">
         <f t="shared" si="25"/>
         <v>101372.58314666818</v>
       </c>
-      <c r="BC11" s="51">
+      <c r="BC11" s="49">
         <f t="shared" si="26"/>
         <v>294.0548456986221</v>
       </c>
@@ -4501,19 +4494,19 @@
       <c r="C12" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="44">
         <f t="shared" si="47"/>
         <v>10</v>
       </c>
-      <c r="E12" s="47">
+      <c r="E12" s="45">
         <f t="shared" si="48"/>
         <v>0.99999999999999989</v>
       </c>
-      <c r="F12" s="51">
+      <c r="F12" s="49">
         <f t="shared" si="27"/>
         <v>-8.2465614413943178E-20</v>
       </c>
-      <c r="G12" s="54">
+      <c r="G12" s="52">
         <f t="shared" si="28"/>
         <v>-4.8888183155920215</v>
       </c>
@@ -4525,178 +4518,178 @@
         <f t="shared" si="1"/>
         <v>-4.8888183155920218E-3</v>
       </c>
-      <c r="J12" s="51">
+      <c r="J12" s="49">
         <f t="shared" si="29"/>
         <v>4.8888183155920215</v>
       </c>
-      <c r="K12" s="49">
+      <c r="K12" s="47">
         <f t="shared" si="2"/>
         <v>6378132.1111816848</v>
       </c>
-      <c r="L12" s="50">
+      <c r="L12" s="48">
         <f t="shared" si="3"/>
         <v>4.8888183155920215</v>
       </c>
-      <c r="M12" s="51">
+      <c r="M12" s="49">
         <f t="shared" si="30"/>
         <v>-3.4431895596176826E-19</v>
       </c>
-      <c r="N12" s="51">
+      <c r="N12" s="49">
         <f t="shared" si="31"/>
         <v>-9.7747104472570072</v>
       </c>
-      <c r="O12" s="51">
+      <c r="O12" s="49">
         <f t="shared" si="32"/>
         <v>9.7747104472570072</v>
       </c>
-      <c r="P12" s="51">
+      <c r="P12" s="49">
         <f t="shared" si="4"/>
         <v>-1.2077177709807872E-18</v>
       </c>
-      <c r="Q12" s="51">
+      <c r="Q12" s="49">
         <f t="shared" si="5"/>
         <v>-9.76062663295499</v>
       </c>
-      <c r="R12" s="51">
+      <c r="R12" s="49">
         <f t="shared" si="33"/>
         <v>9.76062663295499</v>
       </c>
-      <c r="S12" s="51">
+      <c r="S12" s="49">
         <f t="shared" si="34"/>
         <v>-1.5707963267948966</v>
       </c>
-      <c r="T12" s="51">
+      <c r="T12" s="49">
         <f t="shared" si="35"/>
         <v>-90</v>
       </c>
-      <c r="U12" s="51">
+      <c r="U12" s="49">
         <f t="shared" si="6"/>
         <v>-1.292943027463642E-26</v>
       </c>
-      <c r="V12" s="51">
+      <c r="V12" s="49">
         <f t="shared" si="7"/>
         <v>-2.2566112869944024E-28</v>
       </c>
-      <c r="W12" s="52"/>
-      <c r="X12" s="50">
+      <c r="W12" s="50"/>
+      <c r="X12" s="48">
         <f t="shared" si="36"/>
         <v>-31890665.199154459</v>
       </c>
-      <c r="Y12" s="49">
+      <c r="Y12" s="47">
         <f xml:space="preserve"> (W13-X11)/(2*$B$2)</f>
         <v>43.990950053557754</v>
       </c>
-      <c r="Z12" s="51">
+      <c r="Z12" s="49">
         <f t="shared" si="38"/>
         <v>-31890665.199154459</v>
       </c>
-      <c r="AA12" s="46">
+      <c r="AA12" s="44">
         <f t="shared" si="8"/>
         <v>-50093732.460283846</v>
       </c>
-      <c r="AB12" s="51">
+      <c r="AB12" s="49">
         <f t="shared" si="9"/>
         <v>-393435210.72935069</v>
       </c>
-      <c r="AC12" s="51">
+      <c r="AC12" s="49">
         <f t="shared" si="10"/>
         <v>500937397.53877664</v>
       </c>
-      <c r="AD12" s="51">
+      <c r="AD12" s="49">
         <f t="shared" si="39"/>
         <v>-7.8539816339744828</v>
       </c>
-      <c r="AE12" s="51">
+      <c r="AE12" s="49">
         <f xml:space="preserve"> (Y13-AD11)/(2*$B$2)</f>
         <v>0</v>
       </c>
-      <c r="AF12" s="51">
+      <c r="AF12" s="49">
         <f t="shared" si="41"/>
         <v>4.1489956304111912E-26</v>
       </c>
-      <c r="AG12" s="51">
+      <c r="AG12" s="49">
         <f xml:space="preserve"> (AA13-AF11)/(2*$B$2)</f>
         <v>1.9724473276006034E-25</v>
       </c>
-      <c r="AH12" s="52"/>
-      <c r="AI12" s="51">
+      <c r="AH12" s="50"/>
+      <c r="AI12" s="49">
         <f t="shared" si="43"/>
         <v>200</v>
       </c>
-      <c r="AJ12" s="53">
+      <c r="AJ12" s="51">
         <f t="shared" si="11"/>
         <v>2.8722126195685514E-2</v>
       </c>
-      <c r="AK12" s="51">
+      <c r="AK12" s="49">
         <f t="shared" si="44"/>
         <v>0.35</v>
       </c>
-      <c r="AL12" s="51">
+      <c r="AL12" s="49">
         <f t="shared" si="12"/>
         <v>3.9430907906588941</v>
       </c>
-      <c r="AM12" s="51">
+      <c r="AM12" s="49">
         <f t="shared" si="13"/>
         <v>-2.4154357948700767E-16</v>
       </c>
-      <c r="AN12" s="51">
+      <c r="AN12" s="49">
         <f t="shared" si="14"/>
         <v>3.9430907906588941</v>
       </c>
-      <c r="AO12" s="46">
+      <c r="AO12" s="44">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="AP12" s="46">
+      <c r="AP12" s="44">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AQ12" s="46">
+      <c r="AQ12" s="44">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AR12" s="46">
+      <c r="AR12" s="44">
         <f t="shared" si="17"/>
         <v>4777.248216385764</v>
       </c>
-      <c r="AS12" s="46">
+      <c r="AS12" s="44">
         <f t="shared" si="18"/>
         <v>4781.431552723272</v>
       </c>
-      <c r="AT12" s="46">
+      <c r="AT12" s="44">
         <f t="shared" si="19"/>
         <v>9558.679769109036</v>
       </c>
-      <c r="AU12" s="46">
+      <c r="AU12" s="44">
         <f t="shared" si="20"/>
         <v>977.47104472570072</v>
       </c>
-      <c r="AV12" s="52"/>
-      <c r="AW12" s="51">
+      <c r="AV12" s="50"/>
+      <c r="AW12" s="49">
         <f t="shared" si="46"/>
         <v>-9.7803420869082842</v>
       </c>
-      <c r="AX12" s="51">
+      <c r="AX12" s="49">
         <f t="shared" si="21"/>
         <v>1.2645425107477272E-25</v>
       </c>
-      <c r="AY12" s="51">
+      <c r="AY12" s="49">
         <f t="shared" si="22"/>
         <v>-9.7803420869082842</v>
       </c>
-      <c r="AZ12" s="51">
+      <c r="AZ12" s="49">
         <f t="shared" si="23"/>
         <v>340.31987676195479</v>
       </c>
-      <c r="BA12" s="53">
+      <c r="BA12" s="51">
         <f t="shared" si="24"/>
         <v>1.2010498562577365</v>
       </c>
-      <c r="BB12" s="46">
+      <c r="BB12" s="44">
         <f t="shared" si="25"/>
         <v>101383.74388757549</v>
       </c>
-      <c r="BC12" s="51">
+      <c r="BC12" s="49">
         <f t="shared" si="26"/>
         <v>294.06113859915013</v>
       </c>
@@ -4827,7 +4820,7 @@
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B18" s="17">
         <f xml:space="preserve"> B14*B24*LN((B9+B10)/B9)</f>
@@ -4873,8 +4866,9 @@
       <c r="A20" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="44" t="s">
-        <v>65</v>
+      <c r="B20" s="54">
+        <f xml:space="preserve"> 5.972*10^24</f>
+        <v>5.9720000000000003E+24</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>19</v>
@@ -4898,7 +4892,7 @@
       <c r="A21" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="54">
         <v>6378137</v>
       </c>
       <c r="C21" s="20" t="s">
@@ -4923,7 +4917,7 @@
       <c r="A22" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="54">
         <v>6356752.2999999998</v>
       </c>
       <c r="C22" s="20" t="s">
@@ -4948,7 +4942,7 @@
       <c r="A23" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="54">
         <f>SQRT((((B21^2)*COS(B6))^2+((B22^2)*SIN(B6))^2)/((B21*COS(B6))^2+(B22*SIN(B6))^2))</f>
         <v>6378137</v>
       </c>
@@ -4974,7 +4968,7 @@
       <c r="A24" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="45">
+      <c r="B24" s="54">
         <v>9.8066499999999994</v>
       </c>
       <c r="C24" s="21" t="s">
@@ -4999,11 +4993,12 @@
       <c r="A25" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="54">
+        <f xml:space="preserve"> 6.67408*10^(-11)</f>
+        <v>6.674079999999999E-11</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>63</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>64</v>
       </c>
       <c r="H25" s="10"/>
       <c r="Q25" s="5"/>
@@ -5070,7 +5065,7 @@
     </row>
     <row r="29" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A29" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H29" s="10"/>
       <c r="Q29" s="5"/>
@@ -5089,7 +5084,7 @@
     </row>
     <row r="30" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A30" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H30" s="10"/>
       <c r="Q30" s="5"/>

</xml_diff>